<commit_message>
some more fixes in prep for some test games
* reworked the custom use button code entirely. now uses entirely separate UseButton objects instead of modifying the shown one, making it more flexible and less prone to error
* when use of a panel is blocked for any reason (madmate trying to fix lights, for example), the mod now displays a "blocked" message on the use button, preventing them from interacting with it in any way. this should make things a little more obvious for players
* added graphical buttons for the GM's zoom in/out ability
* made all players' positions visible on the GM's map
* disabled shadows for the GM when they're alive
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-Madmate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A2E8B-70E7-4ECE-9C6D-8841D5DBE135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06575350-B50C-4DD6-87BB-84418EE1ACD2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="3360" windowWidth="19740" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="5160" windowWidth="18615" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="839">
   <si>
     <t>presetSelection</t>
   </si>
@@ -2463,9 +2463,6 @@
     <t>♥ {0} と恋人になりました ♥</t>
   </si>
   <si>
-    <t>残弾: {0}</t>
-  </si>
-  <si>
     <t>Shots: {0}</t>
   </si>
   <si>
@@ -2484,17 +2481,6 @@
     <t>{0} and the ship has {1}</t>
   </si>
   <si>
-    <t>{0}個　とクルー全体が　{1}個</t>
-  </si>
-  <si>
-    <t>CREWMEMBER {0} HAS
-EMERGENCY MEETINGS LEFT</t>
-  </si>
-  <si>
-    <t>船員 {0} がボタン
-残っている</t>
-  </si>
-  <si>
     <t>Disable Admin Table</t>
   </si>
   <si>
@@ -2529,6 +2515,33 @@
   </si>
   <si>
     <t>カメラ・ドアログの使用禁止</t>
+  </si>
+  <si>
+    <t>{0}回　とクルー全体が　{1}回</t>
+  </si>
+  <si>
+    <t>残り {0}発</t>
+  </si>
+  <si>
+    <t>CREWMEMBER {0} HAS\n\n\nEMERGENCY MEETINGS LEFT</t>
+  </si>
+  <si>
+    <t>船員 {0} が残り\n\n\n緊急招集できる</t>
+  </si>
+  <si>
+    <t>切断</t>
+  </si>
+  <si>
+    <t>ゲームマスターだ</t>
+  </si>
+  <si>
+    <t>buttonBlocked</t>
+  </si>
+  <si>
+    <t>BLOCKED</t>
+  </si>
+  <si>
+    <t>使用禁止</t>
   </si>
 </sst>
 </file>
@@ -2566,9 +2579,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2849,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q401"/>
+  <dimension ref="A1:Q403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="M196" sqref="M196"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="A403" sqref="A403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3927,7 +3938,7 @@
         <v>71</v>
       </c>
       <c r="B119" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="M119" t="s">
         <v>245</v>
@@ -4262,7 +4273,7 @@
         <v>93</v>
       </c>
       <c r="B155" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="M155" t="s">
         <v>269</v>
@@ -4578,46 +4589,46 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>821</v>
+      </c>
+      <c r="B191" t="s">
+        <v>818</v>
+      </c>
+      <c r="M191" t="s">
         <v>825</v>
-      </c>
-      <c r="B191" t="s">
-        <v>822</v>
-      </c>
-      <c r="M191" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B192" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="M192" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>822</v>
+      </c>
+      <c r="B193" t="s">
+        <v>819</v>
+      </c>
+      <c r="M193" t="s">
         <v>826</v>
-      </c>
-      <c r="B193" t="s">
-        <v>823</v>
-      </c>
-      <c r="M193" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="B194" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="M194" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
@@ -5999,6 +6010,9 @@
       <c r="B363" t="s">
         <v>490</v>
       </c>
+      <c r="M363" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
@@ -6007,6 +6021,9 @@
       <c r="B364" t="s">
         <v>490</v>
       </c>
+      <c r="M364" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
@@ -6199,6 +6216,9 @@
       <c r="B385" t="s">
         <v>528</v>
       </c>
+      <c r="M385" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="387" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
@@ -6293,32 +6313,53 @@
         <v>544</v>
       </c>
       <c r="B398" t="s">
+        <v>812</v>
+      </c>
+      <c r="M398" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
         <v>813</v>
       </c>
-      <c r="M398" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="400" spans="1:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
-        <v>814</v>
-      </c>
       <c r="B400" s="1" t="s">
-        <v>820</v>
-      </c>
+        <v>832</v>
+      </c>
+      <c r="C400" s="1"/>
+      <c r="D400" s="1"/>
+      <c r="E400" s="1"/>
+      <c r="F400" s="1"/>
+      <c r="G400" s="1"/>
+      <c r="H400" s="1"/>
+      <c r="I400" s="1"/>
+      <c r="J400" s="1"/>
+      <c r="K400" s="1"/>
+      <c r="L400" s="1"/>
       <c r="M400" s="1" t="s">
-        <v>821</v>
+        <v>833</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B401" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M401" t="s">
-        <v>819</v>
+        <v>830</v>
+      </c>
+    </row>
+    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>836</v>
+      </c>
+      <c r="B403" t="s">
+        <v>837</v>
+      </c>
+      <c r="M403" t="s">
+        <v>838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix: results screen doesn't display properly if the game ends during a camouflage/morph
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-Madmate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340989ED-69F9-4B03-A302-209686D1F513}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91D86A6-14AA-46C7-BE4D-A55F1AD571AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="4230" windowWidth="22230" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2056,15 +2056,6 @@
     <t>タスクがある</t>
   </si>
   <si>
-    <t>多プレイヤーにワープできる</t>
-  </si>
-  <si>
-    <t>多プレイヤーを殺害・蘇生できる</t>
-  </si>
-  <si>
-    <t>多プレイヤーに設定を隠せる</t>
-  </si>
-  <si>
     <t>ゲーム開始時に死亡する</t>
   </si>
   <si>
@@ -2887,6 +2878,15 @@
   </si>
   <si>
     <t>Kill everyone and recruit a Sidekick</t>
+  </si>
+  <si>
+    <t>他プレイヤーにワープできる</t>
+  </si>
+  <si>
+    <t>他プレイヤーを殺害・蘇生できる</t>
+  </si>
+  <si>
+    <t>他プレイヤーに設定を隠せる</t>
   </si>
 </sst>
 </file>
@@ -3209,8 +3209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="B318" sqref="B318"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,7 +3342,7 @@
         <v>518</v>
       </c>
       <c r="M8" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
         <v>519</v>
       </c>
       <c r="M9" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -3416,7 +3416,7 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="M16" t="s">
         <v>674</v>
@@ -3427,7 +3427,7 @@
         <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="M17" t="s">
         <v>675</v>
@@ -3438,10 +3438,10 @@
         <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="M18" t="s">
-        <v>676</v>
+        <v>948</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -3449,10 +3449,10 @@
         <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="M19" t="s">
-        <v>677</v>
+        <v>949</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -3460,10 +3460,10 @@
         <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="M20" t="s">
-        <v>678</v>
+        <v>950</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -3471,10 +3471,10 @@
         <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="M21" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="M28" t="s">
         <v>173</v>
@@ -3548,7 +3548,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="M32" t="s">
         <v>176</v>
@@ -3581,10 +3581,10 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="M36" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -3592,7 +3592,7 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="M37" t="s">
         <v>179</v>
@@ -3603,7 +3603,7 @@
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="M38" t="s">
         <v>180</v>
@@ -3625,7 +3625,7 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="M41" t="s">
         <v>182</v>
@@ -3636,7 +3636,7 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="M42" t="s">
         <v>183</v>
@@ -3658,7 +3658,7 @@
         <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="M45" t="s">
         <v>185</v>
@@ -3669,7 +3669,7 @@
         <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="M46" t="s">
         <v>186</v>
@@ -3680,7 +3680,7 @@
         <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="M47" t="s">
         <v>187</v>
@@ -3702,7 +3702,7 @@
         <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="M50" t="s">
         <v>171</v>
@@ -3724,7 +3724,7 @@
         <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="M53" t="s">
         <v>190</v>
@@ -3735,7 +3735,7 @@
         <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="M54" t="s">
         <v>191</v>
@@ -3845,10 +3845,10 @@
         <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="M68" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,7 @@
         <v>544</v>
       </c>
       <c r="M69" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3867,10 +3867,10 @@
         <v>27</v>
       </c>
       <c r="B70" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="M70" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3878,10 +3878,10 @@
         <v>28</v>
       </c>
       <c r="B71" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="M71" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3889,10 +3889,10 @@
         <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="M72" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3911,10 +3911,10 @@
         <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="M75" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3922,7 +3922,7 @@
         <v>32</v>
       </c>
       <c r="B76" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="M76" t="s">
         <v>202</v>
@@ -3944,10 +3944,10 @@
         <v>34</v>
       </c>
       <c r="B79" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="M79" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -3955,10 +3955,10 @@
         <v>35</v>
       </c>
       <c r="B80" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="M80" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>37</v>
       </c>
       <c r="B83" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="M83" t="s">
         <v>205</v>
@@ -3988,7 +3988,7 @@
         <v>38</v>
       </c>
       <c r="B84" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="M84" t="s">
         <v>206</v>
@@ -4010,10 +4010,10 @@
         <v>40</v>
       </c>
       <c r="B87" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="M87" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -4021,10 +4021,10 @@
         <v>41</v>
       </c>
       <c r="B88" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="M88" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -4032,10 +4032,10 @@
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="M89" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -4043,10 +4043,10 @@
         <v>43</v>
       </c>
       <c r="B90" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="M90" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -4057,7 +4057,7 @@
         <v>549</v>
       </c>
       <c r="M91" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -4098,10 +4098,10 @@
         <v>48</v>
       </c>
       <c r="B95" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="M95" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -4109,10 +4109,10 @@
         <v>49</v>
       </c>
       <c r="B96" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="M96" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>57</v>
       </c>
       <c r="B99" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="M99" t="s">
         <v>212</v>
@@ -4175,10 +4175,10 @@
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="M106" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -4186,7 +4186,7 @@
         <v>62</v>
       </c>
       <c r="B107" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="M107" t="s">
         <v>202</v>
@@ -4197,10 +4197,10 @@
         <v>63</v>
       </c>
       <c r="B108" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="M108" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -4219,7 +4219,7 @@
         <v>65</v>
       </c>
       <c r="B112" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="M112" t="s">
         <v>217</v>
@@ -4230,7 +4230,7 @@
         <v>66</v>
       </c>
       <c r="B113" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="M113" t="s">
         <v>218</v>
@@ -4241,7 +4241,7 @@
         <v>67</v>
       </c>
       <c r="B114" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="M114" t="s">
         <v>219</v>
@@ -4252,7 +4252,7 @@
         <v>68</v>
       </c>
       <c r="B115" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="M115" t="s">
         <v>220</v>
@@ -4285,7 +4285,7 @@
         <v>71</v>
       </c>
       <c r="B119" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="M119" t="s">
         <v>223</v>
@@ -4310,7 +4310,7 @@
         <v>561</v>
       </c>
       <c r="M121" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -4321,7 +4321,7 @@
         <v>562</v>
       </c>
       <c r="M122" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -4340,7 +4340,7 @@
         <v>76</v>
       </c>
       <c r="B125" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="M125" t="s">
         <v>226</v>
@@ -4362,7 +4362,7 @@
         <v>78</v>
       </c>
       <c r="B127" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="M127" t="s">
         <v>228</v>
@@ -4381,18 +4381,18 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="B130" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="M130" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B131" t="s">
         <v>565</v>
@@ -4403,24 +4403,24 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B132" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="M132" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B133" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="M133" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>567</v>
       </c>
       <c r="M135" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -4461,10 +4461,10 @@
         <v>83</v>
       </c>
       <c r="B138" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="M138" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -4472,7 +4472,7 @@
         <v>84</v>
       </c>
       <c r="B139" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="M139" t="s">
         <v>233</v>
@@ -4491,18 +4491,18 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B142" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="M142" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="B143" t="s">
         <v>570</v>
@@ -4513,24 +4513,24 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>683</v>
+      </c>
+      <c r="B144" t="s">
+        <v>687</v>
+      </c>
+      <c r="M144" t="s">
         <v>686</v>
-      </c>
-      <c r="B144" t="s">
-        <v>690</v>
-      </c>
-      <c r="M144" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="B145" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="M145" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -4538,7 +4538,7 @@
         <v>87</v>
       </c>
       <c r="B146" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="M146" t="s">
         <v>236</v>
@@ -4549,7 +4549,7 @@
         <v>86</v>
       </c>
       <c r="B147" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="M147" t="s">
         <v>237</v>
@@ -4576,7 +4576,7 @@
         <v>89</v>
       </c>
       <c r="B150" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="M150" t="s">
         <v>239</v>
@@ -4587,7 +4587,7 @@
         <v>90</v>
       </c>
       <c r="B151" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="M151" t="s">
         <v>240</v>
@@ -4598,10 +4598,10 @@
         <v>91</v>
       </c>
       <c r="B152" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="M152" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -4620,7 +4620,7 @@
         <v>93</v>
       </c>
       <c r="B155" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="M155" t="s">
         <v>242</v>
@@ -4631,7 +4631,7 @@
         <v>94</v>
       </c>
       <c r="B156" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="M156" t="s">
         <v>243</v>
@@ -4697,7 +4697,7 @@
         <v>100</v>
       </c>
       <c r="B164" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="M164" t="s">
         <v>249</v>
@@ -4719,10 +4719,10 @@
         <v>102</v>
       </c>
       <c r="B166" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="M166" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -4730,10 +4730,10 @@
         <v>103</v>
       </c>
       <c r="B167" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="M167" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -4752,7 +4752,7 @@
         <v>114</v>
       </c>
       <c r="B170" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="M170" t="s">
         <v>252</v>
@@ -4763,7 +4763,7 @@
         <v>115</v>
       </c>
       <c r="B171" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="M171" t="s">
         <v>253</v>
@@ -4774,10 +4774,10 @@
         <v>116</v>
       </c>
       <c r="B172" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="M172" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -4785,10 +4785,10 @@
         <v>117</v>
       </c>
       <c r="B173" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="M173" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -4840,7 +4840,7 @@
         <v>122</v>
       </c>
       <c r="B180" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="M180" t="s">
         <v>258</v>
@@ -4851,10 +4851,10 @@
         <v>123</v>
       </c>
       <c r="B181" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="M181" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -4862,10 +4862,10 @@
         <v>124</v>
       </c>
       <c r="B182" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="M182" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -4873,10 +4873,10 @@
         <v>125</v>
       </c>
       <c r="B183" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="M183" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -4884,21 +4884,21 @@
         <v>126</v>
       </c>
       <c r="B184" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="M184" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B186" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="M186" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -4906,10 +4906,10 @@
         <v>134</v>
       </c>
       <c r="B188" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="M188" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -4920,7 +4920,7 @@
         <v>585</v>
       </c>
       <c r="M189" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -4947,46 +4947,46 @@
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="B193" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="M193" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B194" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="M194" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B195" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="M195" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>711</v>
+      </c>
+      <c r="B196" t="s">
+        <v>707</v>
+      </c>
+      <c r="M196" t="s">
         <v>714</v>
-      </c>
-      <c r="B196" t="s">
-        <v>710</v>
-      </c>
-      <c r="M196" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
@@ -5019,7 +5019,7 @@
         <v>590</v>
       </c>
       <c r="M201" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.25">
@@ -5052,7 +5052,7 @@
         <v>271</v>
       </c>
       <c r="M205" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
@@ -5107,7 +5107,7 @@
         <v>594</v>
       </c>
       <c r="M212" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -5118,7 +5118,7 @@
         <v>594</v>
       </c>
       <c r="M213" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -5984,7 +5984,7 @@
         <v>454</v>
       </c>
       <c r="B318" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="M318" t="s">
         <v>455</v>
@@ -6295,7 +6295,7 @@
         <v>639</v>
       </c>
       <c r="M356" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.25">
@@ -6372,7 +6372,7 @@
         <v>452</v>
       </c>
       <c r="M365" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.25">
@@ -6383,7 +6383,7 @@
         <v>452</v>
       </c>
       <c r="M366" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.25">
@@ -6410,35 +6410,35 @@
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="B371" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="M371" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="B372" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="M372" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="B373" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="M373" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.25">
@@ -6506,24 +6506,24 @@
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B382" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="M382" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="B383" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="M383" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="384" spans="1:13" x14ac:dyDescent="0.25">
@@ -6583,101 +6583,101 @@
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="B389" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="M389" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="B390" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="M390" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="B391" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="M391" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="B392" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="M392" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="B393" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="M393" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="B394" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="M394" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="B395" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="M395" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B396" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="M396" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="B397" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="M397" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="398" spans="1:13" x14ac:dyDescent="0.25">
@@ -6688,7 +6688,7 @@
         <v>511</v>
       </c>
       <c r="M398" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="399" spans="1:13" x14ac:dyDescent="0.25">
@@ -6718,10 +6718,10 @@
         <v>485</v>
       </c>
       <c r="B401" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="M401" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
     </row>
     <row r="403" spans="1:13" x14ac:dyDescent="0.25">
@@ -6773,10 +6773,10 @@
         <v>496</v>
       </c>
       <c r="B408" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="M408" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="410" spans="1:13" x14ac:dyDescent="0.25">
@@ -6817,18 +6817,18 @@
         <v>503</v>
       </c>
       <c r="B414" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="M414" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="416" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C416" s="1"/>
       <c r="D416" s="1"/>
@@ -6841,147 +6841,147 @@
       <c r="K416" s="1"/>
       <c r="L416" s="1"/>
       <c r="M416" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="B417" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="M417" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="419" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="B419" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="M419" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="421" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="B421" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="M421" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="422" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="B422" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="M422" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="423" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="B423" t="s">
+        <v>734</v>
+      </c>
+      <c r="M423" t="s">
         <v>737</v>
-      </c>
-      <c r="M423" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="424" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="B424" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="M424" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="B425" t="s">
         <v>288</v>
       </c>
       <c r="M425" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="426" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="B426" t="s">
+        <v>736</v>
+      </c>
+      <c r="M426" t="s">
         <v>739</v>
-      </c>
-      <c r="M426" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
+        <v>836</v>
+      </c>
+      <c r="B428" t="s">
+        <v>837</v>
+      </c>
+      <c r="M428" t="s">
         <v>839</v>
-      </c>
-      <c r="B428" t="s">
-        <v>840</v>
-      </c>
-      <c r="M428" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B429" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="M429" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B430" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="M430" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B431" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="M431" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="C433" s="3"/>
       <c r="D433" s="3"/>
@@ -6994,15 +6994,15 @@
       <c r="K433" s="3"/>
       <c r="L433" s="3"/>
       <c r="M433" s="2" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="434" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C434" s="3"/>
       <c r="D434" s="3"/>
@@ -7015,18 +7015,18 @@
       <c r="K434" s="3"/>
       <c r="L434" s="3"/>
       <c r="M434" s="2" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="B435" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="M435" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -7038,7 +7038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F94718-1E67-46BF-B76C-539A7DE72FFF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7099,218 +7099,218 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="B2" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="B3" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="B4" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="B5" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="B6" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="B7" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="B8" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="B9" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="B10" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B11" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="B12" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="B13" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="B14" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="B15" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="B16" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="B17" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B18" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="B19" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="B20" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="B21" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="B22" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="B23" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="B24" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="B25" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B26" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="B27" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="B28" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjustments to the new upstream 2.9.x code that make it compatible with GM edition (mostly translation related)
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2134643F-2051-47BC-8C11-0C6295247EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4585FC9-E822-4C39-8509-871AB77658D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2400" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="2085" windowWidth="28800" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="1179">
   <si>
     <t>presetSelection</t>
   </si>
@@ -3618,6 +3618,209 @@
   </si>
   <si>
     <t>Block Skipping in Meetings</t>
+  </si>
+  <si>
+    <t>vulture</t>
+  </si>
+  <si>
+    <t>vultureIntroDesc</t>
+  </si>
+  <si>
+    <t>vultureShortDesc</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>mediumIntroDesc</t>
+  </si>
+  <si>
+    <t>mediumShortDesc</t>
+  </si>
+  <si>
+    <t>Vulture</t>
+  </si>
+  <si>
+    <t>Eat corpses to win</t>
+  </si>
+  <si>
+    <t>Eat dead bodies</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Question the souls</t>
+  </si>
+  <si>
+    <t>vultureCooldown</t>
+  </si>
+  <si>
+    <t>vultureNumberToWin</t>
+  </si>
+  <si>
+    <t>vultureCanUseVents</t>
+  </si>
+  <si>
+    <t>vultureShowArrows</t>
+  </si>
+  <si>
+    <t>mediumCooldown</t>
+  </si>
+  <si>
+    <t>mediumDuration</t>
+  </si>
+  <si>
+    <t>mediumOneTimeUse</t>
+  </si>
+  <si>
+    <t>Questioning Cooldown</t>
+  </si>
+  <si>
+    <t>Questioning Duration</t>
+  </si>
+  <si>
+    <t>Each Soul Can Only Be Questioned Once</t>
+  </si>
+  <si>
+    <t>Eat Cooldown</t>
+  </si>
+  <si>
+    <t>Number Of Corpses Required</t>
+  </si>
+  <si>
+    <t>喰らうクールダウン</t>
+  </si>
+  <si>
+    <t>死体を指す矢印を表示</t>
+  </si>
+  <si>
+    <t>ヴァルチャー</t>
+  </si>
+  <si>
+    <t>死体を喰らおう</t>
+  </si>
+  <si>
+    <t>ミーディアム</t>
+  </si>
+  <si>
+    <t>Question the souls of the dead to gain information</t>
+  </si>
+  <si>
+    <t>霊能力クールダウン</t>
+  </si>
+  <si>
+    <t>霊能力時間</t>
+  </si>
+  <si>
+    <t>1人ずつ1回のみ霊能力を使える</t>
+  </si>
+  <si>
+    <t>会議中、複数回撃てる</t>
+  </si>
+  <si>
+    <t>guesserHasMultipleShotsPerMeeting</t>
+  </si>
+  <si>
+    <t>jackalCanSeeEngineerVent</t>
+  </si>
+  <si>
+    <t>Can See If Engineer Is In A Vent</t>
+  </si>
+  <si>
+    <t>Can Shoot Multiple Times Per Meeting</t>
+  </si>
+  <si>
+    <t>ベント内のエンジニアが見える</t>
+  </si>
+  <si>
+    <t>mediumQuestion1</t>
+  </si>
+  <si>
+    <t>mediumQuestion2</t>
+  </si>
+  <si>
+    <t>mediumQuestion3</t>
+  </si>
+  <si>
+    <t>What is your role? My role is {0}.</t>
+  </si>
+  <si>
+    <t>What is your killer's color type? My killer is a {0} color.</t>
+  </si>
+  <si>
+    <t>mediumQuestion4</t>
+  </si>
+  <si>
+    <t>When did you die? I died {0}s before the meeting started.</t>
+  </si>
+  <si>
+    <t>What is your killer's role? My killer is {0}.</t>
+  </si>
+  <si>
+    <t>「君の役職は何でしょう」『私は{0}です』</t>
+  </si>
+  <si>
+    <t>「君を殺した人の役職は何でしょう」『私を殺した人は{0}です』</t>
+  </si>
+  <si>
+    <t>「君を殺した人はどんな色でしょう」『私を殺した人は{0}色をしていました』</t>
+  </si>
+  <si>
+    <t>必要な死体の数</t>
+  </si>
+  <si>
+    <t>Show Arrows Pointing Towards Corpses</t>
+  </si>
+  <si>
+    <t>幽霊から情報を聞き出そう</t>
+  </si>
+  <si>
+    <t>残り {0}体</t>
+  </si>
+  <si>
+    <t>vultureCorpses</t>
+  </si>
+  <si>
+    <t>vultureWin</t>
+  </si>
+  <si>
+    <t>Vulture Wins</t>
+  </si>
+  <si>
+    <t>Vulture {0} Win</t>
+  </si>
+  <si>
+    <t>ヴァルチャー勝利</t>
+  </si>
+  <si>
+    <t>ヴァルチャー{0}勝利</t>
+  </si>
+  <si>
+    <t>vultureWinExtra</t>
+  </si>
+  <si>
+    <t>「君はいつ死んだんでしょう」『私は会議の{0}秒前に死にました』</t>
+  </si>
+  <si>
+    <t>vultureFullDesc</t>
+  </si>
+  <si>
+    <t>mediumFullDesc</t>
+  </si>
+  <si>
+    <t>The Vulture does not have any tasks, he has to win the game as a solo.
+The Vulture is a neutral role that must eat a specified number of corpses
+(depending on the options) in order to win.
+Depending on the options, when a player dies, the Vulture gets an arrow pointing
+to the corpse.</t>
+  </si>
+  <si>
+    <t>The medium is a crewmate who can ask the souls of dead players for information.
+Like the Seer, it sees the places where the players have died (after the next meeting)
+and can question them. It then gets random information about the soul or the killer
+in the chat. The souls only stay for one round, i.e. until the next meeting.
+Depending on the options, the souls can only be questioned once and then disappear.</t>
   </si>
 </sst>
 </file>
@@ -3941,10 +4144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q450"/>
+  <dimension ref="A1:Q477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView topLeftCell="A446" workbookViewId="0">
+      <selection activeCell="M467" sqref="M467"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4684,3236 +4887,3478 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>33</v>
-      </c>
-      <c r="B81" t="s">
-        <v>543</v>
-      </c>
-      <c r="M81" t="s">
-        <v>202</v>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1150</v>
+      </c>
+      <c r="M80" t="s">
+        <v>1146</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>773</v>
+        <v>543</v>
       </c>
       <c r="M82" t="s">
-        <v>737</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" t="s">
+        <v>773</v>
+      </c>
+      <c r="M83" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>35</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>774</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M84" t="s">
         <v>736</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>36</v>
-      </c>
-      <c r="B85" t="s">
-        <v>544</v>
-      </c>
-      <c r="M85" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B86" t="s">
-        <v>775</v>
+        <v>544</v>
       </c>
       <c r="M86" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" t="s">
+        <v>775</v>
+      </c>
+      <c r="M87" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>38</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>776</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M88" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>39</v>
-      </c>
-      <c r="B89" t="s">
-        <v>545</v>
-      </c>
-      <c r="M89" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B90" t="s">
-        <v>777</v>
+        <v>545</v>
       </c>
       <c r="M90" t="s">
-        <v>743</v>
+        <v>206</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B91" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="M91" t="s">
-        <v>754</v>
+        <v>743</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="M92" t="s">
-        <v>738</v>
+        <v>754</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="M93" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94" t="s">
-        <v>546</v>
+        <v>780</v>
       </c>
       <c r="M94" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="M95" t="s">
-        <v>207</v>
+        <v>740</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="M96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B97" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="M97" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B98" t="s">
-        <v>781</v>
+        <v>549</v>
       </c>
       <c r="M98" t="s">
-        <v>741</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>48</v>
+      </c>
+      <c r="B99" t="s">
+        <v>781</v>
+      </c>
+      <c r="M99" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>49</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>794</v>
       </c>
-      <c r="M99" t="s">
+      <c r="M100" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1149</v>
+      </c>
+      <c r="M101" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>56</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>550</v>
       </c>
-      <c r="M101" t="s">
+      <c r="M103" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>57</v>
-      </c>
-      <c r="B102" t="s">
-        <v>782</v>
-      </c>
-      <c r="M102" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>551</v>
+        <v>782</v>
       </c>
       <c r="M104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B106" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="M106" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B108" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="M108" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>61</v>
-      </c>
-      <c r="B109" t="s">
-        <v>777</v>
-      </c>
-      <c r="M109" t="s">
-        <v>743</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B110" t="s">
-        <v>772</v>
+        <v>553</v>
       </c>
       <c r="M110" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B111" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="M111" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>949</v>
+        <v>62</v>
       </c>
       <c r="B112" t="s">
-        <v>950</v>
+        <v>772</v>
       </c>
       <c r="M112" t="s">
-        <v>951</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113" t="s">
+        <v>783</v>
+      </c>
+      <c r="M113" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>64</v>
+        <v>949</v>
       </c>
       <c r="B114" t="s">
-        <v>554</v>
+        <v>950</v>
       </c>
       <c r="M114" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>65</v>
-      </c>
-      <c r="B115" t="s">
-        <v>784</v>
-      </c>
-      <c r="M115" t="s">
-        <v>216</v>
+        <v>951</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B116" t="s">
-        <v>785</v>
+        <v>554</v>
       </c>
       <c r="M116" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B117" t="s">
-        <v>801</v>
+        <v>784</v>
       </c>
       <c r="M117" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
       <c r="M118" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>67</v>
+      </c>
+      <c r="B119" t="s">
+        <v>801</v>
+      </c>
+      <c r="M119" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B120" t="s">
-        <v>555</v>
+        <v>802</v>
       </c>
       <c r="M120" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>70</v>
-      </c>
-      <c r="B121" t="s">
-        <v>556</v>
-      </c>
-      <c r="M121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B122" t="s">
-        <v>699</v>
+        <v>555</v>
       </c>
       <c r="M122" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B123" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M123" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B124" t="s">
-        <v>558</v>
+        <v>699</v>
       </c>
       <c r="M124" t="s">
-        <v>745</v>
+        <v>222</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B125" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M125" t="s">
-        <v>746</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>73</v>
+      </c>
+      <c r="B126" t="s">
+        <v>558</v>
+      </c>
+      <c r="M126" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B127" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="M127" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>76</v>
-      </c>
-      <c r="B128" t="s">
-        <v>803</v>
-      </c>
-      <c r="M128" t="s">
-        <v>225</v>
+        <v>746</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B129" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M129" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B130" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="M130" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>77</v>
+      </c>
+      <c r="B131" t="s">
+        <v>561</v>
+      </c>
+      <c r="M131" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B132" t="s">
-        <v>562</v>
+        <v>804</v>
       </c>
       <c r="M132" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>687</v>
-      </c>
-      <c r="B133" t="s">
-        <v>811</v>
-      </c>
-      <c r="M133" t="s">
-        <v>689</v>
+        <v>227</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>673</v>
+        <v>79</v>
       </c>
       <c r="B134" t="s">
         <v>562</v>
       </c>
       <c r="M134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>676</v>
+        <v>687</v>
       </c>
       <c r="B135" t="s">
-        <v>686</v>
+        <v>811</v>
       </c>
       <c r="M135" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B136" t="s">
-        <v>685</v>
+        <v>562</v>
       </c>
       <c r="M136" t="s">
-        <v>675</v>
+        <v>229</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>80</v>
+        <v>676</v>
       </c>
       <c r="B137" t="s">
-        <v>563</v>
+        <v>686</v>
       </c>
       <c r="M137" t="s">
-        <v>230</v>
+        <v>674</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>81</v>
+        <v>677</v>
       </c>
       <c r="B138" t="s">
-        <v>564</v>
+        <v>685</v>
       </c>
       <c r="M138" t="s">
-        <v>833</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>80</v>
+      </c>
+      <c r="B139" t="s">
+        <v>563</v>
+      </c>
+      <c r="M139" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B140" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M140" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>83</v>
-      </c>
-      <c r="B141" t="s">
-        <v>773</v>
-      </c>
-      <c r="M141" t="s">
-        <v>737</v>
+        <v>833</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B142" t="s">
-        <v>786</v>
+        <v>565</v>
       </c>
       <c r="M142" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>83</v>
+      </c>
+      <c r="B143" t="s">
+        <v>773</v>
+      </c>
+      <c r="M143" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B144" t="s">
-        <v>566</v>
+        <v>786</v>
       </c>
       <c r="M144" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>688</v>
-      </c>
-      <c r="B145" t="s">
-        <v>756</v>
-      </c>
-      <c r="M145" t="s">
-        <v>747</v>
+        <v>232</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>678</v>
+        <v>85</v>
       </c>
       <c r="B146" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M146" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="B147" t="s">
-        <v>683</v>
+        <v>756</v>
       </c>
       <c r="M147" t="s">
-        <v>682</v>
+        <v>747</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B148" t="s">
-        <v>684</v>
+        <v>567</v>
       </c>
       <c r="M148" t="s">
-        <v>681</v>
+        <v>234</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>87</v>
+        <v>679</v>
       </c>
       <c r="B149" t="s">
-        <v>787</v>
+        <v>683</v>
       </c>
       <c r="M149" t="s">
-        <v>235</v>
+        <v>682</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>86</v>
+        <v>680</v>
       </c>
       <c r="B150" t="s">
-        <v>788</v>
+        <v>684</v>
       </c>
       <c r="M150" t="s">
-        <v>236</v>
+        <v>681</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>87</v>
+      </c>
       <c r="B151" t="s">
-        <v>568</v>
+        <v>787</v>
+      </c>
+      <c r="M151" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B152" t="s">
-        <v>569</v>
+        <v>788</v>
       </c>
       <c r="M152" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>89</v>
-      </c>
       <c r="B153" t="s">
-        <v>805</v>
-      </c>
-      <c r="M153" t="s">
-        <v>238</v>
+        <v>568</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B154" t="s">
-        <v>806</v>
+        <v>569</v>
       </c>
       <c r="M154" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B155" t="s">
-        <v>789</v>
+        <v>805</v>
       </c>
       <c r="M155" t="s">
-        <v>1034</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>90</v>
+      </c>
+      <c r="B156" t="s">
+        <v>806</v>
+      </c>
+      <c r="M156" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B157" t="s">
-        <v>570</v>
+        <v>789</v>
       </c>
       <c r="M157" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>93</v>
-      </c>
-      <c r="B158" t="s">
-        <v>790</v>
-      </c>
-      <c r="M158" t="s">
-        <v>241</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B159" t="s">
-        <v>791</v>
+        <v>570</v>
       </c>
       <c r="M159" t="s">
-        <v>242</v>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>93</v>
+      </c>
+      <c r="B160" t="s">
+        <v>790</v>
+      </c>
+      <c r="M160" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B161" t="s">
-        <v>571</v>
+        <v>791</v>
       </c>
       <c r="M161" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>96</v>
-      </c>
-      <c r="B162" t="s">
-        <v>572</v>
-      </c>
-      <c r="M162" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B163" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="M163" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B164" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="M164" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>97</v>
+      </c>
+      <c r="B165" t="s">
+        <v>573</v>
+      </c>
+      <c r="M165" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B166" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="M166" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>100</v>
-      </c>
-      <c r="B167" t="s">
-        <v>792</v>
-      </c>
-      <c r="M167" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B168" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="M168" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B169" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="M169" t="s">
-        <v>738</v>
+        <v>248</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B170" t="s">
-        <v>794</v>
+        <v>576</v>
       </c>
       <c r="M170" t="s">
-        <v>742</v>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>102</v>
+      </c>
+      <c r="B171" t="s">
+        <v>793</v>
+      </c>
+      <c r="M171" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B172" t="s">
-        <v>577</v>
+        <v>794</v>
       </c>
       <c r="M172" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>114</v>
-      </c>
-      <c r="B173" t="s">
-        <v>755</v>
-      </c>
-      <c r="M173" t="s">
-        <v>251</v>
+        <v>742</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B174" t="s">
-        <v>807</v>
+        <v>577</v>
       </c>
       <c r="M174" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B175" t="s">
-        <v>808</v>
+        <v>755</v>
       </c>
       <c r="M175" t="s">
-        <v>831</v>
+        <v>251</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B176" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="M176" t="s">
-        <v>832</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>116</v>
+      </c>
+      <c r="B177" t="s">
+        <v>808</v>
+      </c>
+      <c r="M177" t="s">
+        <v>831</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B178" t="s">
-        <v>578</v>
+        <v>809</v>
       </c>
       <c r="M178" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>119</v>
-      </c>
-      <c r="B179" t="s">
-        <v>579</v>
-      </c>
-      <c r="M179" t="s">
-        <v>254</v>
+        <v>832</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B180" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="M180" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>119</v>
+      </c>
+      <c r="B181" t="s">
+        <v>579</v>
+      </c>
+      <c r="M181" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B182" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M182" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>122</v>
-      </c>
-      <c r="B183" t="s">
-        <v>792</v>
-      </c>
-      <c r="M183" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B184" t="s">
-        <v>793</v>
+        <v>581</v>
       </c>
       <c r="M184" t="s">
-        <v>738</v>
+        <v>256</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B185" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="M185" t="s">
-        <v>742</v>
+        <v>257</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B186" t="s">
-        <v>774</v>
+        <v>793</v>
       </c>
       <c r="M186" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B187" t="s">
-        <v>810</v>
+        <v>794</v>
       </c>
       <c r="M187" t="s">
-        <v>748</v>
+        <v>742</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>125</v>
+      </c>
+      <c r="B188" t="s">
+        <v>774</v>
+      </c>
+      <c r="M188" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>902</v>
+        <v>126</v>
       </c>
       <c r="B189" t="s">
-        <v>900</v>
+        <v>810</v>
       </c>
       <c r="M189" t="s">
-        <v>899</v>
+        <v>748</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>133</v>
+        <v>902</v>
       </c>
       <c r="B191" t="s">
-        <v>1112</v>
+        <v>900</v>
       </c>
       <c r="M191" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>134</v>
-      </c>
-      <c r="B192" t="s">
-        <v>1113</v>
-      </c>
-      <c r="M192" t="s">
-        <v>752</v>
+        <v>899</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>135</v>
+        <v>1125</v>
       </c>
       <c r="B193" t="s">
-        <v>582</v>
+        <v>1135</v>
       </c>
       <c r="M193" t="s">
-        <v>258</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>136</v>
+        <v>1126</v>
       </c>
       <c r="B194" t="s">
-        <v>583</v>
+        <v>1136</v>
       </c>
       <c r="M194" t="s">
-        <v>259</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>1069</v>
+        <v>1127</v>
       </c>
       <c r="B195" t="s">
-        <v>1071</v>
+        <v>779</v>
       </c>
       <c r="M195" t="s">
-        <v>1070</v>
+        <v>738</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M196" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>955</v>
+        <v>1167</v>
       </c>
       <c r="B197" t="s">
-        <v>958</v>
+        <v>972</v>
       </c>
       <c r="M197" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>956</v>
-      </c>
-      <c r="B198" t="s">
-        <v>959</v>
-      </c>
-      <c r="M198" t="s">
-        <v>974</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>957</v>
+        <v>1129</v>
       </c>
       <c r="B199" t="s">
-        <v>960</v>
+        <v>1132</v>
       </c>
       <c r="M199" t="s">
-        <v>975</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>702</v>
+        <v>1130</v>
       </c>
       <c r="B200" t="s">
-        <v>962</v>
+        <v>1133</v>
       </c>
       <c r="M200" t="s">
-        <v>965</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>704</v>
+        <v>1131</v>
       </c>
       <c r="B201" t="s">
-        <v>963</v>
+        <v>1134</v>
       </c>
       <c r="M201" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>703</v>
-      </c>
-      <c r="B202" t="s">
-        <v>964</v>
-      </c>
-      <c r="M202" t="s">
-        <v>967</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>705</v>
+        <v>133</v>
       </c>
       <c r="B203" t="s">
-        <v>701</v>
+        <v>1112</v>
       </c>
       <c r="M203" t="s">
-        <v>706</v>
+        <v>751</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>968</v>
+        <v>134</v>
       </c>
       <c r="B204" t="s">
-        <v>969</v>
+        <v>1113</v>
       </c>
       <c r="M204" t="s">
-        <v>970</v>
+        <v>752</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>971</v>
+        <v>135</v>
       </c>
       <c r="B205" t="s">
-        <v>972</v>
+        <v>582</v>
       </c>
       <c r="M205" t="s">
-        <v>973</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>136</v>
+      </c>
+      <c r="B206" t="s">
+        <v>583</v>
+      </c>
+      <c r="M206" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>1069</v>
       </c>
       <c r="B207" t="s">
-        <v>584</v>
+        <v>1071</v>
       </c>
       <c r="M207" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>261</v>
-      </c>
-      <c r="B208" t="s">
-        <v>585</v>
-      </c>
-      <c r="M208" t="s">
-        <v>263</v>
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>955</v>
+      </c>
+      <c r="B209" t="s">
+        <v>958</v>
+      </c>
+      <c r="M209" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>264</v>
+        <v>956</v>
       </c>
       <c r="B210" t="s">
-        <v>586</v>
+        <v>959</v>
       </c>
       <c r="M210" t="s">
-        <v>692</v>
+        <v>974</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>265</v>
+        <v>957</v>
       </c>
       <c r="B211" t="s">
-        <v>587</v>
+        <v>960</v>
       </c>
       <c r="M211" t="s">
-        <v>267</v>
+        <v>975</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>266</v>
+        <v>702</v>
       </c>
       <c r="B212" t="s">
-        <v>588</v>
+        <v>962</v>
       </c>
       <c r="M212" t="s">
-        <v>268</v>
+        <v>965</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>704</v>
+      </c>
+      <c r="B213" t="s">
+        <v>963</v>
+      </c>
+      <c r="M213" t="s">
+        <v>966</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>269</v>
+        <v>703</v>
       </c>
       <c r="B214" t="s">
-        <v>270</v>
+        <v>964</v>
       </c>
       <c r="M214" t="s">
-        <v>750</v>
+        <v>967</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>705</v>
+      </c>
+      <c r="B215" t="s">
+        <v>701</v>
+      </c>
+      <c r="M215" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>271</v>
+        <v>968</v>
       </c>
       <c r="B216" t="s">
-        <v>543</v>
+        <v>969</v>
       </c>
       <c r="M216" t="s">
-        <v>202</v>
+        <v>970</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>272</v>
+        <v>971</v>
       </c>
       <c r="B217" t="s">
-        <v>589</v>
+        <v>972</v>
       </c>
       <c r="M217" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>274</v>
-      </c>
-      <c r="B218" t="s">
-        <v>589</v>
-      </c>
-      <c r="M218" t="s">
-        <v>273</v>
+        <v>973</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>260</v>
+      </c>
+      <c r="B219" t="s">
+        <v>584</v>
+      </c>
+      <c r="M219" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="B220" t="s">
-        <v>551</v>
+        <v>585</v>
       </c>
       <c r="M220" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>276</v>
-      </c>
-      <c r="B221" t="s">
-        <v>590</v>
-      </c>
-      <c r="M221" t="s">
-        <v>753</v>
+        <v>263</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="B222" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="M222" t="s">
-        <v>753</v>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>265</v>
+      </c>
+      <c r="B223" t="s">
+        <v>587</v>
+      </c>
+      <c r="M223" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B224" t="s">
-        <v>552</v>
+        <v>588</v>
       </c>
       <c r="M224" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>279</v>
-      </c>
-      <c r="B225" t="s">
-        <v>591</v>
-      </c>
-      <c r="M225" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B226" t="s">
-        <v>639</v>
+        <v>270</v>
       </c>
       <c r="M226" t="s">
-        <v>280</v>
+        <v>750</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B228" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="M228" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B229" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="M229" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B230" t="s">
-        <v>640</v>
+        <v>589</v>
       </c>
       <c r="M230" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B232" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="M232" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="B233" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="M233" t="s">
-        <v>289</v>
+        <v>753</v>
       </c>
     </row>
     <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B234" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="M234" t="s">
-        <v>289</v>
+        <v>753</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B236" t="s">
-        <v>594</v>
+        <v>552</v>
       </c>
       <c r="M236" t="s">
-        <v>1028</v>
+        <v>213</v>
       </c>
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B237" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="M237" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="B238" t="s">
-        <v>595</v>
+        <v>639</v>
       </c>
       <c r="M238" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B240" t="s">
-        <v>596</v>
+        <v>553</v>
       </c>
       <c r="M240" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B241" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="M241" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="B242" t="s">
-        <v>595</v>
+        <v>640</v>
       </c>
       <c r="M242" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="B244" t="s">
-        <v>598</v>
+        <v>554</v>
       </c>
       <c r="M244" t="s">
-        <v>301</v>
+        <v>215</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="B245" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="M245" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
       <c r="B246" t="s">
-        <v>641</v>
+        <v>593</v>
       </c>
       <c r="M246" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="B248" t="s">
-        <v>523</v>
+        <v>594</v>
       </c>
       <c r="M248" t="s">
-        <v>171</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B249" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="M249" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B250" t="s">
-        <v>642</v>
+        <v>595</v>
       </c>
       <c r="M250" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="B252" t="s">
-        <v>525</v>
+        <v>596</v>
       </c>
       <c r="M252" t="s">
-        <v>174</v>
+        <v>296</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="B253" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="M253" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
     </row>
     <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="B254" t="s">
-        <v>643</v>
+        <v>595</v>
       </c>
       <c r="M254" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B256" t="s">
-        <v>527</v>
+        <v>598</v>
       </c>
       <c r="M256" t="s">
-        <v>177</v>
+        <v>301</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="B257" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="M257" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="B258" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="M258" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="B260" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="M260" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B261" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="M261" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="B262" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="M262" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="B264" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="M264" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="B265" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="M265" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B266" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="M266" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="B268" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="M268" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="B269" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="M269" t="s">
-        <v>1068</v>
+        <v>317</v>
       </c>
     </row>
     <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B270" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="M270" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B272" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="M272" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="B273" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="M273" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="B274" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="M274" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="B276" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="M276" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="B277" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="M277" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="B278" t="s">
-        <v>607</v>
+        <v>646</v>
       </c>
       <c r="M278" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="B280" t="s">
-        <v>555</v>
+        <v>530</v>
       </c>
       <c r="M280" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B281" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="M281" t="s">
-        <v>341</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="B282" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="M282" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="B284" t="s">
-        <v>560</v>
+        <v>531</v>
       </c>
       <c r="M284" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="B285" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="M285" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="B286" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="M286" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="B288" t="s">
-        <v>562</v>
+        <v>532</v>
       </c>
       <c r="M288" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="B289" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="M289" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
       <c r="B290" t="s">
-        <v>651</v>
+        <v>607</v>
       </c>
       <c r="M290" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="B292" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="M292" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="B293" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="M293" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="B294" t="s">
-        <v>611</v>
+        <v>649</v>
       </c>
       <c r="M294" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
     </row>
     <row r="296" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="B296" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="M296" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="297" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B297" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="M297" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="298" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="B298" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="M298" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="300" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="B300" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="M300" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="301" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="B301" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="M301" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
       <c r="B302" t="s">
-        <v>613</v>
+        <v>651</v>
       </c>
       <c r="M302" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="B304" t="s">
-        <v>569</v>
+        <v>550</v>
       </c>
       <c r="M304" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="B305" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="M305" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="B306" t="s">
-        <v>653</v>
+        <v>611</v>
       </c>
       <c r="M306" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="B308" t="s">
-        <v>615</v>
+        <v>565</v>
       </c>
       <c r="M308" t="s">
-        <v>373</v>
+        <v>231</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>374</v>
+        <v>359</v>
       </c>
       <c r="B309" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="M309" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>376</v>
+        <v>361</v>
       </c>
       <c r="B310" t="s">
-        <v>617</v>
+        <v>652</v>
       </c>
       <c r="M310" t="s">
-        <v>377</v>
+        <v>362</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>378</v>
+        <v>363</v>
       </c>
       <c r="B312" t="s">
-        <v>618</v>
+        <v>566</v>
       </c>
       <c r="M312" t="s">
-        <v>379</v>
+        <v>233</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B313" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="M313" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
       <c r="B314" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="M314" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
       <c r="B316" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="M316" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="317" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>383</v>
+        <v>368</v>
       </c>
       <c r="B317" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="M317" t="s">
-        <v>384</v>
+        <v>369</v>
       </c>
     </row>
     <row r="318" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
       <c r="B318" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="M318" t="s">
-        <v>386</v>
+        <v>371</v>
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>387</v>
+        <v>372</v>
       </c>
       <c r="B320" t="s">
-        <v>571</v>
+        <v>615</v>
       </c>
       <c r="M320" t="s">
-        <v>243</v>
+        <v>373</v>
       </c>
     </row>
     <row r="321" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="B321" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="M321" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="B322" t="s">
-        <v>655</v>
+        <v>617</v>
       </c>
       <c r="M322" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
     </row>
     <row r="324" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="B324" t="s">
-        <v>545</v>
+        <v>618</v>
       </c>
       <c r="M324" t="s">
-        <v>206</v>
+        <v>379</v>
       </c>
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="B325" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="M325" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="B326" t="s">
-        <v>656</v>
+        <v>617</v>
       </c>
       <c r="M326" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>451</v>
-      </c>
-      <c r="B327" t="s">
-        <v>930</v>
-      </c>
-      <c r="M327" t="s">
-        <v>452</v>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>382</v>
+      </c>
+      <c r="B328" t="s">
+        <v>570</v>
+      </c>
+      <c r="M328" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="B329" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="M329" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="B330" t="s">
-        <v>623</v>
+        <v>654</v>
       </c>
       <c r="M330" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
-        <v>400</v>
-      </c>
-      <c r="B331" t="s">
-        <v>623</v>
-      </c>
-      <c r="M331" t="s">
-        <v>399</v>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>387</v>
+      </c>
+      <c r="B332" t="s">
+        <v>571</v>
+      </c>
+      <c r="M332" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="B333" t="s">
-        <v>575</v>
+        <v>620</v>
       </c>
       <c r="M333" t="s">
-        <v>247</v>
+        <v>389</v>
       </c>
     </row>
     <row r="334" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
       <c r="B334" t="s">
-        <v>624</v>
+        <v>655</v>
       </c>
       <c r="M334" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>404</v>
-      </c>
-      <c r="B335" t="s">
-        <v>657</v>
-      </c>
-      <c r="M335" t="s">
-        <v>405</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>392</v>
+      </c>
+      <c r="B336" t="s">
+        <v>545</v>
+      </c>
+      <c r="M336" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="B337" t="s">
-        <v>577</v>
+        <v>621</v>
       </c>
       <c r="M337" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="B338" t="s">
-        <v>625</v>
+        <v>656</v>
       </c>
       <c r="M338" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>410</v>
+        <v>451</v>
       </c>
       <c r="B339" t="s">
-        <v>625</v>
+        <v>930</v>
       </c>
       <c r="M339" t="s">
-        <v>411</v>
+        <v>452</v>
       </c>
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="B341" t="s">
-        <v>544</v>
+        <v>622</v>
       </c>
       <c r="M341" t="s">
-        <v>203</v>
+        <v>397</v>
       </c>
     </row>
     <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B342" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="M342" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="B343" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="M343" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="B345" t="s">
-        <v>627</v>
+        <v>575</v>
       </c>
       <c r="M345" t="s">
-        <v>417</v>
+        <v>247</v>
       </c>
     </row>
     <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B346" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="M346" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="B347" t="s">
-        <v>628</v>
+        <v>657</v>
       </c>
       <c r="M347" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
     </row>
     <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="B349" t="s">
-        <v>629</v>
+        <v>577</v>
       </c>
       <c r="M349" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="B350" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="M350" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
     </row>
     <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B351" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="M351" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="353" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="B353" t="s">
-        <v>578</v>
+        <v>544</v>
       </c>
       <c r="M353" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
     </row>
     <row r="354" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="B354" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="M354" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
     <row r="355" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="B355" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="M355" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
     <row r="357" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="B357" t="s">
-        <v>581</v>
+        <v>627</v>
       </c>
       <c r="M357" t="s">
-        <v>256</v>
+        <v>417</v>
       </c>
     </row>
     <row r="358" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="B358" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="M358" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="359" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B359" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="M359" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="361" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B361" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="M361" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="B362" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="M362" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
     </row>
     <row r="363" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="B363" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="M363" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="B365" t="s">
-        <v>635</v>
+        <v>578</v>
       </c>
       <c r="M365" t="s">
-        <v>693</v>
+        <v>253</v>
       </c>
     </row>
     <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="B366" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="M366" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="367" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="B367" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="M367" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="369" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="B369" t="s">
-        <v>637</v>
+        <v>581</v>
       </c>
       <c r="M369" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
     </row>
     <row r="370" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="B370" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="M370" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="B371" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="M371" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="B373" t="s">
-        <v>168</v>
+        <v>633</v>
       </c>
       <c r="M373" t="s">
-        <v>168</v>
+        <v>435</v>
       </c>
     </row>
     <row r="374" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="B374" t="s">
-        <v>449</v>
+        <v>634</v>
       </c>
       <c r="M374" t="s">
-        <v>712</v>
+        <v>437</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="B375" t="s">
-        <v>449</v>
+        <v>634</v>
       </c>
       <c r="M375" t="s">
-        <v>712</v>
+        <v>437</v>
       </c>
     </row>
     <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="B377" t="s">
-        <v>455</v>
+        <v>635</v>
       </c>
       <c r="M377" t="s">
-        <v>455</v>
+        <v>693</v>
       </c>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="B378" t="s">
-        <v>456</v>
+        <v>636</v>
       </c>
       <c r="M378" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
-        <v>895</v>
-      </c>
-      <c r="B380" t="s">
-        <v>900</v>
-      </c>
-      <c r="M380" t="s">
-        <v>899</v>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>442</v>
+      </c>
+      <c r="B379" t="s">
+        <v>636</v>
+      </c>
+      <c r="M379" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>896</v>
+        <v>443</v>
       </c>
       <c r="B381" t="s">
-        <v>901</v>
+        <v>637</v>
       </c>
       <c r="M381" t="s">
-        <v>898</v>
+        <v>199</v>
       </c>
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>897</v>
+        <v>444</v>
       </c>
       <c r="B382" t="s">
-        <v>901</v>
+        <v>638</v>
       </c>
       <c r="M382" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
-        <v>462</v>
-      </c>
-      <c r="B384" t="s">
-        <v>658</v>
-      </c>
-      <c r="M384" t="s">
-        <v>457</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>446</v>
+      </c>
+      <c r="B383" t="s">
+        <v>638</v>
+      </c>
+      <c r="M383" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="385" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="B385" t="s">
-        <v>659</v>
+        <v>168</v>
       </c>
       <c r="M385" t="s">
-        <v>458</v>
+        <v>168</v>
       </c>
     </row>
     <row r="386" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="B386" t="s">
-        <v>660</v>
+        <v>449</v>
       </c>
       <c r="M386" t="s">
-        <v>459</v>
+        <v>712</v>
       </c>
     </row>
     <row r="387" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="B387" t="s">
-        <v>661</v>
+        <v>449</v>
       </c>
       <c r="M387" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="388" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
-        <v>466</v>
-      </c>
-      <c r="B388" t="s">
-        <v>662</v>
-      </c>
-      <c r="M388" t="s">
-        <v>461</v>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>453</v>
+      </c>
+      <c r="B389" t="s">
+        <v>455</v>
+      </c>
+      <c r="M389" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>473</v>
+        <v>454</v>
       </c>
       <c r="B390" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="391" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
-        <v>814</v>
-      </c>
-      <c r="B391" t="s">
-        <v>816</v>
-      </c>
-      <c r="M391" t="s">
-        <v>818</v>
+        <v>456</v>
+      </c>
+      <c r="M390" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>815</v>
+        <v>895</v>
       </c>
       <c r="B392" t="s">
-        <v>817</v>
+        <v>900</v>
       </c>
       <c r="M392" t="s">
-        <v>819</v>
+        <v>899</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>478</v>
+        <v>896</v>
       </c>
       <c r="B393" t="s">
-        <v>503</v>
+        <v>901</v>
       </c>
       <c r="M393" t="s">
-        <v>468</v>
+        <v>898</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>474</v>
+        <v>897</v>
       </c>
       <c r="B394" t="s">
-        <v>504</v>
+        <v>901</v>
       </c>
       <c r="M394" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
-        <v>475</v>
-      </c>
-      <c r="B395" t="s">
-        <v>505</v>
-      </c>
-      <c r="M395" t="s">
-        <v>470</v>
+        <v>898</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>476</v>
+        <v>1114</v>
       </c>
       <c r="B396" t="s">
-        <v>506</v>
+        <v>1120</v>
       </c>
       <c r="M396" t="s">
-        <v>471</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>477</v>
+        <v>1115</v>
       </c>
       <c r="B397" t="s">
-        <v>507</v>
+        <v>1121</v>
       </c>
       <c r="M397" t="s">
-        <v>472</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="398" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>903</v>
+        <v>1116</v>
       </c>
       <c r="B398" t="s">
-        <v>910</v>
+        <v>1122</v>
       </c>
       <c r="M398" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
-        <v>904</v>
-      </c>
-      <c r="B399" t="s">
-        <v>911</v>
-      </c>
-      <c r="M399" t="s">
-        <v>918</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="400" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>905</v>
+        <v>1117</v>
       </c>
       <c r="B400" t="s">
-        <v>912</v>
+        <v>1123</v>
       </c>
       <c r="M400" t="s">
-        <v>919</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>906</v>
+        <v>1118</v>
       </c>
       <c r="B401" t="s">
-        <v>913</v>
+        <v>1142</v>
       </c>
       <c r="M401" t="s">
-        <v>920</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="402" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>907</v>
+        <v>1119</v>
       </c>
       <c r="B402" t="s">
-        <v>914</v>
+        <v>1124</v>
       </c>
       <c r="M402" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A403" t="s">
-        <v>908</v>
-      </c>
-      <c r="B403" t="s">
-        <v>915</v>
-      </c>
-      <c r="M403" t="s">
-        <v>922</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="404" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>909</v>
+        <v>462</v>
       </c>
       <c r="B404" t="s">
-        <v>916</v>
+        <v>658</v>
       </c>
       <c r="M404" t="s">
-        <v>923</v>
+        <v>457</v>
       </c>
     </row>
     <row r="405" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>924</v>
+        <v>463</v>
       </c>
       <c r="B405" t="s">
-        <v>925</v>
+        <v>659</v>
       </c>
       <c r="M405" t="s">
-        <v>926</v>
+        <v>458</v>
       </c>
     </row>
     <row r="406" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>929</v>
+        <v>464</v>
       </c>
       <c r="B406" t="s">
-        <v>927</v>
+        <v>660</v>
       </c>
       <c r="M406" t="s">
-        <v>928</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>465</v>
+      </c>
+      <c r="B407" t="s">
+        <v>661</v>
+      </c>
+      <c r="M407" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="408" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="B408" t="s">
-        <v>508</v>
+        <v>662</v>
       </c>
       <c r="M408" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A409" t="s">
-        <v>480</v>
-      </c>
-      <c r="B409" t="s">
-        <v>484</v>
-      </c>
-      <c r="M409" t="s">
-        <v>501</v>
+        <v>461</v>
       </c>
     </row>
     <row r="410" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B410" t="s">
-        <v>483</v>
-      </c>
-      <c r="M410" t="s">
-        <v>502</v>
+        <v>467</v>
       </c>
     </row>
     <row r="411" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>935</v>
+        <v>814</v>
       </c>
       <c r="B411" t="s">
-        <v>936</v>
+        <v>816</v>
       </c>
       <c r="M411" t="s">
-        <v>937</v>
+        <v>818</v>
       </c>
     </row>
     <row r="412" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>938</v>
+        <v>815</v>
       </c>
       <c r="B412" t="s">
-        <v>939</v>
+        <v>817</v>
       </c>
       <c r="M412" t="s">
-        <v>940</v>
+        <v>819</v>
       </c>
     </row>
     <row r="413" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>941</v>
+        <v>478</v>
       </c>
       <c r="B413" t="s">
-        <v>942</v>
+        <v>503</v>
       </c>
       <c r="M413" t="s">
-        <v>943</v>
+        <v>468</v>
       </c>
     </row>
     <row r="414" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>1061</v>
+        <v>474</v>
       </c>
       <c r="B414" t="s">
-        <v>1062</v>
+        <v>504</v>
       </c>
       <c r="M414" t="s">
-        <v>1063</v>
+        <v>469</v>
       </c>
     </row>
     <row r="415" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="B415" t="s">
-        <v>813</v>
+        <v>505</v>
       </c>
       <c r="M415" t="s">
-        <v>711</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>476</v>
+      </c>
+      <c r="B416" t="s">
+        <v>506</v>
+      </c>
+      <c r="M416" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
       <c r="B417" t="s">
-        <v>663</v>
+        <v>507</v>
       </c>
       <c r="M417" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
     </row>
     <row r="418" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>490</v>
+        <v>1168</v>
       </c>
       <c r="B418" t="s">
-        <v>664</v>
+        <v>1169</v>
       </c>
       <c r="M418" t="s">
-        <v>486</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="419" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>491</v>
+        <v>903</v>
       </c>
       <c r="B419" t="s">
-        <v>665</v>
+        <v>910</v>
       </c>
       <c r="M419" t="s">
-        <v>487</v>
+        <v>917</v>
       </c>
     </row>
     <row r="420" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>492</v>
+        <v>904</v>
       </c>
       <c r="B420" t="s">
-        <v>666</v>
+        <v>911</v>
       </c>
       <c r="M420" t="s">
-        <v>488</v>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>905</v>
+      </c>
+      <c r="B421" t="s">
+        <v>912</v>
+      </c>
+      <c r="M421" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="422" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>493</v>
+        <v>906</v>
       </c>
       <c r="B422" t="s">
-        <v>694</v>
+        <v>913</v>
       </c>
       <c r="M422" t="s">
-        <v>695</v>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>907</v>
+      </c>
+      <c r="B423" t="s">
+        <v>914</v>
+      </c>
+      <c r="M423" t="s">
+        <v>921</v>
       </c>
     </row>
     <row r="424" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>667</v>
+        <v>908</v>
       </c>
       <c r="B424" t="s">
-        <v>494</v>
+        <v>915</v>
       </c>
       <c r="M424" t="s">
-        <v>498</v>
+        <v>922</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>668</v>
+        <v>909</v>
       </c>
       <c r="B425" t="s">
-        <v>495</v>
+        <v>916</v>
       </c>
       <c r="M425" t="s">
-        <v>497</v>
+        <v>923</v>
       </c>
     </row>
     <row r="426" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>669</v>
+        <v>1173</v>
       </c>
       <c r="B426" t="s">
-        <v>496</v>
+        <v>1170</v>
       </c>
       <c r="M426" t="s">
-        <v>499</v>
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>924</v>
+      </c>
+      <c r="B427" t="s">
+        <v>925</v>
+      </c>
+      <c r="M427" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>500</v>
+        <v>929</v>
       </c>
       <c r="B428" t="s">
-        <v>696</v>
+        <v>927</v>
       </c>
       <c r="M428" t="s">
-        <v>708</v>
+        <v>928</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>697</v>
-      </c>
-      <c r="B430" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="C430" s="1"/>
-      <c r="D430" s="1"/>
-      <c r="E430" s="1"/>
-      <c r="F430" s="1"/>
-      <c r="G430" s="1"/>
-      <c r="H430" s="1"/>
-      <c r="I430" s="1"/>
-      <c r="J430" s="1"/>
-      <c r="K430" s="1"/>
-      <c r="L430" s="1"/>
-      <c r="M430" s="1" t="s">
-        <v>710</v>
+        <v>479</v>
+      </c>
+      <c r="B430" t="s">
+        <v>508</v>
+      </c>
+      <c r="M430" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>698</v>
+        <v>480</v>
       </c>
       <c r="B431" t="s">
-        <v>700</v>
+        <v>484</v>
       </c>
       <c r="M431" t="s">
-        <v>707</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>481</v>
+      </c>
+      <c r="B432" t="s">
+        <v>483</v>
+      </c>
+      <c r="M432" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>713</v>
+        <v>935</v>
       </c>
       <c r="B433" t="s">
-        <v>714</v>
+        <v>936</v>
       </c>
       <c r="M433" t="s">
-        <v>715</v>
+        <v>937</v>
+      </c>
+    </row>
+    <row r="434" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>938</v>
+      </c>
+      <c r="B434" t="s">
+        <v>939</v>
+      </c>
+      <c r="M434" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>716</v>
+        <v>941</v>
       </c>
       <c r="B435" t="s">
-        <v>717</v>
+        <v>942</v>
       </c>
       <c r="M435" t="s">
-        <v>732</v>
+        <v>943</v>
       </c>
     </row>
     <row r="436" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>718</v>
+        <v>1061</v>
       </c>
       <c r="B436" t="s">
-        <v>723</v>
+        <v>1062</v>
       </c>
       <c r="M436" t="s">
-        <v>730</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="437" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>719</v>
+        <v>482</v>
       </c>
       <c r="B437" t="s">
-        <v>724</v>
+        <v>813</v>
       </c>
       <c r="M437" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A438" t="s">
-        <v>720</v>
-      </c>
-      <c r="B438" t="s">
-        <v>725</v>
-      </c>
-      <c r="M438" t="s">
-        <v>731</v>
+        <v>711</v>
       </c>
     </row>
     <row r="439" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>721</v>
+        <v>489</v>
       </c>
       <c r="B439" t="s">
-        <v>287</v>
+        <v>663</v>
       </c>
       <c r="M439" t="s">
-        <v>728</v>
+        <v>485</v>
       </c>
     </row>
     <row r="440" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>722</v>
+        <v>490</v>
       </c>
       <c r="B440" t="s">
-        <v>726</v>
+        <v>664</v>
       </c>
       <c r="M440" t="s">
-        <v>729</v>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>491</v>
+      </c>
+      <c r="B441" t="s">
+        <v>665</v>
+      </c>
+      <c r="M441" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="442" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>821</v>
+        <v>492</v>
       </c>
       <c r="B442" t="s">
-        <v>822</v>
+        <v>666</v>
       </c>
       <c r="M442" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A443" t="s">
-        <v>952</v>
-      </c>
-      <c r="B443" t="s">
-        <v>953</v>
-      </c>
-      <c r="M443" t="s">
-        <v>954</v>
+        <v>488</v>
       </c>
     </row>
     <row r="444" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>825</v>
+        <v>493</v>
       </c>
       <c r="B444" t="s">
-        <v>823</v>
+        <v>694</v>
       </c>
       <c r="M444" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="445" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A445" t="s">
-        <v>828</v>
-      </c>
-      <c r="B445" t="s">
-        <v>823</v>
-      </c>
-      <c r="M445" t="s">
-        <v>829</v>
+        <v>695</v>
       </c>
     </row>
     <row r="446" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>830</v>
+        <v>667</v>
       </c>
       <c r="B446" t="s">
-        <v>826</v>
+        <v>494</v>
       </c>
       <c r="M446" t="s">
-        <v>826</v>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="447" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>668</v>
+      </c>
+      <c r="B447" t="s">
+        <v>495</v>
+      </c>
+      <c r="M447" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="448" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>834</v>
-      </c>
-      <c r="B448" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="C448" s="3"/>
-      <c r="D448" s="3"/>
-      <c r="E448" s="3"/>
-      <c r="F448" s="3"/>
-      <c r="G448" s="3"/>
-      <c r="H448" s="3"/>
-      <c r="I448" s="3"/>
-      <c r="J448" s="3"/>
-      <c r="K448" s="3"/>
-      <c r="L448" s="3"/>
-      <c r="M448" s="2" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A449" t="s">
-        <v>836</v>
-      </c>
-      <c r="B449" s="2" t="s">
-        <v>934</v>
-      </c>
-      <c r="C449" s="3"/>
-      <c r="D449" s="3"/>
-      <c r="E449" s="3"/>
-      <c r="F449" s="3"/>
-      <c r="G449" s="3"/>
-      <c r="H449" s="3"/>
-      <c r="I449" s="3"/>
-      <c r="J449" s="3"/>
-      <c r="K449" s="3"/>
-      <c r="L449" s="3"/>
-      <c r="M449" s="2" t="s">
-        <v>835</v>
+        <v>669</v>
+      </c>
+      <c r="B448" t="s">
+        <v>496</v>
+      </c>
+      <c r="M448" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="450" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
+        <v>500</v>
+      </c>
+      <c r="B450" t="s">
+        <v>696</v>
+      </c>
+      <c r="M450" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>697</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C452" s="1"/>
+      <c r="D452" s="1"/>
+      <c r="E452" s="1"/>
+      <c r="F452" s="1"/>
+      <c r="G452" s="1"/>
+      <c r="H452" s="1"/>
+      <c r="I452" s="1"/>
+      <c r="J452" s="1"/>
+      <c r="K452" s="1"/>
+      <c r="L452" s="1"/>
+      <c r="M452" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>698</v>
+      </c>
+      <c r="B453" t="s">
+        <v>700</v>
+      </c>
+      <c r="M453" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>713</v>
+      </c>
+      <c r="B455" t="s">
+        <v>714</v>
+      </c>
+      <c r="M455" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="457" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>716</v>
+      </c>
+      <c r="B457" t="s">
+        <v>717</v>
+      </c>
+      <c r="M457" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="458" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>718</v>
+      </c>
+      <c r="B458" t="s">
+        <v>723</v>
+      </c>
+      <c r="M458" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="459" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>719</v>
+      </c>
+      <c r="B459" t="s">
+        <v>724</v>
+      </c>
+      <c r="M459" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>720</v>
+      </c>
+      <c r="B460" t="s">
+        <v>725</v>
+      </c>
+      <c r="M460" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="461" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>721</v>
+      </c>
+      <c r="B461" t="s">
+        <v>287</v>
+      </c>
+      <c r="M461" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="462" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>722</v>
+      </c>
+      <c r="B462" t="s">
+        <v>726</v>
+      </c>
+      <c r="M462" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="464" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B464" t="s">
+        <v>1155</v>
+      </c>
+      <c r="M464" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="465" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B465" t="s">
+        <v>1156</v>
+      </c>
+      <c r="M465" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1158</v>
+      </c>
+      <c r="M466" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1159</v>
+      </c>
+      <c r="M467" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="469" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>821</v>
+      </c>
+      <c r="B469" t="s">
+        <v>822</v>
+      </c>
+      <c r="M469" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="470" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>952</v>
+      </c>
+      <c r="B470" t="s">
+        <v>953</v>
+      </c>
+      <c r="M470" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="471" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>825</v>
+      </c>
+      <c r="B471" t="s">
+        <v>823</v>
+      </c>
+      <c r="M471" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="472" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>828</v>
+      </c>
+      <c r="B472" t="s">
+        <v>823</v>
+      </c>
+      <c r="M472" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="473" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>830</v>
+      </c>
+      <c r="B473" t="s">
+        <v>826</v>
+      </c>
+      <c r="M473" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="475" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>834</v>
+      </c>
+      <c r="B475" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="C475" s="3"/>
+      <c r="D475" s="3"/>
+      <c r="E475" s="3"/>
+      <c r="F475" s="3"/>
+      <c r="G475" s="3"/>
+      <c r="H475" s="3"/>
+      <c r="I475" s="3"/>
+      <c r="J475" s="3"/>
+      <c r="K475" s="3"/>
+      <c r="L475" s="3"/>
+      <c r="M475" s="2" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="476" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>836</v>
+      </c>
+      <c r="B476" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C476" s="3"/>
+      <c r="D476" s="3"/>
+      <c r="E476" s="3"/>
+      <c r="F476" s="3"/>
+      <c r="G476" s="3"/>
+      <c r="H476" s="3"/>
+      <c r="I476" s="3"/>
+      <c r="J476" s="3"/>
+      <c r="K476" s="3"/>
+      <c r="L476" s="3"/>
+      <c r="M476" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="477" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
         <v>837</v>
       </c>
-      <c r="B450" t="s">
+      <c r="B477" t="s">
         <v>839</v>
       </c>
-      <c r="M450" t="s">
+      <c r="M477" t="s">
         <v>838</v>
       </c>
     </row>
@@ -7924,10 +8369,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8218,7 +8663,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>997</v>
       </c>
@@ -8436,6 +8881,22 @@
       </c>
       <c r="M42" s="4" t="s">
         <v>1056</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>1178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few fixes to the 2.9.X updates
* translated the updater text
* fix for the game not ending if someone disconnects in the middle
* add a list of what counts as a "light" and a "dark" color to the in-game overlay
* updated README.md
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4585FC9-E822-4C39-8509-871AB77658D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FA636D-649A-41D3-913C-E79EAC8D2876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="2085" windowWidth="28800" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7950" yWindow="2610" windowWidth="22515" windowHeight="13410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="1199">
   <si>
     <t>presetSelection</t>
   </si>
@@ -2541,12 +2541,6 @@
     <t>creditsMain</t>
   </si>
   <si>
-    <t>&lt;size=80%&gt;MOD &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;、
-&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt;、&lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;
-ボタンデザイン &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;
-カスタマイズ・日本語訳 &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;&lt;/size&gt;</t>
-  </si>
-  <si>
     <t>creditsFull</t>
   </si>
   <si>
@@ -2559,10 +2553,6 @@
     <t>GM Edition v{0}</t>
   </si>
   <si>
-    <t>MOD &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;、&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt;、&lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;
-デザイン &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;、カスタマイズ・日本語訳 &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;</t>
-  </si>
-  <si>
     <t>Banner.png</t>
   </si>
   <si>
@@ -2837,16 +2827,6 @@
   </si>
   <si>
     <t>他プレイヤーを殺害・蘇生できる</t>
-  </si>
-  <si>
-    <t>Modded by &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;, &lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;, Design by &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;
-Customization by &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;</t>
-  </si>
-  <si>
-    <t>&lt;size=80%&gt;Modded by &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;,
-&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;
-Button design by &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;
-Customization by &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;&lt;/size&gt;</t>
   </si>
   <si>
     <t>roleSummaryExiled</t>
@@ -3178,12 +3158,6 @@
   <si>
     <t>・死体を消せる&lt;color=#ff1919ff&gt;インポスター&lt;/color&gt;_x000D_
 ・キルすることも可能だが&lt;color=#ff1919ff&gt;クリーナー&lt;/color&gt;の能力とキルクールは同期している</t>
-  </si>
-  <si>
-    <t>・探偵_x000D_
-・プレイヤーの足跡が見える_x000D_
-・一定時間内に死体を発見すると、犯人についての情報が得られる_x000D_
-・会議に入ったら、チャットで表示される</t>
   </si>
   <si>
     <t>・誰か1人にシールドを貼れる_x000D_
@@ -3698,9 +3672,6 @@
     <t>ヴァルチャー</t>
   </si>
   <si>
-    <t>死体を喰らおう</t>
-  </si>
-  <si>
     <t>ミーディアム</t>
   </si>
   <si>
@@ -3758,27 +3729,12 @@
     <t>What is your killer's role? My killer is {0}.</t>
   </si>
   <si>
-    <t>「君の役職は何でしょう」『私は{0}です』</t>
-  </si>
-  <si>
-    <t>「君を殺した人の役職は何でしょう」『私を殺した人は{0}です』</t>
-  </si>
-  <si>
-    <t>「君を殺した人はどんな色でしょう」『私を殺した人は{0}色をしていました』</t>
-  </si>
-  <si>
     <t>必要な死体の数</t>
   </si>
   <si>
     <t>Show Arrows Pointing Towards Corpses</t>
   </si>
   <si>
-    <t>幽霊から情報を聞き出そう</t>
-  </si>
-  <si>
-    <t>残り {0}体</t>
-  </si>
-  <si>
     <t>vultureCorpses</t>
   </si>
   <si>
@@ -3798,9 +3754,6 @@
   </si>
   <si>
     <t>vultureWinExtra</t>
-  </si>
-  <si>
-    <t>「君はいつ死んだんでしょう」『私は会議の{0}秒前に死にました』</t>
   </si>
   <si>
     <t>vultureFullDesc</t>
@@ -3821,6 +3774,142 @@
 and can question them. It then gets random information about the soul or the killer
 in the chat. The souls only stay for one round, i.e. until the next meeting.
 Depending on the options, the souls can only be questioned once and then disappear.</t>
+  </si>
+  <si>
+    <t>死骸を喰らおう</t>
+  </si>
+  <si>
+    <t>&lt;size=80%&gt;Modded by &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;, &lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;
+&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;Mallöris&lt;/color&gt;
+Button design by &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;
+Customization by &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>&lt;size=80%&gt;MOD &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;、&lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;
+&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt;、&lt;color=#FCCE03FF&gt;Mallöris&lt;/color&gt;
+ボタンデザイン &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;
+カスタマイズ・日本語訳 &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;&lt;/size&gt;</t>
+  </si>
+  <si>
+    <t>Modded by &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;, &lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt;, &lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt; &amp; &lt;color=#FCCE03FF&gt;Mallöris&lt;/color&gt;
+Design by &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;, Customization by &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>MOD &lt;color=#FCCE03FF&gt;Eisbison&lt;/color&gt;、&lt;color=#FCCE03FF&gt;Thunderstorm584&lt;/color&gt;、&lt;color=#FCCE03FF&gt;EndOfFile&lt;/color&gt;、&lt;color=#FCCE03FF&gt;Mallöris&lt;/color&gt;
+デザイン &lt;color=#FCCE03FF&gt;Bavari&lt;/color&gt;、カスタマイズ・日本語訳 &lt;color=#c1a9ff&gt;Virtual_Dusk&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>「あなたの役職は何でしょう」『私は{0}です』</t>
+  </si>
+  <si>
+    <t>「あなたを殺した人はどんな色でしょう」『私を殺した人は{0}色をしていました』</t>
+  </si>
+  <si>
+    <t>「あなたはいつ死んだんでしょう」『私は会議の{0}秒前に死にました』</t>
+  </si>
+  <si>
+    <t>「あなたを殺した人の役職は何でしょう」『私を殺した人は{0}です』</t>
+  </si>
+  <si>
+    <t>・一定数の死体を食べると勝利する
+・死体の場所が矢印にてある程度わかる（設定による）
+・食べた死体はその場から消える
+・ベントの使用が可能（設定による）</t>
+  </si>
+  <si>
+    <t>残り {0}人</t>
+  </si>
+  <si>
+    <t>取り残された魂から情報を聞き出そう</t>
+  </si>
+  <si>
+    <t>魂から情報を聞き出そう</t>
+  </si>
+  <si>
+    <t>updatePleaseWait</t>
+  </si>
+  <si>
+    <t>updateManually</t>
+  </si>
+  <si>
+    <t>updateInProgress</t>
+  </si>
+  <si>
+    <t>updateRestart</t>
+  </si>
+  <si>
+    <t>updateFailed</t>
+  </si>
+  <si>
+    <t>Unable to auto-update.
+Please update manually.</t>
+  </si>
+  <si>
+    <t>Update might already
+be in progress.</t>
+  </si>
+  <si>
+    <t>Update failed.
+Try again later,
+or update manually.</t>
+  </si>
+  <si>
+    <t>Update
+The Other Roles GM</t>
+  </si>
+  <si>
+    <t>アップデート中
+少々お待ちください…</t>
+  </si>
+  <si>
+    <t>アップデート実行中</t>
+  </si>
+  <si>
+    <t>Updating The Other Roles GM
+Please wait...</t>
+  </si>
+  <si>
+    <t>The Other Roles GM
+updated successfully.
+Please restart the game.</t>
+  </si>
+  <si>
+    <t>The Other Roles GMの
+アップデートが完了しました
+ゲームを再起動してください</t>
+  </si>
+  <si>
+    <t>自動アップデートが
+できませんでした
+手動で更新してください</t>
+  </si>
+  <si>
+    <t>updateButton</t>
+  </si>
+  <si>
+    <t>TOR GMを
+アップデート</t>
+  </si>
+  <si>
+    <t xml:space="preserve">・魂から情報を得られる
+・死体が上がった次のターンその魂が見える
+・魂は次の会議後に消える
+【色調表記】
+・濃い色
+　赤、青、緑、黒、紫、茶、マルーン、タン
+・淡い色
+　ピンク、オレンジ、黄色、白、水色、黄緑、ローズ、　バナナ、グレー、コーラル </t>
+  </si>
+  <si>
+    <t xml:space="preserve">・探偵
+・プレイヤーの足跡が見える
+・一定時間内に死体を発見すると、犯人についての情報が得られる
+・会議に入ったら、チャットで表示される
+【色調表記】
+・濃い色
+　赤、青、緑、黒、紫、茶、マルーン、タン
+・淡い色
+　ピンク、オレンジ、黄色、白、水色、黄緑、ローズ、　バナナ、グレー、コーラル </t>
   </si>
 </sst>
 </file>
@@ -4144,15 +4233,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q477"/>
+  <dimension ref="A1:Q484"/>
   <sheetViews>
-    <sheetView topLeftCell="A446" workbookViewId="0">
-      <selection activeCell="M467" sqref="M467"/>
+    <sheetView topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="M484" sqref="M484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -4378,7 +4469,7 @@
         <v>759</v>
       </c>
       <c r="M18" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -4389,7 +4480,7 @@
         <v>760</v>
       </c>
       <c r="M19" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -4493,13 +4584,13 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1059</v>
+        <v>1054</v>
       </c>
       <c r="B34" t="s">
-        <v>1067</v>
+        <v>1062</v>
       </c>
       <c r="M34" t="s">
-        <v>1060</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -4823,13 +4914,13 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="B73" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="M73" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4837,10 +4928,10 @@
         <v>29</v>
       </c>
       <c r="B74" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="M74" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4878,24 +4969,24 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1064</v>
+        <v>1059</v>
       </c>
       <c r="B79" t="s">
-        <v>1065</v>
+        <v>1060</v>
       </c>
       <c r="M79" t="s">
-        <v>1066</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="B80" t="s">
-        <v>1150</v>
+        <v>1144</v>
       </c>
       <c r="M80" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -5087,13 +5178,13 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>1148</v>
+        <v>1142</v>
       </c>
       <c r="B101" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
       <c r="M101" t="s">
-        <v>1151</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -5186,13 +5277,13 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="B114" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="M114" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -5593,7 +5684,7 @@
         <v>789</v>
       </c>
       <c r="M157" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -5884,40 +5975,40 @@
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B191" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="M191" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="B193" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="M193" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="B194" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="M194" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="B195" t="s">
         <v>779</v>
@@ -5928,57 +6019,57 @@
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="B196" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="M196" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>1167</v>
+        <v>1156</v>
       </c>
       <c r="B197" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="M197" t="s">
-        <v>1166</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="B199" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="M199" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
       <c r="B200" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="M200" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="B201" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="M201" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.25">
@@ -5986,7 +6077,7 @@
         <v>133</v>
       </c>
       <c r="B203" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="M203" t="s">
         <v>751</v>
@@ -5997,7 +6088,7 @@
         <v>134</v>
       </c>
       <c r="B204" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="M204" t="s">
         <v>752</v>
@@ -6027,46 +6118,46 @@
     </row>
     <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>1069</v>
+        <v>1064</v>
       </c>
       <c r="B207" t="s">
-        <v>1071</v>
+        <v>1066</v>
       </c>
       <c r="M207" t="s">
-        <v>1070</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="B209" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="M209" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="B210" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="M210" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="B211" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="M211" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -6074,10 +6165,10 @@
         <v>702</v>
       </c>
       <c r="B212" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="M212" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.25">
@@ -6085,10 +6176,10 @@
         <v>704</v>
       </c>
       <c r="B213" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="M213" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.25">
@@ -6096,10 +6187,10 @@
         <v>703</v>
       </c>
       <c r="B214" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="M214" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.25">
@@ -6115,24 +6206,24 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="B216" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="M216" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="B217" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="M217" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.25">
@@ -6374,7 +6465,7 @@
         <v>594</v>
       </c>
       <c r="M248" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
@@ -6649,7 +6740,7 @@
         <v>605</v>
       </c>
       <c r="M281" t="s">
-        <v>1068</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.25">
@@ -7130,7 +7221,7 @@
         <v>451</v>
       </c>
       <c r="B339" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="M339" t="s">
         <v>452</v>
@@ -7556,101 +7647,101 @@
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B392" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="M392" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
+        <v>894</v>
+      </c>
+      <c r="B393" t="s">
+        <v>899</v>
+      </c>
+      <c r="M393" t="s">
         <v>896</v>
-      </c>
-      <c r="B393" t="s">
-        <v>901</v>
-      </c>
-      <c r="M393" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="B394" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="M394" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="B396" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="M396" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="B397" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="M397" t="s">
-        <v>1140</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="398" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="B398" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
       <c r="M398" t="s">
-        <v>1140</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="400" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="B400" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="M400" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
       <c r="B401" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="M401" t="s">
-        <v>1165</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="402" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B402" t="s">
         <v>1119</v>
       </c>
-      <c r="B402" t="s">
-        <v>1124</v>
-      </c>
       <c r="M402" t="s">
-        <v>1165</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="404" spans="1:13" x14ac:dyDescent="0.25">
@@ -7795,123 +7886,123 @@
     </row>
     <row r="418" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>1168</v>
+        <v>1157</v>
       </c>
       <c r="B418" t="s">
-        <v>1169</v>
+        <v>1158</v>
       </c>
       <c r="M418" t="s">
-        <v>1171</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="419" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B419" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="M419" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="420" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B420" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="M420" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="421" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="B421" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="M421" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="422" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B422" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="M422" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="423" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="B423" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="M423" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="424" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B424" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="M424" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B425" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="M425" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="426" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>1173</v>
+        <v>1162</v>
       </c>
       <c r="B426" t="s">
-        <v>1170</v>
+        <v>1159</v>
       </c>
       <c r="M426" t="s">
-        <v>1172</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="427" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
+        <v>922</v>
+      </c>
+      <c r="B427" t="s">
+        <v>923</v>
+      </c>
+      <c r="M427" t="s">
         <v>924</v>
-      </c>
-      <c r="B427" t="s">
-        <v>925</v>
-      </c>
-      <c r="M427" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="428" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="B428" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="M428" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.25">
@@ -7949,46 +8040,46 @@
     </row>
     <row r="433" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="B433" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="M433" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
     </row>
     <row r="434" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="B434" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="M434" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="B435" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="M435" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="436" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>1061</v>
+        <v>1056</v>
       </c>
       <c r="B436" t="s">
-        <v>1062</v>
+        <v>1057</v>
       </c>
       <c r="M436" t="s">
-        <v>1063</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="437" spans="1:13" x14ac:dyDescent="0.25">
@@ -8212,32 +8303,32 @@
     </row>
     <row r="464" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1152</v>
+        <v>1146</v>
       </c>
       <c r="B464" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="M464" t="s">
-        <v>1160</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="465" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1153</v>
+        <v>1147</v>
       </c>
       <c r="B465" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="M465" t="s">
-        <v>1162</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="466" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="B466" t="s">
-        <v>1158</v>
+        <v>1152</v>
       </c>
       <c r="M466" t="s">
         <v>1174</v>
@@ -8245,13 +8336,13 @@
     </row>
     <row r="467" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="B467" t="s">
-        <v>1159</v>
+        <v>1153</v>
       </c>
       <c r="M467" t="s">
-        <v>1161</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="469" spans="1:13" x14ac:dyDescent="0.25">
@@ -8267,13 +8358,13 @@
     </row>
     <row r="470" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
       <c r="B470" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="M470" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="471" spans="1:13" x14ac:dyDescent="0.25">
@@ -8314,7 +8405,7 @@
         <v>834</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>933</v>
+        <v>1170</v>
       </c>
       <c r="C475" s="3"/>
       <c r="D475" s="3"/>
@@ -8327,15 +8418,15 @@
       <c r="K475" s="3"/>
       <c r="L475" s="3"/>
       <c r="M475" s="2" t="s">
-        <v>840</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="476" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>934</v>
+        <v>1168</v>
       </c>
       <c r="C476" s="3"/>
       <c r="D476" s="3"/>
@@ -8348,18 +8439,84 @@
       <c r="K476" s="3"/>
       <c r="L476" s="3"/>
       <c r="M476" s="2" t="s">
-        <v>835</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="477" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
+        <v>836</v>
+      </c>
+      <c r="B477" t="s">
+        <v>838</v>
+      </c>
+      <c r="M477" t="s">
         <v>837</v>
       </c>
-      <c r="B477" t="s">
-        <v>839</v>
-      </c>
-      <c r="M477" t="s">
-        <v>838</v>
+    </row>
+    <row r="479" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B479" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="M479" s="4" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="480" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B480" s="4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M480" s="4" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="481" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B481" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="M481" s="4" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="482" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B482" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="M482" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="483" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B483" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="M483" s="4" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="484" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B484" s="4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="M484" s="4" t="s">
+        <v>1194</v>
       </c>
     </row>
   </sheetData>
@@ -8371,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8434,469 +8591,475 @@
     </row>
     <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1083</v>
+        <v>1078</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1084</v>
+        <v>1079</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1085</v>
+        <v>1080</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>1053</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1086</v>
+        <v>1081</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1076</v>
+        <v>1071</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1075</v>
+        <v>1070</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1074</v>
+        <v>1069</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1088</v>
+        <v>1083</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1089</v>
+        <v>1084</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1073</v>
+        <v>1068</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>1057</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1090</v>
+        <v>1085</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1072</v>
+        <v>1067</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1091</v>
+        <v>1086</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>1055</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1092</v>
+        <v>1087</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1093</v>
+        <v>1088</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>1040</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1094</v>
+        <v>1089</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>1095</v>
+        <v>1090</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>1041</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1096</v>
+        <v>1091</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1097</v>
+        <v>1092</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>1043</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1098</v>
+        <v>1093</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1099</v>
+        <v>1094</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>1045</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1100</v>
+        <v>1095</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>1046</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>1047</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1104</v>
+        <v>1099</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>1048</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1105</v>
+        <v>1100</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>1049</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1106</v>
+        <v>1101</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1107</v>
+        <v>1102</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>1050</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>1051</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>1079</v>
+        <v>1074</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>1052</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1078</v>
+        <v>1073</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>1082</v>
+        <v>1077</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>1058</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>1056</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1175</v>
+        <v>1163</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>1165</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1176</v>
+        <v>1164</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>1178</v>
+        <v>1166</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>1197</v>
       </c>
     </row>
   </sheetData>
@@ -8969,218 +9132,218 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B2" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B3" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="B4" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B5" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="B6" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B7" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B8" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B9" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="B10" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B11" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="B12" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B13" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B14" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B15" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B16" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B17" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B18" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B19" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B20" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="B21" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B22" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B23" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B24" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B25" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B26" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B27" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B28" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed a bug with lovers not showing the description properly
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1087D9B0-616F-4C4E-BA4A-E0B39E2FF170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2F8953-0FC0-4CEE-A3A4-A252B7D9E8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2220" windowWidth="24465" windowHeight="12570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="3720" windowWidth="23325" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -5184,8 +5184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q529"/>
   <sheetViews>
-    <sheetView topLeftCell="A491" workbookViewId="0">
-      <selection activeCell="A505" sqref="A505"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="A419" sqref="A419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9818,7 +9818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
probably the final update for v3.3.0
* changes across the codebase to prepare for pluralizing all roles
* move the ninja button code into the ninja file
* better divide the shared per-instance code and per-role code
* fix a bug where a lover trying to shift their partner resulted in a one-person couple
* pluralize sheriff
* don't show the "lovers" role name anywhere, only the colored heart
  this makes the UI a bit cleaner and easier to read
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED94ACED-5F45-466D-BB95-84B91E0CEB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E3509F-D64F-421F-9D0B-70F02F3BFEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3960" windowWidth="24795" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="4125" windowWidth="24795" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -5233,12 +5233,6 @@
     <t>shifterIsNeutralRate</t>
   </si>
   <si>
-    <t>Chance Shifter Is Neutral</t>
-  </si>
-  <si>
-    <t>第３陣営になる確率</t>
-  </si>
-  <si>
     <t>swapperSwapsLeft</t>
   </si>
   <si>
@@ -5499,6 +5493,12 @@
   </si>
   <si>
     <t>忍術中、他人にターゲットされる</t>
+  </si>
+  <si>
+    <t>チェインシフターになる確率</t>
+  </si>
+  <si>
+    <t>Chance Shifter Is Chain Shifter</t>
   </si>
 </sst>
 </file>
@@ -5825,8 +5825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B522" workbookViewId="0">
-      <selection activeCell="B528" sqref="B528"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="B239" sqref="B239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6592,13 +6592,13 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1700</v>
+      </c>
+      <c r="M98" t="s">
         <v>1701</v>
-      </c>
-      <c r="B98" t="s">
-        <v>1702</v>
-      </c>
-      <c r="M98" t="s">
-        <v>1703</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -7025,7 +7025,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="B163" t="s">
         <v>556</v>
@@ -7036,7 +7036,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="B164" t="s">
         <v>557</v>
@@ -7047,7 +7047,7 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="B165" t="s">
         <v>557</v>
@@ -7058,7 +7058,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="B167" t="s">
         <v>558</v>
@@ -7069,7 +7069,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="B168" t="s">
         <v>557</v>
@@ -7080,7 +7080,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="B169" t="s">
         <v>557</v>
@@ -7157,24 +7157,24 @@
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B177" t="s">
         <v>1632</v>
       </c>
-      <c r="B177" t="s">
-        <v>1634</v>
-      </c>
       <c r="M177" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="B178" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="M178" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
@@ -7190,10 +7190,10 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="B181" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="M181" t="s">
         <v>632</v>
@@ -7559,7 +7559,7 @@
         <v>540</v>
       </c>
       <c r="M232" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="233" spans="1:13" x14ac:dyDescent="0.25">
@@ -7570,23 +7570,23 @@
         <v>540</v>
       </c>
       <c r="M233" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="B235" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="M235" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="B236" t="s">
         <v>1619</v>
@@ -7597,7 +7597,7 @@
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="B237" t="s">
         <v>1619</v>
@@ -7611,10 +7611,10 @@
         <v>1621</v>
       </c>
       <c r="B239" t="s">
-        <v>1622</v>
+        <v>1708</v>
       </c>
       <c r="M239" t="s">
-        <v>1623</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.25">
@@ -7630,13 +7630,13 @@
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B241" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="M241" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
@@ -8389,13 +8389,13 @@
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="B348" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="M348" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">
@@ -8580,35 +8580,35 @@
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B372" t="s">
         <v>1637</v>
       </c>
-      <c r="B372" t="s">
-        <v>1639</v>
-      </c>
       <c r="M372" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B373" t="s">
         <v>1638</v>
       </c>
-      <c r="B373" t="s">
-        <v>1640</v>
-      </c>
       <c r="M373" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B375" t="s">
+        <v>1644</v>
+      </c>
+      <c r="M375" t="s">
         <v>1645</v>
-      </c>
-      <c r="B375" t="s">
-        <v>1646</v>
-      </c>
-      <c r="M375" t="s">
-        <v>1647</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.25">
@@ -9635,44 +9635,44 @@
     </row>
     <row r="525" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="B525" t="s">
+        <v>1665</v>
+      </c>
+      <c r="M525" t="s">
         <v>1667</v>
-      </c>
-      <c r="M525" t="s">
-        <v>1669</v>
       </c>
     </row>
     <row r="526" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="B526" t="s">
+        <v>1666</v>
+      </c>
+      <c r="M526" t="s">
         <v>1668</v>
-      </c>
-      <c r="M526" t="s">
-        <v>1670</v>
       </c>
     </row>
     <row r="527" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B527" t="s">
         <v>1666</v>
       </c>
-      <c r="B527" t="s">
+      <c r="M527" t="s">
         <v>1668</v>
-      </c>
-      <c r="M527" t="s">
-        <v>1670</v>
       </c>
     </row>
     <row r="528" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="B528" s="4"/>
       <c r="M528" s="4" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="529" spans="1:13" x14ac:dyDescent="0.25">
@@ -9681,62 +9681,62 @@
     </row>
     <row r="530" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="B530" s="4" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="M530" s="4" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="531" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="B531" s="4" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="M531" s="4" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="532" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="M532" s="4" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="533" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="B533" s="4" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="M533" s="4" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="534" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="B534" s="4" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="M534" s="4" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="535" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="B535" t="s">
         <v>700</v>
@@ -9747,13 +9747,13 @@
     </row>
     <row r="536" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B536" s="4" t="s">
+        <v>1705</v>
+      </c>
+      <c r="M536" s="4" t="s">
         <v>1706</v>
-      </c>
-      <c r="B536" s="4" t="s">
-        <v>1707</v>
-      </c>
-      <c r="M536" s="4" t="s">
-        <v>1708</v>
       </c>
     </row>
     <row r="540" spans="1:13" x14ac:dyDescent="0.25">
@@ -10077,13 +10077,13 @@
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1689</v>
+      </c>
+      <c r="M583" t="s">
         <v>1690</v>
-      </c>
-      <c r="B583" t="s">
-        <v>1691</v>
-      </c>
-      <c r="M583" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="587" spans="1:13" x14ac:dyDescent="0.25">
@@ -10906,13 +10906,13 @@
     </row>
     <row r="672" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="B672" t="s">
         <v>744</v>
       </c>
       <c r="M672" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="673" spans="1:13" x14ac:dyDescent="0.25">
@@ -10928,24 +10928,24 @@
     </row>
     <row r="674" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="B674" t="s">
         <v>744</v>
       </c>
       <c r="M674" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="675" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="B675" s="5" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="M675" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="677" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -11603,18 +11603,18 @@
     </row>
     <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
     </row>
   </sheetData>
@@ -12664,24 +12664,24 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M33" t="s">
         <v>1675</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1676</v>
-      </c>
-      <c r="M33" t="s">
-        <v>1677</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B34" t="s">
         <v>1685</v>
       </c>
-      <c r="B34" t="s">
-        <v>1687</v>
-      </c>
       <c r="M34" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readme, add some missing text
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E3509F-D64F-421F-9D0B-70F02F3BFEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493E62C4-A79B-43E1-A7D1-D2722B4D5A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="4125" windowWidth="24795" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10065" yWindow="3240" windowWidth="24795" windowHeight="13890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="1709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="1711">
   <si>
     <t>presetSelection</t>
   </si>
@@ -5499,6 +5499,20 @@
   </si>
   <si>
     <t>Chance Shifter Is Chain Shifter</t>
+  </si>
+  <si>
+    <t>The Ninja is an Impostor that can turn invisible.
+While stealthed, the Ninja moves faster than a normal Crewmate,
+and kills don't cause them to warp. However, using their stealth ability
+increases their kill cooldown--a penalty for killing while invisible,
+and a short penalty applied after unstealthing.</t>
+  </si>
+  <si>
+    <t>A Neutral version of the Shifter, known as the Chain-Shifter,
+is able to steal roles from any player, regardless of their team.
+The shifted player then inherits the role of Chain-Shifter, and must
+steal another player's role. The player who retains the Chain-Shifter
+role at the end of the game automatically loses.</t>
   </si>
 </sst>
 </file>
@@ -5825,8 +5839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="A227" sqref="A227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9666,11 +9680,13 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="528" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>1658</v>
       </c>
-      <c r="B528" s="4"/>
+      <c r="B528" s="4" t="s">
+        <v>1709</v>
+      </c>
       <c r="M528" s="4" t="s">
         <v>1660</v>
       </c>
@@ -11056,8 +11072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11601,9 +11617,12 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1656</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>998</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>1659</v>
@@ -11612,6 +11631,9 @@
     <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1657</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>1710</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>1661</v>

</xml_diff>

<commit_message>
was not handling FixedUpdate for roles even remotely correctly
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35376C26-3A02-4EC8-AB28-E7A8CBFC7282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF85839-7DB9-416E-A72B-3D729521165A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="2325" windowWidth="24795" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1590" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="1759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="1768">
   <si>
     <t>presetSelection</t>
   </si>
@@ -5569,9 +5569,6 @@
     <t>plagueDoctorDuration</t>
   </si>
   <si>
-    <t>感染距離</t>
-  </si>
-  <si>
     <t>感染に必要な時間</t>
   </si>
   <si>
@@ -5657,6 +5654,36 @@
   </si>
   <si>
     <t>感染クールダウン</t>
+  </si>
+  <si>
+    <t>plagueDoctorInfectKiller</t>
+  </si>
+  <si>
+    <t>plagueDoctorResetMeeting</t>
+  </si>
+  <si>
+    <t>Infect Killer</t>
+  </si>
+  <si>
+    <t>殺した人を自動的に感染させる</t>
+  </si>
+  <si>
+    <t>Partial Infections Reset After Meeting</t>
+  </si>
+  <si>
+    <t>会議後、途中感染状態がリセットされる</t>
+  </si>
+  <si>
+    <t>感染範囲</t>
+  </si>
+  <si>
+    <t>plagueDoctorWinDead</t>
+  </si>
+  <si>
+    <t>Can Still Win After Death</t>
+  </si>
+  <si>
+    <t>死亡後でも勝利できる</t>
   </si>
 </sst>
 </file>
@@ -5981,10 +6008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q711"/>
+  <dimension ref="A1:Q714"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B536" workbookViewId="0">
-      <selection activeCell="M548" sqref="M548"/>
+      <selection activeCell="M556" sqref="M556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9984,24 +10011,24 @@
     </row>
     <row r="548" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B548" t="s">
         <v>1756</v>
       </c>
-      <c r="B548" t="s">
+      <c r="M548" t="s">
         <v>1757</v>
-      </c>
-      <c r="M548" t="s">
-        <v>1758</v>
       </c>
     </row>
     <row r="549" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B549" t="s">
         <v>1751</v>
       </c>
-      <c r="B549" t="s">
-        <v>1752</v>
-      </c>
       <c r="M549" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="550" spans="1:13" x14ac:dyDescent="0.25">
@@ -10009,10 +10036,10 @@
         <v>1727</v>
       </c>
       <c r="B550" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="M550" t="s">
-        <v>1729</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="551" spans="1:13" x14ac:dyDescent="0.25">
@@ -10020,51 +10047,62 @@
         <v>1728</v>
       </c>
       <c r="B551" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="M551" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="552" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B552" t="s">
         <v>1748</v>
       </c>
-      <c r="B552" t="s">
+      <c r="M552" t="s">
         <v>1749</v>
       </c>
-      <c r="M552" t="s">
-        <v>1750</v>
+    </row>
+    <row r="553" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1760</v>
+      </c>
+      <c r="M553" t="s">
+        <v>1761</v>
       </c>
     </row>
     <row r="554" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>1740</v>
+        <v>1759</v>
       </c>
       <c r="B554" t="s">
-        <v>1741</v>
+        <v>1762</v>
       </c>
       <c r="M554" t="s">
-        <v>1743</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="555" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1738</v>
+        <v>1765</v>
       </c>
       <c r="B555" t="s">
-        <v>1739</v>
+        <v>1766</v>
       </c>
       <c r="M555" t="s">
-        <v>1742</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="557" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>1746</v>
+        <v>1739</v>
       </c>
       <c r="B557" t="s">
-        <v>1747</v>
+        <v>1740</v>
       </c>
       <c r="M557" t="s">
         <v>1742</v>
@@ -10072,950 +10110,909 @@
     </row>
     <row r="558" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1738</v>
+      </c>
+      <c r="M558" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="560" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B560" t="s">
+        <v>1746</v>
+      </c>
+      <c r="M560" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="561" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B561" t="s">
+        <v>882</v>
+      </c>
+      <c r="M561" t="s">
         <v>1753</v>
       </c>
-      <c r="B558" t="s">
-        <v>882</v>
-      </c>
-      <c r="M558" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="562" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A562" t="s">
+    </row>
+    <row r="565" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
         <v>1244</v>
       </c>
-      <c r="B562" t="s">
+      <c r="B565" t="s">
         <v>1245</v>
       </c>
-      <c r="M562" t="s">
+      <c r="M565" t="s">
         <v>1246</v>
       </c>
     </row>
-    <row r="566" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A566" t="s">
+    <row r="569" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
         <v>374</v>
       </c>
-      <c r="B566" t="s">
+      <c r="B569" t="s">
         <v>562</v>
       </c>
-      <c r="M566" t="s">
+      <c r="M569" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="567" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
+    <row r="570" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
         <v>376</v>
       </c>
-      <c r="B567" t="s">
+      <c r="B570" t="s">
         <v>563</v>
       </c>
-      <c r="M567" t="s">
+      <c r="M570" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="568" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A568" t="s">
+    <row r="571" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
         <v>378</v>
       </c>
-      <c r="B568" t="s">
+      <c r="B571" t="s">
         <v>563</v>
       </c>
-      <c r="M568" t="s">
+      <c r="M571" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="572" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A572" t="s">
+    <row r="575" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
         <v>379</v>
       </c>
-      <c r="B572" t="s">
+      <c r="B575" t="s">
         <v>564</v>
       </c>
-      <c r="M572" t="s">
+      <c r="M575" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="573" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A573" t="s">
+    <row r="576" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
         <v>380</v>
       </c>
-      <c r="B573" t="s">
+      <c r="B576" t="s">
         <v>565</v>
       </c>
-      <c r="M573" t="s">
+      <c r="M576" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="574" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A574" t="s">
+    <row r="577" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
         <v>382</v>
       </c>
-      <c r="B574" t="s">
+      <c r="B577" t="s">
         <v>565</v>
       </c>
-      <c r="M574" t="s">
+      <c r="M577" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="578" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A578" t="s">
+    <row r="581" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
         <v>1351</v>
       </c>
-      <c r="B578" t="s">
+      <c r="B581" t="s">
         <v>1354</v>
       </c>
-      <c r="M578" t="s">
+      <c r="M581" t="s">
         <v>1357</v>
-      </c>
-    </row>
-    <row r="579" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A579" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B579" t="s">
-        <v>1355</v>
-      </c>
-      <c r="M579" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="580" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A580" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B580" t="s">
-        <v>1356</v>
-      </c>
-      <c r="M580" t="s">
-        <v>1359</v>
       </c>
     </row>
     <row r="582" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>100</v>
+        <v>1352</v>
       </c>
       <c r="B582" t="s">
-        <v>1013</v>
+        <v>1355</v>
       </c>
       <c r="M582" t="s">
-        <v>674</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>101</v>
+        <v>1353</v>
       </c>
       <c r="B583" t="s">
-        <v>1014</v>
+        <v>1356</v>
       </c>
       <c r="M583" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="584" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A584" t="s">
-        <v>102</v>
-      </c>
-      <c r="B584" t="s">
-        <v>512</v>
-      </c>
-      <c r="M584" t="s">
-        <v>211</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="585" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B585" t="s">
-        <v>513</v>
+        <v>1013</v>
       </c>
       <c r="M585" t="s">
-        <v>212</v>
+        <v>674</v>
       </c>
     </row>
     <row r="586" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
-        <v>970</v>
+        <v>101</v>
       </c>
       <c r="B586" t="s">
-        <v>972</v>
+        <v>1014</v>
       </c>
       <c r="M586" t="s">
-        <v>971</v>
+        <v>675</v>
       </c>
     </row>
     <row r="587" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>1397</v>
+        <v>102</v>
       </c>
       <c r="B587" t="s">
-        <v>1398</v>
+        <v>512</v>
       </c>
       <c r="M587" t="s">
-        <v>1399</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="588" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>103</v>
+      </c>
+      <c r="B588" t="s">
+        <v>513</v>
+      </c>
+      <c r="M588" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="589" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>865</v>
+        <v>970</v>
       </c>
       <c r="B589" t="s">
-        <v>868</v>
+        <v>972</v>
       </c>
       <c r="M589" t="s">
-        <v>871</v>
+        <v>971</v>
       </c>
     </row>
     <row r="590" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>866</v>
+        <v>1397</v>
       </c>
       <c r="B590" t="s">
-        <v>869</v>
+        <v>1398</v>
       </c>
       <c r="M590" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="591" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
-        <v>867</v>
-      </c>
-      <c r="B591" t="s">
-        <v>870</v>
-      </c>
-      <c r="M591" t="s">
-        <v>885</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="592" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
-        <v>626</v>
+        <v>865</v>
       </c>
       <c r="B592" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="M592" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="593" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
-        <v>628</v>
+        <v>866</v>
       </c>
       <c r="B593" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="M593" t="s">
-        <v>876</v>
+        <v>884</v>
       </c>
     </row>
     <row r="594" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>627</v>
+        <v>867</v>
       </c>
       <c r="B594" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="M594" t="s">
-        <v>877</v>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="595" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>626</v>
+      </c>
+      <c r="B595" t="s">
+        <v>872</v>
+      </c>
+      <c r="M595" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="596" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>878</v>
+        <v>628</v>
       </c>
       <c r="B596" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="M596" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="597" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>881</v>
+        <v>627</v>
       </c>
       <c r="B597" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="M597" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
     </row>
     <row r="599" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A599" t="s">
-        <v>1097</v>
+        <v>878</v>
       </c>
       <c r="B599" t="s">
-        <v>1098</v>
+        <v>879</v>
       </c>
       <c r="M599" t="s">
-        <v>1099</v>
+        <v>880</v>
       </c>
     </row>
     <row r="600" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>1085</v>
+        <v>881</v>
       </c>
       <c r="B600" t="s">
-        <v>1087</v>
+        <v>882</v>
       </c>
       <c r="M600" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="601" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
-        <v>1086</v>
-      </c>
-      <c r="B601" t="s">
-        <v>1088</v>
-      </c>
-      <c r="M601" t="s">
-        <v>1090</v>
+        <v>883</v>
       </c>
     </row>
     <row r="602" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>629</v>
+        <v>1097</v>
       </c>
       <c r="B602" t="s">
-        <v>625</v>
+        <v>1098</v>
       </c>
       <c r="M602" t="s">
-        <v>630</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="603" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1525</v>
+        <v>1085</v>
       </c>
       <c r="B603" t="s">
-        <v>1526</v>
+        <v>1087</v>
       </c>
       <c r="M603" t="s">
-        <v>1527</v>
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="604" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B604" t="s">
+        <v>1088</v>
+      </c>
+      <c r="M604" t="s">
+        <v>1090</v>
       </c>
     </row>
     <row r="605" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
+        <v>629</v>
+      </c>
+      <c r="B605" t="s">
+        <v>625</v>
+      </c>
+      <c r="M605" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="606" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B606" t="s">
+        <v>1526</v>
+      </c>
+      <c r="M606" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="608" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
         <v>1688</v>
       </c>
-      <c r="B605" t="s">
+      <c r="B608" t="s">
         <v>1689</v>
       </c>
-      <c r="M605" t="s">
+      <c r="M608" t="s">
         <v>1690</v>
-      </c>
-    </row>
-    <row r="609" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
-        <v>213</v>
-      </c>
-      <c r="B609" t="s">
-        <v>514</v>
-      </c>
-      <c r="M609" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="610" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A610" t="s">
-        <v>214</v>
-      </c>
-      <c r="B610" t="s">
-        <v>515</v>
-      </c>
-      <c r="M610" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="612" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B612" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="M612" t="s">
-        <v>1470</v>
+        <v>215</v>
       </c>
     </row>
     <row r="613" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B613" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="M613" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="614" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A614" t="s">
-        <v>219</v>
-      </c>
-      <c r="B614" t="s">
-        <v>518</v>
-      </c>
-      <c r="M614" t="s">
-        <v>1472</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="615" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>217</v>
+      </c>
+      <c r="B615" t="s">
+        <v>516</v>
+      </c>
+      <c r="M615" t="s">
+        <v>1470</v>
       </c>
     </row>
     <row r="616" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
+        <v>218</v>
+      </c>
+      <c r="B616" t="s">
+        <v>517</v>
+      </c>
+      <c r="M616" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="617" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>219</v>
+      </c>
+      <c r="B617" t="s">
+        <v>518</v>
+      </c>
+      <c r="M617" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="619" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
         <v>220</v>
       </c>
-      <c r="B616" t="s">
+      <c r="B619" t="s">
         <v>221</v>
       </c>
-      <c r="M616" t="s">
+      <c r="M619" t="s">
         <v>673</v>
-      </c>
-    </row>
-    <row r="618" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A618" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B618" t="s">
-        <v>1256</v>
-      </c>
-      <c r="M618" t="s">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="620" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A620" t="s">
-        <v>394</v>
-      </c>
-      <c r="B620" t="s">
-        <v>586</v>
-      </c>
-      <c r="M620" t="s">
-        <v>1573</v>
       </c>
     </row>
     <row r="621" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
-        <v>395</v>
+        <v>1255</v>
       </c>
       <c r="B621" t="s">
-        <v>587</v>
+        <v>1256</v>
       </c>
       <c r="M621" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="622" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A622" t="s">
-        <v>396</v>
-      </c>
-      <c r="B622" t="s">
-        <v>588</v>
-      </c>
-      <c r="M622" t="s">
-        <v>1575</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="623" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B623" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="M623" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="624" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
-        <v>1583</v>
+        <v>395</v>
       </c>
       <c r="B624" t="s">
-        <v>1584</v>
+        <v>587</v>
       </c>
       <c r="M624" t="s">
-        <v>1585</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="625" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>398</v>
-      </c>
-      <c r="B625" s="1" t="s">
-        <v>1570</v>
-      </c>
-      <c r="C625" s="1"/>
-      <c r="D625" s="1"/>
-      <c r="E625" s="1"/>
-      <c r="F625" s="1"/>
-      <c r="G625" s="1"/>
-      <c r="H625" s="1"/>
-      <c r="I625" s="1"/>
-      <c r="J625" s="1"/>
-      <c r="K625" s="1"/>
-      <c r="L625" s="1"/>
-      <c r="M625" s="1" t="s">
-        <v>1473</v>
+        <v>396</v>
+      </c>
+      <c r="B625" t="s">
+        <v>588</v>
+      </c>
+      <c r="M625" t="s">
+        <v>1575</v>
       </c>
     </row>
     <row r="626" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>1571</v>
-      </c>
-      <c r="B626" s="1" t="s">
-        <v>1578</v>
-      </c>
-      <c r="C626" s="1"/>
-      <c r="D626" s="1"/>
-      <c r="E626" s="1"/>
-      <c r="F626" s="1"/>
-      <c r="G626" s="1"/>
-      <c r="H626" s="1"/>
-      <c r="I626" s="1"/>
-      <c r="J626" s="1"/>
-      <c r="K626" s="1"/>
-      <c r="L626" s="1"/>
-      <c r="M626" s="1" t="s">
-        <v>1577</v>
+        <v>397</v>
+      </c>
+      <c r="B626" t="s">
+        <v>589</v>
+      </c>
+      <c r="M626" t="s">
+        <v>1576</v>
       </c>
     </row>
     <row r="627" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B627" s="1" t="s">
-        <v>1579</v>
-      </c>
-      <c r="C627" s="1"/>
-      <c r="D627" s="1"/>
-      <c r="E627" s="1"/>
-      <c r="F627" s="1"/>
-      <c r="G627" s="1"/>
-      <c r="H627" s="1"/>
-      <c r="I627" s="1"/>
-      <c r="J627" s="1"/>
-      <c r="K627" s="1"/>
-      <c r="L627" s="1"/>
-      <c r="M627" s="1" t="s">
-        <v>1577</v>
+        <v>1583</v>
+      </c>
+      <c r="B627" t="s">
+        <v>1584</v>
+      </c>
+      <c r="M627" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="628" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>398</v>
+      </c>
+      <c r="B628" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C628" s="1"/>
+      <c r="D628" s="1"/>
+      <c r="E628" s="1"/>
+      <c r="F628" s="1"/>
+      <c r="G628" s="1"/>
+      <c r="H628" s="1"/>
+      <c r="I628" s="1"/>
+      <c r="J628" s="1"/>
+      <c r="K628" s="1"/>
+      <c r="L628" s="1"/>
+      <c r="M628" s="1" t="s">
+        <v>1473</v>
       </c>
     </row>
     <row r="629" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>405</v>
-      </c>
-      <c r="B629" t="s">
-        <v>399</v>
-      </c>
-      <c r="M629" t="s">
-        <v>399</v>
+        <v>1571</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C629" s="1"/>
+      <c r="D629" s="1"/>
+      <c r="E629" s="1"/>
+      <c r="F629" s="1"/>
+      <c r="G629" s="1"/>
+      <c r="H629" s="1"/>
+      <c r="I629" s="1"/>
+      <c r="J629" s="1"/>
+      <c r="K629" s="1"/>
+      <c r="L629" s="1"/>
+      <c r="M629" s="1" t="s">
+        <v>1577</v>
       </c>
     </row>
     <row r="630" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>735</v>
-      </c>
-      <c r="B630" t="s">
-        <v>737</v>
-      </c>
-      <c r="M630" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="631" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A631" t="s">
-        <v>736</v>
-      </c>
-      <c r="B631" t="s">
-        <v>738</v>
-      </c>
-      <c r="M631" t="s">
-        <v>740</v>
+        <v>1572</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C630" s="1"/>
+      <c r="D630" s="1"/>
+      <c r="E630" s="1"/>
+      <c r="F630" s="1"/>
+      <c r="G630" s="1"/>
+      <c r="H630" s="1"/>
+      <c r="I630" s="1"/>
+      <c r="J630" s="1"/>
+      <c r="K630" s="1"/>
+      <c r="L630" s="1"/>
+      <c r="M630" s="1" t="s">
+        <v>1577</v>
       </c>
     </row>
     <row r="632" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B632" t="s">
-        <v>434</v>
+        <v>399</v>
       </c>
       <c r="M632" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="633" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A633" t="s">
-        <v>406</v>
+        <v>735</v>
       </c>
       <c r="B633" t="s">
-        <v>435</v>
+        <v>737</v>
       </c>
       <c r="M633" t="s">
-        <v>401</v>
+        <v>739</v>
       </c>
     </row>
     <row r="634" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>407</v>
+        <v>736</v>
       </c>
       <c r="B634" t="s">
-        <v>436</v>
+        <v>738</v>
       </c>
       <c r="M634" t="s">
-        <v>402</v>
+        <v>740</v>
       </c>
     </row>
     <row r="635" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B635" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="M635" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="636" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B636" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="M636" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="637" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>1061</v>
+        <v>407</v>
       </c>
       <c r="B637" t="s">
-        <v>1062</v>
+        <v>436</v>
       </c>
       <c r="M637" t="s">
-        <v>1064</v>
+        <v>402</v>
       </c>
     </row>
     <row r="638" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>1554</v>
+        <v>408</v>
       </c>
       <c r="B638" t="s">
-        <v>1555</v>
+        <v>437</v>
       </c>
       <c r="M638" t="s">
-        <v>1556</v>
+        <v>403</v>
       </c>
     </row>
     <row r="639" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>1733</v>
+        <v>409</v>
       </c>
       <c r="B639" t="s">
-        <v>1737</v>
+        <v>438</v>
       </c>
       <c r="M639" t="s">
-        <v>1745</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="640" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B640" t="s">
+        <v>1062</v>
+      </c>
+      <c r="M640" t="s">
+        <v>1064</v>
       </c>
     </row>
     <row r="641" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>819</v>
+        <v>1554</v>
       </c>
       <c r="B641" t="s">
-        <v>826</v>
+        <v>1555</v>
       </c>
       <c r="M641" t="s">
-        <v>833</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>820</v>
+        <v>1732</v>
       </c>
       <c r="B642" t="s">
-        <v>827</v>
+        <v>1736</v>
       </c>
       <c r="M642" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="643" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A643" t="s">
-        <v>821</v>
-      </c>
-      <c r="B643" t="s">
-        <v>828</v>
-      </c>
-      <c r="M643" t="s">
-        <v>835</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="644" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B644" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="M644" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="645" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A645" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="B645" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="M645" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="646" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B646" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="M646" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="647" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="B647" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="M647" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="648" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>1066</v>
+        <v>823</v>
       </c>
       <c r="B648" t="s">
-        <v>1063</v>
+        <v>830</v>
       </c>
       <c r="M648" t="s">
-        <v>1065</v>
+        <v>837</v>
       </c>
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>1558</v>
+        <v>824</v>
       </c>
       <c r="B649" t="s">
-        <v>1559</v>
+        <v>831</v>
       </c>
       <c r="M649" t="s">
-        <v>1557</v>
+        <v>838</v>
       </c>
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>1734</v>
+        <v>825</v>
       </c>
       <c r="B650" t="s">
-        <v>1735</v>
+        <v>832</v>
       </c>
       <c r="M650" t="s">
-        <v>1736</v>
+        <v>839</v>
+      </c>
+    </row>
+    <row r="651" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B651" t="s">
+        <v>1063</v>
+      </c>
+      <c r="M651" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>840</v>
+        <v>1558</v>
       </c>
       <c r="B652" t="s">
-        <v>1531</v>
+        <v>1559</v>
       </c>
       <c r="M652" t="s">
-        <v>1534</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>841</v>
+        <v>1733</v>
       </c>
       <c r="B653" t="s">
-        <v>1535</v>
+        <v>1734</v>
       </c>
       <c r="M653" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="654" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A654" t="s">
-        <v>1494</v>
-      </c>
-      <c r="B654" t="s">
-        <v>1536</v>
-      </c>
-      <c r="M654" t="s">
-        <v>1537</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="655" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1496</v>
+        <v>840</v>
       </c>
       <c r="B655" t="s">
-        <v>1497</v>
+        <v>1531</v>
       </c>
       <c r="M655" t="s">
-        <v>1500</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
+        <v>841</v>
+      </c>
+      <c r="B656" t="s">
+        <v>1535</v>
+      </c>
+      <c r="M656" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="657" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>1494</v>
+      </c>
+      <c r="B657" t="s">
+        <v>1536</v>
+      </c>
+      <c r="M657" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="658" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B658" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M658" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="659" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
         <v>1495</v>
       </c>
-      <c r="B656" t="s">
+      <c r="B659" t="s">
         <v>1498</v>
       </c>
-      <c r="M656" t="s">
+      <c r="M659" t="s">
         <v>1499</v>
-      </c>
-    </row>
-    <row r="660" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A660" t="s">
-        <v>411</v>
-      </c>
-      <c r="B660" t="s">
-        <v>439</v>
-      </c>
-      <c r="M660" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="661" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A661" t="s">
-        <v>412</v>
-      </c>
-      <c r="B661" t="s">
-        <v>415</v>
-      </c>
-      <c r="M661" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="662" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A662" t="s">
-        <v>413</v>
-      </c>
-      <c r="B662" t="s">
-        <v>414</v>
-      </c>
-      <c r="M662" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="663" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>845</v>
+        <v>411</v>
       </c>
       <c r="B663" t="s">
-        <v>846</v>
+        <v>439</v>
       </c>
       <c r="M663" t="s">
-        <v>847</v>
+        <v>733</v>
       </c>
     </row>
     <row r="664" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>848</v>
+        <v>412</v>
       </c>
       <c r="B664" t="s">
-        <v>849</v>
+        <v>415</v>
       </c>
       <c r="M664" t="s">
-        <v>850</v>
+        <v>432</v>
       </c>
     </row>
     <row r="665" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>851</v>
-      </c>
-      <c r="B665" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C665" s="3"/>
-      <c r="D665" s="3"/>
-      <c r="E665" s="3"/>
-      <c r="F665" s="3"/>
-      <c r="G665" s="3"/>
-      <c r="H665" s="3"/>
-      <c r="I665" s="3"/>
-      <c r="J665" s="3"/>
-      <c r="K665" s="3"/>
-      <c r="L665" s="3"/>
-      <c r="M665" s="2" t="s">
-        <v>853</v>
+        <v>413</v>
+      </c>
+      <c r="B665" t="s">
+        <v>414</v>
+      </c>
+      <c r="M665" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="666" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>963</v>
-      </c>
-      <c r="B666" s="2" t="s">
-        <v>964</v>
-      </c>
-      <c r="C666" s="3"/>
-      <c r="D666" s="3"/>
-      <c r="E666" s="3"/>
-      <c r="F666" s="3"/>
-      <c r="G666" s="3"/>
-      <c r="H666" s="3"/>
-      <c r="I666" s="3"/>
-      <c r="J666" s="3"/>
-      <c r="K666" s="3"/>
-      <c r="L666" s="3"/>
-      <c r="M666" s="2" t="s">
-        <v>965</v>
+        <v>845</v>
+      </c>
+      <c r="B666" t="s">
+        <v>846</v>
+      </c>
+      <c r="M666" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="667" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B667" s="2" t="s">
-        <v>1561</v>
-      </c>
-      <c r="C667" s="3"/>
-      <c r="D667" s="3"/>
-      <c r="E667" s="3"/>
-      <c r="F667" s="3"/>
-      <c r="G667" s="3"/>
-      <c r="H667" s="3"/>
-      <c r="I667" s="3"/>
-      <c r="J667" s="3"/>
-      <c r="K667" s="3"/>
-      <c r="L667" s="3"/>
-      <c r="M667" s="2" t="s">
-        <v>1296</v>
+        <v>848</v>
+      </c>
+      <c r="B667" t="s">
+        <v>849</v>
+      </c>
+      <c r="M667" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="668" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>1567</v>
+        <v>851</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>1568</v>
+        <v>852</v>
       </c>
       <c r="C668" s="3"/>
       <c r="D668" s="3"/>
@@ -11028,380 +11025,443 @@
       <c r="K668" s="3"/>
       <c r="L668" s="3"/>
       <c r="M668" s="2" t="s">
-        <v>1569</v>
+        <v>853</v>
       </c>
     </row>
     <row r="669" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B669" t="s">
-        <v>734</v>
-      </c>
-      <c r="M669" t="s">
-        <v>635</v>
+        <v>963</v>
+      </c>
+      <c r="B669" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="C669" s="3"/>
+      <c r="D669" s="3"/>
+      <c r="E669" s="3"/>
+      <c r="F669" s="3"/>
+      <c r="G669" s="3"/>
+      <c r="H669" s="3"/>
+      <c r="I669" s="3"/>
+      <c r="J669" s="3"/>
+      <c r="K669" s="3"/>
+      <c r="L669" s="3"/>
+      <c r="M669" s="2" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="670" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B670" s="2" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C670" s="3"/>
+      <c r="D670" s="3"/>
+      <c r="E670" s="3"/>
+      <c r="F670" s="3"/>
+      <c r="G670" s="3"/>
+      <c r="H670" s="3"/>
+      <c r="I670" s="3"/>
+      <c r="J670" s="3"/>
+      <c r="K670" s="3"/>
+      <c r="L670" s="3"/>
+      <c r="M670" s="2" t="s">
+        <v>1296</v>
       </c>
     </row>
     <row r="671" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1588</v>
+        <v>1567</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>1586</v>
-      </c>
+        <v>1568</v>
+      </c>
+      <c r="C671" s="3"/>
+      <c r="D671" s="3"/>
+      <c r="E671" s="3"/>
+      <c r="F671" s="3"/>
+      <c r="G671" s="3"/>
+      <c r="H671" s="3"/>
+      <c r="I671" s="3"/>
+      <c r="J671" s="3"/>
+      <c r="K671" s="3"/>
+      <c r="L671" s="3"/>
       <c r="M671" s="2" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="673" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A673" t="s">
-        <v>420</v>
-      </c>
-      <c r="B673" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="M673" s="4" t="s">
-        <v>416</v>
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="672" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B672" t="s">
+        <v>734</v>
+      </c>
+      <c r="M672" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="674" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>421</v>
-      </c>
-      <c r="B674" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="M674" s="4" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="675" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A675" t="s">
-        <v>422</v>
-      </c>
-      <c r="B675" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="M675" s="4" t="s">
-        <v>418</v>
+        <v>1588</v>
+      </c>
+      <c r="B674" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="M674" s="2" t="s">
+        <v>1587</v>
       </c>
     </row>
     <row r="676" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
+        <v>420</v>
+      </c>
+      <c r="B676" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="M676" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="677" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
+        <v>421</v>
+      </c>
+      <c r="B677" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="M677" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="678" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>422</v>
+      </c>
+      <c r="B678" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="M678" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="679" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
         <v>423</v>
       </c>
-      <c r="B676" s="4" t="s">
+      <c r="B679" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="M676" s="4" t="s">
+      <c r="M679" s="4" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="677" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A677" t="s">
+    <row r="680" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
         <v>1501</v>
       </c>
-      <c r="B677" s="4" t="s">
+      <c r="B680" s="4" t="s">
         <v>1502</v>
       </c>
-      <c r="M677" s="4" t="s">
+      <c r="M680" s="4" t="s">
         <v>1503</v>
-      </c>
-    </row>
-    <row r="680" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A680" t="s">
-        <v>594</v>
-      </c>
-      <c r="B680" t="s">
-        <v>425</v>
-      </c>
-      <c r="M680" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="681" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A681" t="s">
-        <v>595</v>
-      </c>
-      <c r="B681" t="s">
-        <v>426</v>
-      </c>
-      <c r="M681" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="682" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A682" t="s">
-        <v>596</v>
-      </c>
-      <c r="B682" t="s">
-        <v>427</v>
-      </c>
-      <c r="M682" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="683" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>1528</v>
+        <v>594</v>
       </c>
       <c r="B683" t="s">
-        <v>1530</v>
+        <v>425</v>
       </c>
       <c r="M683" t="s">
-        <v>1529</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="684" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>595</v>
+      </c>
+      <c r="B684" t="s">
+        <v>426</v>
+      </c>
+      <c r="M684" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="685" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>621</v>
+        <v>596</v>
       </c>
       <c r="B685" t="s">
-        <v>633</v>
+        <v>427</v>
       </c>
       <c r="M685" t="s">
-        <v>634</v>
+        <v>430</v>
       </c>
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>622</v>
+        <v>1528</v>
       </c>
       <c r="B686" t="s">
-        <v>624</v>
+        <v>1530</v>
       </c>
       <c r="M686" t="s">
-        <v>631</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="688" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="B688" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="M688" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="690" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A690" t="s">
-        <v>742</v>
-      </c>
-      <c r="B690" t="s">
-        <v>743</v>
-      </c>
-      <c r="M690" t="s">
-        <v>745</v>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="689" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>622</v>
+      </c>
+      <c r="B689" t="s">
+        <v>624</v>
+      </c>
+      <c r="M689" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="691" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>862</v>
+        <v>637</v>
       </c>
       <c r="B691" t="s">
-        <v>863</v>
+        <v>638</v>
       </c>
       <c r="M691" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="692" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A692" t="s">
-        <v>746</v>
-      </c>
-      <c r="B692" t="s">
-        <v>744</v>
-      </c>
-      <c r="M692" t="s">
-        <v>748</v>
+        <v>639</v>
       </c>
     </row>
     <row r="693" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="B693" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="M693" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
     </row>
     <row r="694" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>751</v>
+        <v>862</v>
       </c>
       <c r="B694" t="s">
-        <v>747</v>
+        <v>863</v>
       </c>
       <c r="M694" t="s">
-        <v>747</v>
+        <v>864</v>
       </c>
     </row>
     <row r="695" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1590</v>
+        <v>746</v>
       </c>
       <c r="B695" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="M695" t="s">
-        <v>1591</v>
+        <v>748</v>
       </c>
     </row>
     <row r="696" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>1744</v>
+        <v>749</v>
       </c>
       <c r="B696" t="s">
-        <v>863</v>
+        <v>744</v>
       </c>
       <c r="M696" t="s">
-        <v>863</v>
+        <v>750</v>
       </c>
     </row>
     <row r="697" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>1641</v>
+        <v>751</v>
       </c>
       <c r="B697" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="M697" t="s">
-        <v>1642</v>
+        <v>747</v>
       </c>
     </row>
     <row r="698" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1609</v>
+        <v>1590</v>
       </c>
       <c r="B698" t="s">
-        <v>1610</v>
+        <v>747</v>
       </c>
       <c r="M698" t="s">
-        <v>1611</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="699" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1686</v>
+        <v>1743</v>
       </c>
       <c r="B699" t="s">
-        <v>744</v>
+        <v>863</v>
       </c>
       <c r="M699" t="s">
-        <v>1687</v>
+        <v>863</v>
       </c>
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B700" t="s">
+        <v>744</v>
+      </c>
+      <c r="M700" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="701" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B701" t="s">
+        <v>1610</v>
+      </c>
+      <c r="M701" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="702" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B702" t="s">
+        <v>744</v>
+      </c>
+      <c r="M702" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="703" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
         <v>1691</v>
       </c>
-      <c r="B700" s="5" t="s">
+      <c r="B703" s="5" t="s">
         <v>1692</v>
       </c>
-      <c r="M700" t="s">
+      <c r="M703" t="s">
         <v>1692</v>
       </c>
     </row>
-    <row r="702" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A702" t="s">
+    <row r="705" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
         <v>755</v>
       </c>
-      <c r="B702" s="4" t="s">
+      <c r="B705" s="4" t="s">
         <v>1436</v>
       </c>
-      <c r="M702" s="4" t="s">
+      <c r="M705" s="4" t="s">
         <v>1437</v>
       </c>
     </row>
-    <row r="703" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A703" t="s">
+    <row r="706" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A706" t="s">
         <v>756</v>
       </c>
-      <c r="B703" s="4" t="s">
+      <c r="B706" s="4" t="s">
         <v>1438</v>
       </c>
-      <c r="M703" s="4" t="s">
+      <c r="M706" s="4" t="s">
         <v>1439</v>
       </c>
     </row>
-    <row r="704" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
+    <row r="707" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
         <v>757</v>
       </c>
-      <c r="B704" t="s">
+      <c r="B707" t="s">
         <v>759</v>
       </c>
-      <c r="M704" t="s">
+      <c r="M707" t="s">
         <v>758</v>
-      </c>
-    </row>
-    <row r="706" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A706" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B706" s="4" t="s">
-        <v>1440</v>
-      </c>
-      <c r="M706" s="4" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="707" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A707" t="s">
-        <v>1076</v>
-      </c>
-      <c r="B707" s="4" t="s">
-        <v>1442</v>
-      </c>
-      <c r="M707" s="4" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="708" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
-        <v>1077</v>
-      </c>
-      <c r="B708" s="4" t="s">
-        <v>1444</v>
-      </c>
-      <c r="M708" s="4" t="s">
-        <v>1445</v>
       </c>
     </row>
     <row r="709" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
       <c r="B709" s="4" t="s">
-        <v>1446</v>
-      </c>
-      <c r="M709" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="710" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>1440</v>
+      </c>
+      <c r="M709" s="4" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="710" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="B710" s="4" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
       <c r="M710" s="4" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="711" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B711" s="4" t="s">
+        <v>1444</v>
+      </c>
+      <c r="M711" s="4" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="712" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="M712" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="713" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B713" s="4" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M713" s="4" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="714" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
         <v>1080</v>
       </c>
-      <c r="B711" s="4" t="s">
+      <c r="B714" s="4" t="s">
         <v>1449</v>
       </c>
-      <c r="M711" s="4" t="s">
+      <c r="M714" s="4" t="s">
         <v>1445</v>
       </c>
     </row>

</xml_diff>

<commit_message>
only run the lovers ondeath function on actual lovers
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF85839-7DB9-416E-A72B-3D729521165A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E2D459-617D-49D8-BFAE-67730DB9DD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1590" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7245" yWindow="3390" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -2758,9 +2758,6 @@
     <t>shifterFullDesc</t>
   </si>
   <si>
-    <t>swapperFullDesc</t>
-  </si>
-  <si>
     <t>seerFullDesc</t>
   </si>
   <si>
@@ -5629,9 +5626,6 @@
     <t>Immunity Time After Meeting</t>
   </si>
   <si>
-    <t>会議後、感染しない時間</t>
-  </si>
-  <si>
     <t>plagueDoctorNumInfections</t>
   </si>
   <si>
@@ -5684,6 +5678,12 @@
   </si>
   <si>
     <t>死亡後でも勝利できる</t>
+  </si>
+  <si>
+    <t>会議後、感染されない期間</t>
+  </si>
+  <si>
+    <t>niceSwapperFullDesc</t>
   </si>
 </sst>
 </file>
@@ -6010,8 +6010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q714"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B536" workbookViewId="0">
-      <selection activeCell="M556" sqref="M556"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="A354" sqref="A354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6073,13 +6073,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B2" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="M2" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6156,7 +6156,7 @@
         <v>446</v>
       </c>
       <c r="M10" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -6167,7 +6167,7 @@
         <v>447</v>
       </c>
       <c r="M11" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6178,7 +6178,7 @@
         <v>448</v>
       </c>
       <c r="M12" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6189,7 +6189,7 @@
         <v>449</v>
       </c>
       <c r="M13" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6200,7 +6200,7 @@
         <v>450</v>
       </c>
       <c r="M14" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -6211,18 +6211,18 @@
         <v>451</v>
       </c>
       <c r="M15" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B17" t="s">
         <v>1360</v>
       </c>
-      <c r="B17" t="s">
-        <v>1361</v>
-      </c>
       <c r="M17" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -6337,7 +6337,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B34" t="s">
         <v>452</v>
@@ -6365,7 +6365,7 @@
         <v>523</v>
       </c>
       <c r="M37" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -6508,7 +6508,7 @@
         <v>455</v>
       </c>
       <c r="M56" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -6519,7 +6519,7 @@
         <v>456</v>
       </c>
       <c r="M60" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -6563,18 +6563,18 @@
         <v>457</v>
       </c>
       <c r="M65" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>960</v>
+      </c>
+      <c r="B66" t="s">
+        <v>967</v>
+      </c>
+      <c r="M66" t="s">
         <v>961</v>
-      </c>
-      <c r="B66" t="s">
-        <v>968</v>
-      </c>
-      <c r="M66" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -6662,7 +6662,7 @@
         <v>532</v>
       </c>
       <c r="M81" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -6673,7 +6673,7 @@
         <v>573</v>
       </c>
       <c r="M82" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -6689,13 +6689,13 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B85" t="s">
         <v>1095</v>
       </c>
-      <c r="B85" t="s">
-        <v>1096</v>
-      </c>
       <c r="M85" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -6772,18 +6772,18 @@
         <v>688</v>
       </c>
       <c r="M96" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B98" t="s">
         <v>1699</v>
       </c>
-      <c r="B98" t="s">
+      <c r="M98" t="s">
         <v>1700</v>
-      </c>
-      <c r="M98" t="s">
-        <v>1701</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -6805,7 +6805,7 @@
         <v>534</v>
       </c>
       <c r="M103" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -6975,7 +6975,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B131" t="s">
         <v>469</v>
@@ -7052,10 +7052,10 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B141" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="M141" t="s">
         <v>657</v>
@@ -7066,7 +7066,7 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="M142" t="s">
         <v>157</v>
@@ -7074,7 +7074,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B146" t="s">
         <v>470</v>
@@ -7085,7 +7085,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B147" t="s">
         <v>566</v>
@@ -7096,7 +7096,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B148" t="s">
         <v>566</v>
@@ -7128,18 +7128,18 @@
         <v>690</v>
       </c>
       <c r="M151" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B152" t="s">
         <v>1606</v>
       </c>
-      <c r="B152" t="s">
+      <c r="M152" t="s">
         <v>1607</v>
-      </c>
-      <c r="M152" t="s">
-        <v>1608</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -7161,7 +7161,7 @@
         <v>691</v>
       </c>
       <c r="M154" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -7199,7 +7199,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B161" t="s">
         <v>472</v>
@@ -7210,7 +7210,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="B163" t="s">
         <v>556</v>
@@ -7221,7 +7221,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B164" t="s">
         <v>557</v>
@@ -7232,7 +7232,7 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B165" t="s">
         <v>557</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B167" t="s">
         <v>558</v>
@@ -7254,7 +7254,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B168" t="s">
         <v>557</v>
@@ -7265,7 +7265,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B169" t="s">
         <v>557</v>
@@ -7279,7 +7279,7 @@
         <v>23</v>
       </c>
       <c r="B171" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="M171" t="s">
         <v>657</v>
@@ -7298,87 +7298,87 @@
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>965</v>
+      </c>
+      <c r="B173" t="s">
         <v>966</v>
       </c>
-      <c r="B173" t="s">
-        <v>967</v>
-      </c>
       <c r="M173" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B174" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="M174" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B175" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="M175" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B176" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="M176" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B177" t="s">
+        <v>1631</v>
+      </c>
+      <c r="M177" t="s">
         <v>1632</v>
-      </c>
-      <c r="M177" t="s">
-        <v>1633</v>
       </c>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B178" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="M178" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B180" t="s">
         <v>1402</v>
       </c>
-      <c r="B180" t="s">
+      <c r="M180" t="s">
         <v>1403</v>
-      </c>
-      <c r="M180" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B181" t="s">
         <v>1646</v>
-      </c>
-      <c r="B181" t="s">
-        <v>1647</v>
       </c>
       <c r="M181" t="s">
         <v>632</v>
@@ -7617,13 +7617,13 @@
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B216" t="s">
         <v>1046</v>
       </c>
-      <c r="B216" t="s">
-        <v>1047</v>
-      </c>
       <c r="M216" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.25">
@@ -7711,7 +7711,7 @@
         <v>540</v>
       </c>
       <c r="M228" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.25">
@@ -7722,12 +7722,12 @@
         <v>540</v>
       </c>
       <c r="M229" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B231" t="s">
         <v>480</v>
@@ -7738,68 +7738,68 @@
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B232" t="s">
         <v>540</v>
       </c>
       <c r="M232" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B233" t="s">
         <v>540</v>
       </c>
       <c r="M233" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B235" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="M235" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B236" t="s">
+        <v>1618</v>
+      </c>
+      <c r="M236" t="s">
         <v>1619</v>
-      </c>
-      <c r="M236" t="s">
-        <v>1620</v>
       </c>
     </row>
     <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B237" t="s">
+        <v>1618</v>
+      </c>
+      <c r="M237" t="s">
         <v>1619</v>
-      </c>
-      <c r="M237" t="s">
-        <v>1620</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="B239" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="M239" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.25">
@@ -7815,46 +7815,46 @@
     </row>
     <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B241" t="s">
+        <v>1648</v>
+      </c>
+      <c r="M241" t="s">
         <v>1649</v>
-      </c>
-      <c r="M241" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B242" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="M242" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B243" t="s">
+        <v>1716</v>
+      </c>
+      <c r="M243" t="s">
         <v>1717</v>
-      </c>
-      <c r="M243" t="s">
-        <v>1718</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
+        <v>1710</v>
+      </c>
+      <c r="B245" t="s">
         <v>1711</v>
       </c>
-      <c r="B245" t="s">
+      <c r="M245" t="s">
         <v>1712</v>
-      </c>
-      <c r="M245" t="s">
-        <v>1713</v>
       </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.25">
@@ -7873,10 +7873,10 @@
         <v>227</v>
       </c>
       <c r="B250" t="s">
+        <v>1341</v>
+      </c>
+      <c r="M250" t="s">
         <v>1342</v>
-      </c>
-      <c r="M250" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="251" spans="1:13" x14ac:dyDescent="0.25">
@@ -7884,21 +7884,21 @@
         <v>228</v>
       </c>
       <c r="B251" t="s">
+        <v>1341</v>
+      </c>
+      <c r="M251" t="s">
         <v>1342</v>
-      </c>
-      <c r="M251" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B253" t="s">
         <v>1348</v>
       </c>
-      <c r="B253" t="s">
+      <c r="M253" t="s">
         <v>1349</v>
-      </c>
-      <c r="M253" t="s">
-        <v>1350</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.25">
@@ -7936,35 +7936,35 @@
     </row>
     <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="B261" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="M261" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B262" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="M262" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B263" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="M263" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.25">
@@ -8129,7 +8129,7 @@
         <v>723</v>
       </c>
       <c r="M287" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.25">
@@ -8277,10 +8277,10 @@
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B306" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="M306" t="s">
         <v>652</v>
@@ -8288,10 +8288,10 @@
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B307" t="s">
         <v>1413</v>
-      </c>
-      <c r="B307" t="s">
-        <v>1414</v>
       </c>
       <c r="M307" t="s">
         <v>653</v>
@@ -8360,7 +8360,7 @@
         <v>725</v>
       </c>
       <c r="M317" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="321" spans="1:13" x14ac:dyDescent="0.25">
@@ -8448,7 +8448,7 @@
         <v>493</v>
       </c>
       <c r="M329" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="330" spans="1:13" x14ac:dyDescent="0.25">
@@ -8464,13 +8464,13 @@
     </row>
     <row r="331" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B331" t="s">
+        <v>1376</v>
+      </c>
+      <c r="M331" t="s">
         <v>1378</v>
-      </c>
-      <c r="B331" t="s">
-        <v>1377</v>
-      </c>
-      <c r="M331" t="s">
-        <v>1379</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.25">
@@ -8497,18 +8497,18 @@
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B339" t="s">
         <v>1593</v>
       </c>
-      <c r="B339" t="s">
-        <v>1594</v>
-      </c>
       <c r="M339" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B340" t="s">
         <v>541</v>
@@ -8519,7 +8519,7 @@
     </row>
     <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B341" t="s">
         <v>580</v>
@@ -8530,29 +8530,29 @@
     </row>
     <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B343" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="M343" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B344" t="s">
         <v>1598</v>
       </c>
-      <c r="B344" t="s">
+      <c r="M344" t="s">
         <v>1599</v>
-      </c>
-      <c r="M344" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B345" t="s">
         <v>580</v>
@@ -8563,10 +8563,10 @@
     </row>
     <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B347" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="M347" t="s">
         <v>657</v>
@@ -8596,24 +8596,24 @@
     </row>
     <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B350" t="s">
         <v>1602</v>
       </c>
-      <c r="B350" t="s">
-        <v>1603</v>
-      </c>
       <c r="M350" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B352" t="s">
         <v>1622</v>
       </c>
-      <c r="B352" t="s">
-        <v>1623</v>
-      </c>
       <c r="M352" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="356" spans="1:13" x14ac:dyDescent="0.25">
@@ -8782,7 +8782,7 @@
         <v>727</v>
       </c>
       <c r="M374" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.25">
@@ -8793,40 +8793,40 @@
         <v>710</v>
       </c>
       <c r="M375" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="376" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B376" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="M376" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B377" t="s">
+        <v>1637</v>
+      </c>
+      <c r="M377" t="s">
         <v>1638</v>
-      </c>
-      <c r="M377" t="s">
-        <v>1639</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B379" t="s">
         <v>1643</v>
       </c>
-      <c r="B379" t="s">
+      <c r="M379" t="s">
         <v>1644</v>
-      </c>
-      <c r="M379" t="s">
-        <v>1645</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.25">
@@ -8886,35 +8886,35 @@
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B389" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="M389" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B390" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="M390" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B391" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="M391" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.25">
@@ -9068,7 +9068,7 @@
         <v>507</v>
       </c>
       <c r="M416" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.25">
@@ -9101,7 +9101,7 @@
         <v>677</v>
       </c>
       <c r="M420" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="421" spans="1:13" x14ac:dyDescent="0.25">
@@ -9139,13 +9139,13 @@
     </row>
     <row r="425" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B425" t="s">
         <v>1507</v>
       </c>
-      <c r="B425" t="s">
+      <c r="M425" t="s">
         <v>1508</v>
-      </c>
-      <c r="M425" t="s">
-        <v>1509</v>
       </c>
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.25">
@@ -9205,13 +9205,13 @@
     </row>
     <row r="435" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B435" t="s">
+        <v>1579</v>
+      </c>
+      <c r="M435" t="s">
         <v>1581</v>
-      </c>
-      <c r="B435" t="s">
-        <v>1580</v>
-      </c>
-      <c r="M435" t="s">
-        <v>1582</v>
       </c>
     </row>
     <row r="440" spans="1:13" x14ac:dyDescent="0.25">
@@ -9304,13 +9304,13 @@
     </row>
     <row r="449" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B449" t="s">
         <v>1345</v>
       </c>
-      <c r="B449" t="s">
+      <c r="M449" t="s">
         <v>1346</v>
-      </c>
-      <c r="M449" t="s">
-        <v>1347</v>
       </c>
     </row>
     <row r="453" spans="1:13" x14ac:dyDescent="0.25">
@@ -9326,7 +9326,7 @@
     </row>
     <row r="454" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B454" t="s">
         <v>818</v>
@@ -9337,7 +9337,7 @@
     </row>
     <row r="455" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B455" t="s">
         <v>818</v>
@@ -9348,62 +9348,62 @@
     </row>
     <row r="459" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B459" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="M459" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="460" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B460" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="M460" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="461" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B461" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="M461" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="463" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B463" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="M463" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="464" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B464" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="M464" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="465" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B465" t="s">
         <v>700</v>
@@ -9414,320 +9414,320 @@
     </row>
     <row r="466" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B466" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="M466" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="468" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B468" t="s">
         <v>882</v>
       </c>
       <c r="M468" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="472" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B472" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="M472" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="473" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B473" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="M473" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="474" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B474" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="M474" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="476" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B476" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="M476" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="477" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B477" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="M477" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="478" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B478" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="M478" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="480" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B480" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="M480" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="481" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B481" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="M481" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="482" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B482" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="M482" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="483" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B483" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="M483" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="487" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B487" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="M487" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="488" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B488" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="M488" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="489" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B489" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="M489" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="490" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B490" s="4" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="M490" s="4" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="491" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
+        <v>1543</v>
+      </c>
+      <c r="M491" s="4" t="s">
         <v>1544</v>
-      </c>
-      <c r="M491" s="4" t="s">
-        <v>1545</v>
       </c>
     </row>
     <row r="493" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B493" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="M493" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="494" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B494" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="M494" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="495" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B495" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="M495" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="496" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B496" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="M496" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="497" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B497" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="M497" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="501" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B501" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="M501" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="502" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B502" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="M502" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="503" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B503" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="M503" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="504" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B504" s="4" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="M504" s="4" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="505" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="507" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B507" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="M507" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="508" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B508" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="M508" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="510" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B510" t="s">
         <v>1510</v>
-      </c>
-      <c r="B510" t="s">
-        <v>1511</v>
       </c>
       <c r="M510" t="s">
         <v>632</v>
@@ -9735,164 +9735,164 @@
     </row>
     <row r="514" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B514" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="M514" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="515" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B515" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="M515" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="516" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B516" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="M516" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="517" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="B517" s="4" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="M517" s="4" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="518" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="M518" s="4" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="520" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B520" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="M520" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="521" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="B521" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="M521" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="522" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B522" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="M522" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="523" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="B523" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="M523" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="524" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B524" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="M524" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="525" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B525" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="M525" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="529" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B529" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="M529" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="530" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B530" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="M530" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="531" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B531" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="M531" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="532" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="M532" s="4" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="533" spans="1:13" x14ac:dyDescent="0.25">
@@ -9901,62 +9901,62 @@
     </row>
     <row r="534" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="B534" s="4" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="M534" s="4" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="535" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="B535" s="4" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="M535" s="4" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="536" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="B536" s="4" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="M536" s="4" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="537" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B537" s="4" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="M537" s="4" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="538" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B538" s="4" t="s">
         <v>1694</v>
       </c>
-      <c r="B538" s="4" t="s">
-        <v>1695</v>
-      </c>
       <c r="M538" s="4" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="539" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B539" t="s">
         <v>700</v>
@@ -9967,189 +9967,189 @@
     </row>
     <row r="540" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B540" s="4" t="s">
         <v>1704</v>
       </c>
-      <c r="B540" s="4" t="s">
+      <c r="M540" s="4" t="s">
         <v>1705</v>
-      </c>
-      <c r="M540" s="4" t="s">
-        <v>1706</v>
       </c>
     </row>
     <row r="544" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B544" t="s">
         <v>1720</v>
       </c>
-      <c r="B544" t="s">
+      <c r="M544" t="s">
         <v>1721</v>
-      </c>
-      <c r="M544" t="s">
-        <v>1722</v>
       </c>
     </row>
     <row r="545" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B545" t="s">
+        <v>1724</v>
+      </c>
+      <c r="M545" t="s">
         <v>1725</v>
-      </c>
-      <c r="M545" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="546" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B546" t="s">
         <v>1724</v>
       </c>
-      <c r="B546" t="s">
+      <c r="M546" t="s">
         <v>1725</v>
-      </c>
-      <c r="M546" t="s">
-        <v>1726</v>
       </c>
     </row>
     <row r="548" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1754</v>
+      </c>
+      <c r="M548" t="s">
         <v>1755</v>
-      </c>
-      <c r="B548" t="s">
-        <v>1756</v>
-      </c>
-      <c r="M548" t="s">
-        <v>1757</v>
       </c>
     </row>
     <row r="549" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="B549" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="M549" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="550" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B550" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="M550" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="551" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1729</v>
+      </c>
+      <c r="M551" t="s">
         <v>1728</v>
-      </c>
-      <c r="B551" t="s">
-        <v>1730</v>
-      </c>
-      <c r="M551" t="s">
-        <v>1729</v>
       </c>
     </row>
     <row r="552" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B552" t="s">
         <v>1747</v>
       </c>
-      <c r="B552" t="s">
-        <v>1748</v>
-      </c>
       <c r="M552" t="s">
-        <v>1749</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="553" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B553" t="s">
         <v>1758</v>
       </c>
-      <c r="B553" t="s">
-        <v>1760</v>
-      </c>
       <c r="M553" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="554" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="B554" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="M554" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="555" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1764</v>
+      </c>
+      <c r="M555" t="s">
         <v>1765</v>
-      </c>
-      <c r="B555" t="s">
-        <v>1766</v>
-      </c>
-      <c r="M555" t="s">
-        <v>1767</v>
       </c>
     </row>
     <row r="557" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B557" t="s">
         <v>1739</v>
       </c>
-      <c r="B557" t="s">
-        <v>1740</v>
-      </c>
       <c r="M557" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="558" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B558" t="s">
         <v>1737</v>
       </c>
-      <c r="B558" t="s">
-        <v>1738</v>
-      </c>
       <c r="M558" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="560" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B560" t="s">
         <v>1745</v>
       </c>
-      <c r="B560" t="s">
-        <v>1746</v>
-      </c>
       <c r="M560" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="561" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="B561" t="s">
         <v>882</v>
       </c>
       <c r="M561" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="565" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B565" t="s">
         <v>1244</v>
       </c>
-      <c r="B565" t="s">
+      <c r="M565" t="s">
         <v>1245</v>
-      </c>
-      <c r="M565" t="s">
-        <v>1246</v>
       </c>
     </row>
     <row r="569" spans="1:13" x14ac:dyDescent="0.25">
@@ -10220,35 +10220,35 @@
     </row>
     <row r="581" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B581" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="M581" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="582" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="B582" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="M582" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B583" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="M583" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="585" spans="1:13" x14ac:dyDescent="0.25">
@@ -10256,7 +10256,7 @@
         <v>100</v>
       </c>
       <c r="B585" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M585" t="s">
         <v>674</v>
@@ -10267,7 +10267,7 @@
         <v>101</v>
       </c>
       <c r="B586" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="M586" t="s">
         <v>675</v>
@@ -10297,24 +10297,24 @@
     </row>
     <row r="589" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
+        <v>969</v>
+      </c>
+      <c r="B589" t="s">
+        <v>971</v>
+      </c>
+      <c r="M589" t="s">
         <v>970</v>
-      </c>
-      <c r="B589" t="s">
-        <v>972</v>
-      </c>
-      <c r="M589" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="590" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B590" t="s">
         <v>1397</v>
       </c>
-      <c r="B590" t="s">
+      <c r="M590" t="s">
         <v>1398</v>
-      </c>
-      <c r="M590" t="s">
-        <v>1399</v>
       </c>
     </row>
     <row r="592" spans="1:13" x14ac:dyDescent="0.25">
@@ -10407,35 +10407,35 @@
     </row>
     <row r="602" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B602" t="s">
         <v>1097</v>
       </c>
-      <c r="B602" t="s">
+      <c r="M602" t="s">
         <v>1098</v>
-      </c>
-      <c r="M602" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="603" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B603" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="M603" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="604" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B604" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="M604" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="605" spans="1:13" x14ac:dyDescent="0.25">
@@ -10451,24 +10451,24 @@
     </row>
     <row r="606" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B606" t="s">
         <v>1525</v>
       </c>
-      <c r="B606" t="s">
+      <c r="M606" t="s">
         <v>1526</v>
-      </c>
-      <c r="M606" t="s">
-        <v>1527</v>
       </c>
     </row>
     <row r="608" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B608" t="s">
         <v>1688</v>
       </c>
-      <c r="B608" t="s">
+      <c r="M608" t="s">
         <v>1689</v>
-      </c>
-      <c r="M608" t="s">
-        <v>1690</v>
       </c>
     </row>
     <row r="612" spans="1:13" x14ac:dyDescent="0.25">
@@ -10501,7 +10501,7 @@
         <v>516</v>
       </c>
       <c r="M615" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="616" spans="1:13" x14ac:dyDescent="0.25">
@@ -10512,7 +10512,7 @@
         <v>517</v>
       </c>
       <c r="M616" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="617" spans="1:13" x14ac:dyDescent="0.25">
@@ -10523,7 +10523,7 @@
         <v>518</v>
       </c>
       <c r="M617" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="619" spans="1:13" x14ac:dyDescent="0.25">
@@ -10539,13 +10539,13 @@
     </row>
     <row r="621" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B621" t="s">
         <v>1255</v>
       </c>
-      <c r="B621" t="s">
+      <c r="M621" t="s">
         <v>1256</v>
-      </c>
-      <c r="M621" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="623" spans="1:13" x14ac:dyDescent="0.25">
@@ -10556,7 +10556,7 @@
         <v>586</v>
       </c>
       <c r="M623" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="624" spans="1:13" x14ac:dyDescent="0.25">
@@ -10567,7 +10567,7 @@
         <v>587</v>
       </c>
       <c r="M624" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="625" spans="1:13" x14ac:dyDescent="0.25">
@@ -10578,7 +10578,7 @@
         <v>588</v>
       </c>
       <c r="M625" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="626" spans="1:13" x14ac:dyDescent="0.25">
@@ -10589,18 +10589,18 @@
         <v>589</v>
       </c>
       <c r="M626" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="627" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B627" t="s">
         <v>1583</v>
       </c>
-      <c r="B627" t="s">
+      <c r="M627" t="s">
         <v>1584</v>
-      </c>
-      <c r="M627" t="s">
-        <v>1585</v>
       </c>
     </row>
     <row r="628" spans="1:13" x14ac:dyDescent="0.25">
@@ -10608,7 +10608,7 @@
         <v>398</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="C628" s="1"/>
       <c r="D628" s="1"/>
@@ -10621,15 +10621,15 @@
       <c r="K628" s="1"/>
       <c r="L628" s="1"/>
       <c r="M628" s="1" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="629" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C629" s="1"/>
       <c r="D629" s="1"/>
@@ -10642,15 +10642,15 @@
       <c r="K629" s="1"/>
       <c r="L629" s="1"/>
       <c r="M629" s="1" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="630" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C630" s="1"/>
       <c r="D630" s="1"/>
@@ -10663,7 +10663,7 @@
       <c r="K630" s="1"/>
       <c r="L630" s="1"/>
       <c r="M630" s="1" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="632" spans="1:13" x14ac:dyDescent="0.25">
@@ -10756,35 +10756,35 @@
     </row>
     <row r="640" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B640" t="s">
         <v>1061</v>
       </c>
-      <c r="B640" t="s">
-        <v>1062</v>
-      </c>
       <c r="M640" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="641" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B641" t="s">
         <v>1554</v>
       </c>
-      <c r="B641" t="s">
+      <c r="M641" t="s">
         <v>1555</v>
-      </c>
-      <c r="M641" t="s">
-        <v>1556</v>
       </c>
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B642" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="M642" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="644" spans="1:13" x14ac:dyDescent="0.25">
@@ -10866,35 +10866,35 @@
     </row>
     <row r="651" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B651" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="M651" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B652" t="s">
         <v>1558</v>
       </c>
-      <c r="B652" t="s">
-        <v>1559</v>
-      </c>
       <c r="M652" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B653" t="s">
         <v>1733</v>
       </c>
-      <c r="B653" t="s">
+      <c r="M653" t="s">
         <v>1734</v>
-      </c>
-      <c r="M653" t="s">
-        <v>1735</v>
       </c>
     </row>
     <row r="655" spans="1:13" x14ac:dyDescent="0.25">
@@ -10902,10 +10902,10 @@
         <v>840</v>
       </c>
       <c r="B655" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="M655" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.25">
@@ -10913,43 +10913,43 @@
         <v>841</v>
       </c>
       <c r="B656" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="M656" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="657" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B657" t="s">
+        <v>1535</v>
+      </c>
+      <c r="M657" t="s">
         <v>1536</v>
-      </c>
-      <c r="M657" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="658" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B658" t="s">
         <v>1496</v>
       </c>
-      <c r="B658" t="s">
-        <v>1497</v>
-      </c>
       <c r="M658" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="659" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B659" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M659" t="s">
         <v>1498</v>
-      </c>
-      <c r="M659" t="s">
-        <v>1499</v>
       </c>
     </row>
     <row r="663" spans="1:13" x14ac:dyDescent="0.25">
@@ -11030,10 +11030,10 @@
     </row>
     <row r="669" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
+        <v>962</v>
+      </c>
+      <c r="B669" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B669" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C669" s="3"/>
       <c r="D669" s="3"/>
@@ -11046,15 +11046,15 @@
       <c r="K669" s="3"/>
       <c r="L669" s="3"/>
       <c r="M669" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="670" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B670" s="2" t="s">
         <v>1560</v>
-      </c>
-      <c r="B670" s="2" t="s">
-        <v>1561</v>
       </c>
       <c r="C670" s="3"/>
       <c r="D670" s="3"/>
@@ -11067,15 +11067,15 @@
       <c r="K670" s="3"/>
       <c r="L670" s="3"/>
       <c r="M670" s="2" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="671" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B671" s="2" t="s">
         <v>1567</v>
-      </c>
-      <c r="B671" s="2" t="s">
-        <v>1568</v>
       </c>
       <c r="C671" s="3"/>
       <c r="D671" s="3"/>
@@ -11088,12 +11088,12 @@
       <c r="K671" s="3"/>
       <c r="L671" s="3"/>
       <c r="M671" s="2" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="672" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B672" t="s">
         <v>734</v>
@@ -11104,13 +11104,13 @@
     </row>
     <row r="674" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B674" s="2" t="s">
+        <v>1585</v>
+      </c>
+      <c r="M674" s="2" t="s">
         <v>1586</v>
-      </c>
-      <c r="M674" s="2" t="s">
-        <v>1587</v>
       </c>
     </row>
     <row r="676" spans="1:13" x14ac:dyDescent="0.25">
@@ -11159,13 +11159,13 @@
     </row>
     <row r="680" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B680" s="4" t="s">
         <v>1501</v>
       </c>
-      <c r="B680" s="4" t="s">
+      <c r="M680" s="4" t="s">
         <v>1502</v>
-      </c>
-      <c r="M680" s="4" t="s">
-        <v>1503</v>
       </c>
     </row>
     <row r="683" spans="1:13" x14ac:dyDescent="0.25">
@@ -11203,13 +11203,13 @@
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1529</v>
+      </c>
+      <c r="M686" t="s">
         <v>1528</v>
-      </c>
-      <c r="B686" t="s">
-        <v>1530</v>
-      </c>
-      <c r="M686" t="s">
-        <v>1529</v>
       </c>
     </row>
     <row r="688" spans="1:13" x14ac:dyDescent="0.25">
@@ -11302,18 +11302,18 @@
     </row>
     <row r="698" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B698" t="s">
         <v>747</v>
       </c>
       <c r="M698" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="699" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B699" t="s">
         <v>863</v>
@@ -11324,46 +11324,46 @@
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B700" t="s">
         <v>744</v>
       </c>
       <c r="M700" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="701" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B701" t="s">
         <v>1609</v>
       </c>
-      <c r="B701" t="s">
+      <c r="M701" t="s">
         <v>1610</v>
-      </c>
-      <c r="M701" t="s">
-        <v>1611</v>
       </c>
     </row>
     <row r="702" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B702" t="s">
         <v>744</v>
       </c>
       <c r="M702" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="703" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B703" s="5" t="s">
         <v>1691</v>
       </c>
-      <c r="B703" s="5" t="s">
-        <v>1692</v>
-      </c>
       <c r="M703" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="705" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -11371,10 +11371,10 @@
         <v>755</v>
       </c>
       <c r="B705" s="4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="M705" s="4" t="s">
         <v>1436</v>
-      </c>
-      <c r="M705" s="4" t="s">
-        <v>1437</v>
       </c>
     </row>
     <row r="706" spans="1:13" ht="120" x14ac:dyDescent="0.25">
@@ -11382,10 +11382,10 @@
         <v>756</v>
       </c>
       <c r="B706" s="4" t="s">
+        <v>1437</v>
+      </c>
+      <c r="M706" s="4" t="s">
         <v>1438</v>
-      </c>
-      <c r="M706" s="4" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="707" spans="1:13" x14ac:dyDescent="0.25">
@@ -11401,68 +11401,68 @@
     </row>
     <row r="709" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B709" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="M709" s="4" t="s">
         <v>1440</v>
-      </c>
-      <c r="M709" s="4" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="710" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B710" s="4" t="s">
+        <v>1441</v>
+      </c>
+      <c r="M710" s="4" t="s">
         <v>1442</v>
-      </c>
-      <c r="M710" s="4" t="s">
-        <v>1443</v>
       </c>
     </row>
     <row r="711" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B711" s="4" t="s">
+        <v>1443</v>
+      </c>
+      <c r="M711" s="4" t="s">
         <v>1444</v>
-      </c>
-      <c r="M711" s="4" t="s">
-        <v>1445</v>
       </c>
     </row>
     <row r="712" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B712" s="4" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="M712" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="713" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B713" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="M713" s="4" t="s">
         <v>1447</v>
-      </c>
-      <c r="M713" s="4" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="714" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B714" s="4" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="M714" s="4" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
   </sheetData>
@@ -11474,8 +11474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11540,10 +11540,10 @@
         <v>886</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -11551,10 +11551,10 @@
         <v>887</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -11562,10 +11562,10 @@
         <v>888</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
@@ -11573,10 +11573,10 @@
         <v>889</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -11584,10 +11584,10 @@
         <v>890</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -11595,10 +11595,10 @@
         <v>891</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="150" x14ac:dyDescent="0.25">
@@ -11606,10 +11606,10 @@
         <v>892</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="135" x14ac:dyDescent="0.25">
@@ -11617,10 +11617,10 @@
         <v>893</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -11628,10 +11628,10 @@
         <v>894</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -11639,10 +11639,10 @@
         <v>895</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="90" x14ac:dyDescent="0.25">
@@ -11650,10 +11650,10 @@
         <v>896</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="360" x14ac:dyDescent="0.25">
@@ -11661,10 +11661,10 @@
         <v>897</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="135" x14ac:dyDescent="0.25">
@@ -11672,10 +11672,10 @@
         <v>898</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
@@ -11683,10 +11683,10 @@
         <v>899</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="150" x14ac:dyDescent="0.25">
@@ -11694,10 +11694,10 @@
         <v>900</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
@@ -11705,10 +11705,10 @@
         <v>901</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="180" x14ac:dyDescent="0.25">
@@ -11716,10 +11716,10 @@
         <v>902</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="105" x14ac:dyDescent="0.25">
@@ -11727,10 +11727,10 @@
         <v>903</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="195" x14ac:dyDescent="0.25">
@@ -11738,10 +11738,10 @@
         <v>904</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="240" x14ac:dyDescent="0.25">
@@ -11749,296 +11749,296 @@
         <v>905</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>906</v>
+        <v>1767</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="M45" s="4" t="s">
         <v>1241</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>1243</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
   </sheetData>
@@ -12113,376 +12113,376 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B2" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="M2" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B4" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M4" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B5" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="M5" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B6" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="M7" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B8" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="M8" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B9" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="M9" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B10" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B11" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="M11" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B12" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B13" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="M13" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="M14" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B15" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="M15" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B16" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="M16" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B17" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="M17" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B18" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B19" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="M19" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B20" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="B21" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B22" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="M22" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B23" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B24" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="B25" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="M25" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B26" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="M27" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="M28" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B29" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="M29" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B30" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="M31" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="M32" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="M33" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="M34" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="M35" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
   </sheetData>
@@ -12840,175 +12840,175 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="M2" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="M3" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="M4" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="M5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="M6" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="M7" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="M8" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="M9" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="M10" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="M11" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="M12" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="M13" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="M14" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="M15" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="M16" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="M17" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="M18" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="M19" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="M20" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="M21" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="M22" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="M23" t="s">
         <v>344</v>
@@ -13016,96 +13016,96 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="M24" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="M25" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="M26" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M27" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="M28" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="M29" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1405</v>
+      </c>
+      <c r="M30" t="s">
         <v>1406</v>
-      </c>
-      <c r="M30" t="s">
-        <v>1407</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="M31" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="M32" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B33" t="s">
         <v>1673</v>
       </c>
-      <c r="B33" t="s">
+      <c r="M33" t="s">
         <v>1674</v>
-      </c>
-      <c r="M33" t="s">
-        <v>1675</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1684</v>
+      </c>
+      <c r="M34" t="s">
         <v>1683</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1685</v>
-      </c>
-      <c r="M34" t="s">
-        <v>1684</v>
       </c>
     </row>
   </sheetData>
@@ -13179,189 +13179,189 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B2" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="M2" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="M3" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="M4" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="M5" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="M6" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B7" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="M7" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="M8" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B9" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="M9" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B10" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="M10" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B11" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="M11" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B12" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="M12" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B13" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="M13" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B14" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="M14" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B15" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="M15" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B16" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="M16" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B17" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="M17" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B18" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="M18" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
   </sheetData>
@@ -13436,68 +13436,68 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B2" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="M2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B3" t="s">
         <v>1152</v>
       </c>
-      <c r="B3" t="s">
-        <v>1153</v>
-      </c>
       <c r="M3" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B4" t="s">
         <v>1154</v>
       </c>
-      <c r="B4" t="s">
-        <v>1155</v>
-      </c>
       <c r="M4" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B5" t="s">
         <v>1158</v>
       </c>
-      <c r="B5" t="s">
+      <c r="M5" t="s">
         <v>1159</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B6" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="M6" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B7" t="s">
+        <v>1165</v>
+      </c>
+      <c r="M7" t="s">
         <v>1166</v>
-      </c>
-      <c r="M7" t="s">
-        <v>1167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
properly erase plural roles and make it easier to not have this happen again
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387F383D-0AB4-46AA-8B28-096638964043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480FEB20-CCB9-4066-82B9-EC5DAC4E51AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="4875" windowWidth="24510" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="4125" windowWidth="24510" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="1774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1777">
   <si>
     <t>presetSelection</t>
   </si>
@@ -5702,6 +5702,22 @@
   </si>
   <si>
     <t>道連れ</t>
+  </si>
+  <si>
+    <t>plagueDoctorFullDesc</t>
+  </si>
+  <si>
+    <t>・誰か1人に感染病を付与できる
+・感染した人が一定時間の間非感染者の近くにいるとその人も感染者となる
+・感染状況は備蓄される（会議や離れても時間のリセットがされない）
+・ペスト医師がキルされたら、キルした人は感染者となる
+・生存者全員が感染者となることが勝利条件</t>
+  </si>
+  <si>
+    <t>The Plague Doctor is a neutral role whose goal is to infect every living player.
+They start by choosing one player to infect, after which anyone who spends a set
+amount of time in range of the infected player becomes infected themselves.
+Infection progress is cumulative, and does not reset with distance or after meetings.</t>
   </si>
 </sst>
 </file>
@@ -6026,10 +6042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q716"/>
+  <dimension ref="A1:Q717"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A537" workbookViewId="0">
+      <selection activeCell="A548" sqref="A548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10038,174 +10054,174 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="549" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A549" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B549" t="s">
-        <v>1754</v>
-      </c>
-      <c r="M549" t="s">
-        <v>1755</v>
+    <row r="548" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B548" s="4" t="s">
+        <v>1776</v>
+      </c>
+      <c r="M548" s="4" t="s">
+        <v>1775</v>
       </c>
     </row>
     <row r="550" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>1748</v>
+        <v>1753</v>
       </c>
       <c r="B550" t="s">
-        <v>1749</v>
+        <v>1754</v>
       </c>
       <c r="M550" t="s">
-        <v>1752</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="551" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>1726</v>
+        <v>1748</v>
       </c>
       <c r="B551" t="s">
-        <v>1730</v>
+        <v>1749</v>
       </c>
       <c r="M551" t="s">
-        <v>1762</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="552" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B552" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="M552" t="s">
-        <v>1728</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="553" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>1746</v>
+        <v>1727</v>
       </c>
       <c r="B553" t="s">
-        <v>1747</v>
+        <v>1729</v>
       </c>
       <c r="M553" t="s">
-        <v>1766</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="554" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>1756</v>
+        <v>1746</v>
       </c>
       <c r="B554" t="s">
-        <v>1758</v>
+        <v>1747</v>
       </c>
       <c r="M554" t="s">
-        <v>1759</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="555" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B555" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="M555" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="556" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1760</v>
+      </c>
+      <c r="M556" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="557" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
         <v>1763</v>
       </c>
-      <c r="B556" t="s">
+      <c r="B557" t="s">
         <v>1764</v>
       </c>
-      <c r="M556" t="s">
+      <c r="M557" t="s">
         <v>1765</v>
-      </c>
-    </row>
-    <row r="558" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B558" t="s">
-        <v>1739</v>
-      </c>
-      <c r="M558" t="s">
-        <v>1741</v>
       </c>
     </row>
     <row r="559" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B559" t="s">
+        <v>1739</v>
+      </c>
+      <c r="M559" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="560" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
         <v>1736</v>
       </c>
-      <c r="B559" t="s">
+      <c r="B560" t="s">
         <v>1737</v>
       </c>
-      <c r="M559" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="561" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A561" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B561" t="s">
-        <v>1745</v>
-      </c>
-      <c r="M561" t="s">
+      <c r="M560" t="s">
         <v>1740</v>
       </c>
     </row>
     <row r="562" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1745</v>
+      </c>
+      <c r="M562" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="563" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
         <v>1750</v>
       </c>
-      <c r="B562" t="s">
+      <c r="B563" t="s">
         <v>882</v>
       </c>
-      <c r="M562" t="s">
+      <c r="M563" t="s">
         <v>1751</v>
       </c>
     </row>
-    <row r="566" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A566" t="s">
+    <row r="567" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
         <v>1243</v>
       </c>
-      <c r="B566" t="s">
+      <c r="B567" t="s">
         <v>1244</v>
       </c>
-      <c r="M566" t="s">
+      <c r="M567" t="s">
         <v>1245</v>
-      </c>
-    </row>
-    <row r="570" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A570" t="s">
-        <v>374</v>
-      </c>
-      <c r="B570" t="s">
-        <v>562</v>
-      </c>
-      <c r="M570" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="571" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B571" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="M571" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B572" t="s">
         <v>563</v>
@@ -10214,31 +10230,31 @@
         <v>377</v>
       </c>
     </row>
-    <row r="576" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A576" t="s">
-        <v>379</v>
-      </c>
-      <c r="B576" t="s">
-        <v>564</v>
-      </c>
-      <c r="M576" t="s">
-        <v>617</v>
+    <row r="573" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>378</v>
+      </c>
+      <c r="B573" t="s">
+        <v>563</v>
+      </c>
+      <c r="M573" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="577" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B577" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M577" t="s">
-        <v>381</v>
+        <v>617</v>
       </c>
     </row>
     <row r="578" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B578" t="s">
         <v>565</v>
@@ -10247,418 +10263,408 @@
         <v>381</v>
       </c>
     </row>
-    <row r="582" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A582" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B582" t="s">
-        <v>1353</v>
-      </c>
-      <c r="M582" t="s">
-        <v>1356</v>
+    <row r="579" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>382</v>
+      </c>
+      <c r="B579" t="s">
+        <v>565</v>
+      </c>
+      <c r="M579" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B583" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="M583" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="584" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1354</v>
+      </c>
+      <c r="M584" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="585" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
         <v>1352</v>
       </c>
-      <c r="B584" t="s">
+      <c r="B585" t="s">
         <v>1355</v>
       </c>
-      <c r="M584" t="s">
+      <c r="M585" t="s">
         <v>1358</v>
-      </c>
-    </row>
-    <row r="586" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A586" t="s">
-        <v>100</v>
-      </c>
-      <c r="B586" t="s">
-        <v>1012</v>
-      </c>
-      <c r="M586" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="587" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B587" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="M587" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="588" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B588" t="s">
-        <v>512</v>
+        <v>1013</v>
       </c>
       <c r="M588" t="s">
-        <v>211</v>
+        <v>675</v>
       </c>
     </row>
     <row r="589" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B589" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M589" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="590" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>969</v>
+        <v>103</v>
       </c>
       <c r="B590" t="s">
-        <v>971</v>
+        <v>513</v>
       </c>
       <c r="M590" t="s">
-        <v>970</v>
+        <v>212</v>
       </c>
     </row>
     <row r="591" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
+        <v>969</v>
+      </c>
+      <c r="B591" t="s">
+        <v>971</v>
+      </c>
+      <c r="M591" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="592" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
         <v>1396</v>
       </c>
-      <c r="B591" t="s">
+      <c r="B592" t="s">
         <v>1397</v>
       </c>
-      <c r="M591" t="s">
+      <c r="M592" t="s">
         <v>1398</v>
-      </c>
-    </row>
-    <row r="593" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A593" t="s">
-        <v>865</v>
-      </c>
-      <c r="B593" t="s">
-        <v>868</v>
-      </c>
-      <c r="M593" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="594" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A594" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B594" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="M594" t="s">
-        <v>884</v>
+        <v>871</v>
       </c>
     </row>
     <row r="595" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B595" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="M595" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="596" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>626</v>
+        <v>867</v>
       </c>
       <c r="B596" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="M596" t="s">
-        <v>875</v>
+        <v>885</v>
       </c>
     </row>
     <row r="597" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B597" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="M597" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="598" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A598" t="s">
+        <v>628</v>
+      </c>
+      <c r="B598" t="s">
+        <v>873</v>
+      </c>
+      <c r="M598" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="599" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
         <v>627</v>
       </c>
-      <c r="B598" t="s">
+      <c r="B599" t="s">
         <v>874</v>
       </c>
-      <c r="M598" t="s">
+      <c r="M599" t="s">
         <v>877</v>
-      </c>
-    </row>
-    <row r="600" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A600" t="s">
-        <v>878</v>
-      </c>
-      <c r="B600" t="s">
-        <v>879</v>
-      </c>
-      <c r="M600" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="601" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
+        <v>878</v>
+      </c>
+      <c r="B601" t="s">
+        <v>879</v>
+      </c>
+      <c r="M601" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="602" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
         <v>881</v>
       </c>
-      <c r="B601" t="s">
+      <c r="B602" t="s">
         <v>882</v>
       </c>
-      <c r="M601" t="s">
+      <c r="M602" t="s">
         <v>883</v>
-      </c>
-    </row>
-    <row r="603" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B603" t="s">
-        <v>1097</v>
-      </c>
-      <c r="M603" t="s">
-        <v>1098</v>
       </c>
     </row>
     <row r="604" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
-        <v>1084</v>
+        <v>1096</v>
       </c>
       <c r="B604" t="s">
-        <v>1086</v>
+        <v>1097</v>
       </c>
       <c r="M604" t="s">
-        <v>1088</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="605" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A605" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B605" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="M605" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="606" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>629</v>
+        <v>1085</v>
       </c>
       <c r="B606" t="s">
-        <v>625</v>
+        <v>1087</v>
       </c>
       <c r="M606" t="s">
-        <v>630</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="607" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
+        <v>629</v>
+      </c>
+      <c r="B607" t="s">
+        <v>625</v>
+      </c>
+      <c r="M607" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="608" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
         <v>1524</v>
       </c>
-      <c r="B607" t="s">
+      <c r="B608" t="s">
         <v>1525</v>
       </c>
-      <c r="M607" t="s">
+      <c r="M608" t="s">
         <v>1526</v>
       </c>
     </row>
-    <row r="609" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
+    <row r="610" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
         <v>1687</v>
       </c>
-      <c r="B609" t="s">
+      <c r="B610" t="s">
         <v>1688</v>
       </c>
-      <c r="M609" t="s">
+      <c r="M610" t="s">
         <v>1689</v>
-      </c>
-    </row>
-    <row r="613" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A613" t="s">
-        <v>213</v>
-      </c>
-      <c r="B613" t="s">
-        <v>514</v>
-      </c>
-      <c r="M613" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="614" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
+        <v>213</v>
+      </c>
+      <c r="B614" t="s">
+        <v>514</v>
+      </c>
+      <c r="M614" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="615" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
         <v>214</v>
       </c>
-      <c r="B614" t="s">
+      <c r="B615" t="s">
         <v>515</v>
       </c>
-      <c r="M614" t="s">
+      <c r="M615" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="616" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A616" t="s">
-        <v>217</v>
-      </c>
-      <c r="B616" t="s">
-        <v>516</v>
-      </c>
-      <c r="M616" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="617" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B617" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="M617" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="618" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
+        <v>218</v>
+      </c>
+      <c r="B618" t="s">
+        <v>517</v>
+      </c>
+      <c r="M618" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="619" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
         <v>219</v>
       </c>
-      <c r="B618" t="s">
+      <c r="B619" t="s">
         <v>518</v>
       </c>
-      <c r="M618" t="s">
+      <c r="M619" t="s">
         <v>1471</v>
       </c>
     </row>
-    <row r="620" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A620" t="s">
+    <row r="621" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
         <v>220</v>
       </c>
-      <c r="B620" t="s">
+      <c r="B621" t="s">
         <v>221</v>
       </c>
-      <c r="M620" t="s">
+      <c r="M621" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="622" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A622" t="s">
+    <row r="623" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
         <v>1254</v>
       </c>
-      <c r="B622" t="s">
+      <c r="B623" t="s">
         <v>1255</v>
       </c>
-      <c r="M622" t="s">
+      <c r="M623" t="s">
         <v>1256</v>
-      </c>
-    </row>
-    <row r="624" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A624" t="s">
-        <v>394</v>
-      </c>
-      <c r="B624" t="s">
-        <v>586</v>
-      </c>
-      <c r="M624" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="625" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B625" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="M625" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="626" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B626" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="M626" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="627" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B627" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="M627" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="628" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
-        <v>1582</v>
+        <v>397</v>
       </c>
       <c r="B628" t="s">
-        <v>1583</v>
+        <v>589</v>
       </c>
       <c r="M628" t="s">
-        <v>1584</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="629" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>398</v>
-      </c>
-      <c r="B629" s="1" t="s">
-        <v>1569</v>
-      </c>
-      <c r="C629" s="1"/>
-      <c r="D629" s="1"/>
-      <c r="E629" s="1"/>
-      <c r="F629" s="1"/>
-      <c r="G629" s="1"/>
-      <c r="H629" s="1"/>
-      <c r="I629" s="1"/>
-      <c r="J629" s="1"/>
-      <c r="K629" s="1"/>
-      <c r="L629" s="1"/>
-      <c r="M629" s="1" t="s">
-        <v>1472</v>
+        <v>1582</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1583</v>
+      </c>
+      <c r="M629" t="s">
+        <v>1584</v>
       </c>
     </row>
     <row r="630" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>1570</v>
+        <v>398</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>1577</v>
+        <v>1569</v>
       </c>
       <c r="C630" s="1"/>
       <c r="D630" s="1"/>
@@ -10671,15 +10677,15 @@
       <c r="K630" s="1"/>
       <c r="L630" s="1"/>
       <c r="M630" s="1" t="s">
-        <v>1576</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="631" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C631" s="1"/>
       <c r="D631" s="1"/>
@@ -10695,374 +10701,374 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="633" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
-        <v>405</v>
-      </c>
-      <c r="B633" t="s">
-        <v>399</v>
-      </c>
-      <c r="M633" t="s">
-        <v>399</v>
+    <row r="632" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>1571</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C632" s="1"/>
+      <c r="D632" s="1"/>
+      <c r="E632" s="1"/>
+      <c r="F632" s="1"/>
+      <c r="G632" s="1"/>
+      <c r="H632" s="1"/>
+      <c r="I632" s="1"/>
+      <c r="J632" s="1"/>
+      <c r="K632" s="1"/>
+      <c r="L632" s="1"/>
+      <c r="M632" s="1" t="s">
+        <v>1576</v>
       </c>
     </row>
     <row r="634" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
-        <v>735</v>
+        <v>405</v>
       </c>
       <c r="B634" t="s">
-        <v>737</v>
+        <v>399</v>
       </c>
       <c r="M634" t="s">
-        <v>739</v>
+        <v>399</v>
       </c>
     </row>
     <row r="635" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B635" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="M635" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="636" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
-        <v>410</v>
+        <v>736</v>
       </c>
       <c r="B636" t="s">
-        <v>434</v>
+        <v>738</v>
       </c>
       <c r="M636" t="s">
-        <v>400</v>
+        <v>740</v>
       </c>
     </row>
     <row r="637" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A637" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B637" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="M637" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="638" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B638" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M638" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="639" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B639" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="M639" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="640" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B640" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M640" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="641" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1060</v>
+        <v>409</v>
       </c>
       <c r="B641" t="s">
-        <v>1061</v>
+        <v>438</v>
       </c>
       <c r="M641" t="s">
-        <v>1063</v>
+        <v>404</v>
       </c>
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>1553</v>
+        <v>1060</v>
       </c>
       <c r="B642" t="s">
-        <v>1554</v>
+        <v>1061</v>
       </c>
       <c r="M642" t="s">
-        <v>1555</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B643" t="s">
+        <v>1554</v>
+      </c>
+      <c r="M643" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="644" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
         <v>1731</v>
       </c>
-      <c r="B643" t="s">
+      <c r="B644" t="s">
         <v>1735</v>
       </c>
-      <c r="M643" t="s">
+      <c r="M644" t="s">
         <v>1743</v>
-      </c>
-    </row>
-    <row r="645" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
-        <v>819</v>
-      </c>
-      <c r="B645" t="s">
-        <v>826</v>
-      </c>
-      <c r="M645" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="646" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B646" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="M646" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="647" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B647" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="M647" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="648" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A648" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B648" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="M648" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B649" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="M649" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B650" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="M650" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="651" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B651" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="M651" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>1065</v>
+        <v>825</v>
       </c>
       <c r="B652" t="s">
-        <v>1062</v>
+        <v>832</v>
       </c>
       <c r="M652" t="s">
-        <v>1064</v>
+        <v>839</v>
       </c>
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>1557</v>
+        <v>1065</v>
       </c>
       <c r="B653" t="s">
-        <v>1558</v>
+        <v>1062</v>
       </c>
       <c r="M653" t="s">
-        <v>1556</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="654" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B654" t="s">
+        <v>1558</v>
+      </c>
+      <c r="M654" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="655" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
         <v>1732</v>
       </c>
-      <c r="B654" t="s">
+      <c r="B655" t="s">
         <v>1733</v>
       </c>
-      <c r="M654" t="s">
+      <c r="M655" t="s">
         <v>1734</v>
-      </c>
-    </row>
-    <row r="656" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A656" t="s">
-        <v>840</v>
-      </c>
-      <c r="B656" t="s">
-        <v>1530</v>
-      </c>
-      <c r="M656" t="s">
-        <v>1533</v>
       </c>
     </row>
     <row r="657" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B657" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
       <c r="M657" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="658" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>1493</v>
+        <v>841</v>
       </c>
       <c r="B658" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="M658" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="659" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="B659" t="s">
-        <v>1496</v>
+        <v>1535</v>
       </c>
       <c r="M659" t="s">
-        <v>1499</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="660" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B660" t="s">
+        <v>1496</v>
+      </c>
+      <c r="M660" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="661" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
         <v>1494</v>
       </c>
-      <c r="B660" t="s">
+      <c r="B661" t="s">
         <v>1497</v>
       </c>
-      <c r="M660" t="s">
+      <c r="M661" t="s">
         <v>1498</v>
-      </c>
-    </row>
-    <row r="664" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A664" t="s">
-        <v>411</v>
-      </c>
-      <c r="B664" t="s">
-        <v>439</v>
-      </c>
-      <c r="M664" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="665" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B665" t="s">
-        <v>415</v>
+        <v>439</v>
       </c>
       <c r="M665" t="s">
-        <v>432</v>
+        <v>733</v>
       </c>
     </row>
     <row r="666" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B666" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M666" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="667" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>845</v>
+        <v>413</v>
       </c>
       <c r="B667" t="s">
-        <v>846</v>
+        <v>414</v>
       </c>
       <c r="M667" t="s">
-        <v>847</v>
+        <v>433</v>
       </c>
     </row>
     <row r="668" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B668" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="M668" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="669" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>851</v>
-      </c>
-      <c r="B669" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C669" s="3"/>
-      <c r="D669" s="3"/>
-      <c r="E669" s="3"/>
-      <c r="F669" s="3"/>
-      <c r="G669" s="3"/>
-      <c r="H669" s="3"/>
-      <c r="I669" s="3"/>
-      <c r="J669" s="3"/>
-      <c r="K669" s="3"/>
-      <c r="L669" s="3"/>
-      <c r="M669" s="2" t="s">
-        <v>853</v>
+        <v>848</v>
+      </c>
+      <c r="B669" t="s">
+        <v>849</v>
+      </c>
+      <c r="M669" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="670" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A670" t="s">
-        <v>962</v>
+        <v>851</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>963</v>
+        <v>852</v>
       </c>
       <c r="C670" s="3"/>
       <c r="D670" s="3"/>
@@ -11075,15 +11081,15 @@
       <c r="K670" s="3"/>
       <c r="L670" s="3"/>
       <c r="M670" s="2" t="s">
-        <v>964</v>
+        <v>853</v>
       </c>
     </row>
     <row r="671" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1559</v>
+        <v>962</v>
       </c>
       <c r="B671" s="2" t="s">
-        <v>1560</v>
+        <v>963</v>
       </c>
       <c r="C671" s="3"/>
       <c r="D671" s="3"/>
@@ -11096,15 +11102,15 @@
       <c r="K671" s="3"/>
       <c r="L671" s="3"/>
       <c r="M671" s="2" t="s">
-        <v>1295</v>
+        <v>964</v>
       </c>
     </row>
     <row r="672" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B672" s="2" t="s">
-        <v>1567</v>
+        <v>1560</v>
       </c>
       <c r="C672" s="3"/>
       <c r="D672" s="3"/>
@@ -11117,15 +11123,15 @@
       <c r="K672" s="3"/>
       <c r="L672" s="3"/>
       <c r="M672" s="2" t="s">
-        <v>1568</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="673" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1771</v>
+        <v>1566</v>
       </c>
       <c r="B673" s="2" t="s">
-        <v>1772</v>
+        <v>1567</v>
       </c>
       <c r="C673" s="3"/>
       <c r="D673" s="3"/>
@@ -11138,380 +11144,401 @@
       <c r="K673" s="3"/>
       <c r="L673" s="3"/>
       <c r="M673" s="2" t="s">
-        <v>1773</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="674" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B674" s="2" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C674" s="3"/>
+      <c r="D674" s="3"/>
+      <c r="E674" s="3"/>
+      <c r="F674" s="3"/>
+      <c r="G674" s="3"/>
+      <c r="H674" s="3"/>
+      <c r="I674" s="3"/>
+      <c r="J674" s="3"/>
+      <c r="K674" s="3"/>
+      <c r="L674" s="3"/>
+      <c r="M674" s="2" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="675" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
         <v>1588</v>
       </c>
-      <c r="B674" t="s">
+      <c r="B675" t="s">
         <v>734</v>
       </c>
-      <c r="M674" t="s">
+      <c r="M675" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="676" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A676" t="s">
+    <row r="677" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
         <v>1587</v>
       </c>
-      <c r="B676" s="2" t="s">
+      <c r="B677" s="2" t="s">
         <v>1585</v>
       </c>
-      <c r="M676" s="2" t="s">
+      <c r="M677" s="2" t="s">
         <v>1586</v>
-      </c>
-    </row>
-    <row r="678" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A678" t="s">
-        <v>420</v>
-      </c>
-      <c r="B678" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="M678" s="4" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="679" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B679" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="M679" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="680" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B680" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="M680" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="681" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
+        <v>422</v>
+      </c>
+      <c r="B681" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="M681" s="4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="682" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
         <v>423</v>
       </c>
-      <c r="B681" s="4" t="s">
+      <c r="B682" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="M681" s="4" t="s">
+      <c r="M682" s="4" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="682" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A682" t="s">
+    <row r="683" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
         <v>1500</v>
       </c>
-      <c r="B682" s="4" t="s">
+      <c r="B683" s="4" t="s">
         <v>1501</v>
       </c>
-      <c r="M682" s="4" t="s">
+      <c r="M683" s="4" t="s">
         <v>1502</v>
-      </c>
-    </row>
-    <row r="685" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A685" t="s">
-        <v>594</v>
-      </c>
-      <c r="B685" t="s">
-        <v>425</v>
-      </c>
-      <c r="M685" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B686" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M686" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="687" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A687" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B687" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M687" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="688" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
+        <v>596</v>
+      </c>
+      <c r="B688" t="s">
+        <v>427</v>
+      </c>
+      <c r="M688" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="689" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
         <v>1527</v>
       </c>
-      <c r="B688" t="s">
+      <c r="B689" t="s">
         <v>1529</v>
       </c>
-      <c r="M688" t="s">
+      <c r="M689" t="s">
         <v>1528</v>
-      </c>
-    </row>
-    <row r="690" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A690" t="s">
-        <v>621</v>
-      </c>
-      <c r="B690" t="s">
-        <v>633</v>
-      </c>
-      <c r="M690" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="691" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
+        <v>621</v>
+      </c>
+      <c r="B691" t="s">
+        <v>633</v>
+      </c>
+      <c r="M691" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="692" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
         <v>622</v>
       </c>
-      <c r="B691" t="s">
+      <c r="B692" t="s">
         <v>624</v>
       </c>
-      <c r="M691" t="s">
+      <c r="M692" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="693" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A693" t="s">
+    <row r="694" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
         <v>637</v>
       </c>
-      <c r="B693" t="s">
+      <c r="B694" t="s">
         <v>638</v>
       </c>
-      <c r="M693" t="s">
+      <c r="M694" t="s">
         <v>639</v>
-      </c>
-    </row>
-    <row r="695" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A695" t="s">
-        <v>742</v>
-      </c>
-      <c r="B695" t="s">
-        <v>743</v>
-      </c>
-      <c r="M695" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="696" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
-        <v>862</v>
+        <v>742</v>
       </c>
       <c r="B696" t="s">
-        <v>863</v>
+        <v>743</v>
       </c>
       <c r="M696" t="s">
-        <v>864</v>
+        <v>745</v>
       </c>
     </row>
     <row r="697" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
-        <v>746</v>
+        <v>862</v>
       </c>
       <c r="B697" t="s">
-        <v>744</v>
+        <v>863</v>
       </c>
       <c r="M697" t="s">
-        <v>748</v>
+        <v>864</v>
       </c>
     </row>
     <row r="698" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B698" t="s">
         <v>744</v>
       </c>
       <c r="M698" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="699" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B699" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="M699" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1589</v>
+        <v>751</v>
       </c>
       <c r="B700" t="s">
         <v>747</v>
       </c>
       <c r="M700" t="s">
-        <v>1590</v>
+        <v>747</v>
       </c>
     </row>
     <row r="701" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1742</v>
+        <v>1589</v>
       </c>
       <c r="B701" t="s">
-        <v>863</v>
+        <v>747</v>
       </c>
       <c r="M701" t="s">
-        <v>863</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="702" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1640</v>
+        <v>1742</v>
       </c>
       <c r="B702" t="s">
-        <v>744</v>
+        <v>863</v>
       </c>
       <c r="M702" t="s">
-        <v>1641</v>
+        <v>863</v>
       </c>
     </row>
     <row r="703" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1608</v>
+        <v>1640</v>
       </c>
       <c r="B703" t="s">
-        <v>1609</v>
+        <v>744</v>
       </c>
       <c r="M703" t="s">
-        <v>1610</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="704" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1685</v>
+        <v>1608</v>
       </c>
       <c r="B704" t="s">
-        <v>744</v>
+        <v>1609</v>
       </c>
       <c r="M704" t="s">
-        <v>1686</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="705" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B705" t="s">
+        <v>744</v>
+      </c>
+      <c r="M705" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="706" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A706" t="s">
         <v>1690</v>
       </c>
-      <c r="B705" s="5" t="s">
+      <c r="B706" s="5" t="s">
         <v>1691</v>
       </c>
-      <c r="M705" t="s">
+      <c r="M706" t="s">
         <v>1691</v>
       </c>
     </row>
-    <row r="707" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A707" t="s">
+    <row r="708" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
         <v>755</v>
       </c>
-      <c r="B707" s="4" t="s">
+      <c r="B708" s="4" t="s">
         <v>1435</v>
       </c>
-      <c r="M707" s="4" t="s">
+      <c r="M708" s="4" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="708" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
+    <row r="709" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A709" t="s">
         <v>756</v>
       </c>
-      <c r="B708" s="4" t="s">
+      <c r="B709" s="4" t="s">
         <v>1437</v>
       </c>
-      <c r="M708" s="4" t="s">
+      <c r="M709" s="4" t="s">
         <v>1438</v>
       </c>
     </row>
-    <row r="709" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A709" t="s">
+    <row r="710" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A710" t="s">
         <v>757</v>
       </c>
-      <c r="B709" t="s">
+      <c r="B710" t="s">
         <v>759</v>
       </c>
-      <c r="M709" t="s">
+      <c r="M710" t="s">
         <v>758</v>
-      </c>
-    </row>
-    <row r="711" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B711" s="4" t="s">
-        <v>1439</v>
-      </c>
-      <c r="M711" s="4" t="s">
-        <v>1440</v>
       </c>
     </row>
     <row r="712" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B712" s="4" t="s">
+        <v>1439</v>
+      </c>
+      <c r="M712" s="4" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="713" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
         <v>1075</v>
       </c>
-      <c r="B712" s="4" t="s">
+      <c r="B713" s="4" t="s">
         <v>1441</v>
       </c>
-      <c r="M712" s="4" t="s">
+      <c r="M713" s="4" t="s">
         <v>1442</v>
       </c>
     </row>
-    <row r="713" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A713" t="s">
+    <row r="714" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
         <v>1076</v>
       </c>
-      <c r="B713" s="4" t="s">
+      <c r="B714" s="4" t="s">
         <v>1443</v>
       </c>
-      <c r="M713" s="4" t="s">
+      <c r="M714" s="4" t="s">
         <v>1444</v>
       </c>
     </row>
-    <row r="714" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A714" t="s">
+    <row r="715" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
         <v>1077</v>
       </c>
-      <c r="B714" s="4" t="s">
+      <c r="B715" s="4" t="s">
         <v>1445</v>
       </c>
-      <c r="M714" t="s">
+      <c r="M715" t="s">
         <v>1080</v>
-      </c>
-    </row>
-    <row r="715" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
-        <v>1078</v>
-      </c>
-      <c r="B715" s="4" t="s">
-        <v>1446</v>
-      </c>
-      <c r="M715" s="4" t="s">
-        <v>1447</v>
       </c>
     </row>
     <row r="716" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B716" s="4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="M716" s="4" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="717" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A717" t="s">
         <v>1079</v>
       </c>
-      <c r="B716" s="4" t="s">
+      <c r="B717" s="4" t="s">
         <v>1448</v>
       </c>
-      <c r="M716" s="4" t="s">
+      <c r="M717" s="4" t="s">
         <v>1444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes for fox/immoralist/fortune teller
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046ACF0C-A05A-4E7A-AAA0-E8C8FAF37EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA949134-5447-46BA-8C3A-1664A9A5A4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="6210" windowWidth="20445" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7065" yWindow="3915" windowWidth="25425" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="Hats" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6100,8 +6099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q729"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="B203" workbookViewId="0">
+      <selection activeCell="B225" sqref="B225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11678,7 +11677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A33E95B-9199-4E2D-AE11-F907336D1402}">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes in prep for 3.5.0 release
* handle the situation in which everyone is dead at the end of the game
* plague doctor victims are now treated as dead at the end of the game
* dead ninja's clothes now properly go transparent
* fix for unnecessary text showing up around buttons when playing in english
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA949134-5447-46BA-8C3A-1664A9A5A4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446FD3D9-7EB1-4E76-AA1E-E758EFA41DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="3915" windowWidth="25425" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="4305" windowWidth="25425" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="1795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="1828">
   <si>
     <t>presetSelection</t>
   </si>
@@ -5773,6 +5773,112 @@
   <si>
     <t>・能力を使うと一定時間視界が広くなる
 ・能力使用時、透明化中の&lt;color=#ff1919ff&gt;ニンジャ&lt;/color&gt;を視認できる</t>
+  </si>
+  <si>
+    <t>[BLANK]</t>
+  </si>
+  <si>
+    <t>Everyone Died</t>
+  </si>
+  <si>
+    <t>Diseased</t>
+  </si>
+  <si>
+    <t>roleSummaryDiseased</t>
+  </si>
+  <si>
+    <t>病死</t>
+  </si>
+  <si>
+    <t>everyoneDied</t>
+  </si>
+  <si>
+    <t>誰もいなくなった</t>
+  </si>
+  <si>
+    <t>・キルクールがインポスターやジャッカルより短い
+・キルをしたら次のキルまでの時間が表示され時間内にキルをしないと自爆する
+・キルをし続ければ自爆はしない
+・会議で自爆タイマーがリセットされる（設定による）</t>
+  </si>
+  <si>
+    <t>追放されたら、ランダムに道連れにする</t>
+  </si>
+  <si>
+    <t>Take Revenge When Exiled</t>
+  </si>
+  <si>
+    <t>nekoKabochaRevengeExile</t>
+  </si>
+  <si>
+    <t>インポスターに殺されたら、道連れにする</t>
+  </si>
+  <si>
+    <t>Take Revenge on Impostor Killer</t>
+  </si>
+  <si>
+    <t>nekoKabochaRevengeImpostor</t>
+  </si>
+  <si>
+    <t>その他陣営に殺されたら、道連れにする</t>
+  </si>
+  <si>
+    <t>Take Revenge on Neutral Killer</t>
+  </si>
+  <si>
+    <t>nekoKabochaRevengeNeutral</t>
+  </si>
+  <si>
+    <t>クルーに殺されたら、道連れにする</t>
+  </si>
+  <si>
+    <t>Take Revenge on Crew Killer</t>
+  </si>
+  <si>
+    <t>nekoKabochaRevengeCrew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">・殺害された場合のみ殺害したプレイヤーを道連れにする
+以下は設定によって変更可能
+・クルー陣営（シェリフ等）に殺された場合、道連れが発生するorしない
+・インポスター陣営（スパイがいる時）に殺された場合、道連れが発生するorしない
+・その他陣営（ジャッカル等）に殺害された場合、道連れが発生するorしない </t>
+  </si>
+  <si>
+    <t>An Impostor capable of revenge-killing their killer.</t>
+  </si>
+  <si>
+    <t>nekoKabochaFullDesc</t>
+  </si>
+  <si>
+    <t>独りでは絶対に死ねない</t>
+  </si>
+  <si>
+    <t>You will never die alone</t>
+  </si>
+  <si>
+    <t>nekoKabochaShortDesc</t>
+  </si>
+  <si>
+    <t>nekoKabochaIntroDesc</t>
+  </si>
+  <si>
+    <t>ネコカボチャ</t>
+  </si>
+  <si>
+    <t>Neko-Kabocha</t>
+  </si>
+  <si>
+    <t>nekoKabocha</t>
+  </si>
+  <si>
+    <t>視界外のプレイヤーの名前を非表示にする</t>
+  </si>
+  <si>
+    <t>Hide Out-Of-Sight Nametags</t>
+  </si>
+  <si>
+    <t>hideOutOfSightNametags</t>
   </si>
 </sst>
 </file>
@@ -6097,10 +6203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q729"/>
+  <dimension ref="A1:Q743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B203" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+    <sheetView tabSelected="1" topLeftCell="A609" workbookViewId="0">
+      <selection activeCell="A619" sqref="A619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10285,9 +10391,12 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="570" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>1776</v>
+      </c>
+      <c r="M570" s="4" t="s">
+        <v>1802</v>
       </c>
     </row>
     <row r="572" spans="1:13" x14ac:dyDescent="0.25">
@@ -10323,1348 +10432,1473 @@
         <v>1790</v>
       </c>
     </row>
+    <row r="578" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1823</v>
+      </c>
+      <c r="M578" t="s">
+        <v>1822</v>
+      </c>
+    </row>
     <row r="579" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>1239</v>
+        <v>1821</v>
       </c>
       <c r="B579" t="s">
-        <v>1240</v>
+        <v>1819</v>
       </c>
       <c r="M579" t="s">
-        <v>1241</v>
-      </c>
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="580" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1819</v>
+      </c>
+      <c r="M580" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="581" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B581" s="4" t="s">
+        <v>1816</v>
+      </c>
+      <c r="M581" s="4" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="582" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B582" s="4"/>
+      <c r="M582" s="4"/>
     </row>
     <row r="583" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>374</v>
-      </c>
-      <c r="B583" t="s">
-        <v>562</v>
-      </c>
-      <c r="M583" t="s">
-        <v>375</v>
+        <v>1814</v>
+      </c>
+      <c r="B583" s="4" t="s">
+        <v>1813</v>
+      </c>
+      <c r="M583" s="4" t="s">
+        <v>1812</v>
       </c>
     </row>
     <row r="584" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>376</v>
-      </c>
-      <c r="B584" t="s">
-        <v>563</v>
-      </c>
-      <c r="M584" t="s">
-        <v>377</v>
+        <v>1811</v>
+      </c>
+      <c r="B584" s="4" t="s">
+        <v>1810</v>
+      </c>
+      <c r="M584" s="4" t="s">
+        <v>1809</v>
       </c>
     </row>
     <row r="585" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
-        <v>378</v>
-      </c>
-      <c r="B585" t="s">
-        <v>563</v>
-      </c>
-      <c r="M585" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="589" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
-        <v>379</v>
-      </c>
-      <c r="B589" t="s">
-        <v>564</v>
-      </c>
-      <c r="M589" t="s">
-        <v>617</v>
+        <v>1808</v>
+      </c>
+      <c r="B585" s="4" t="s">
+        <v>1807</v>
+      </c>
+      <c r="M585" s="4" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="586" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B586" s="4" t="s">
+        <v>1804</v>
+      </c>
+      <c r="M586" s="4" t="s">
+        <v>1803</v>
       </c>
     </row>
     <row r="590" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
-        <v>380</v>
+        <v>1239</v>
       </c>
       <c r="B590" t="s">
-        <v>565</v>
+        <v>1240</v>
       </c>
       <c r="M590" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="591" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
-        <v>382</v>
-      </c>
-      <c r="B591" t="s">
-        <v>565</v>
-      </c>
-      <c r="M591" t="s">
-        <v>381</v>
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="594" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>374</v>
+      </c>
+      <c r="B594" t="s">
+        <v>562</v>
+      </c>
+      <c r="M594" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="595" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A595" t="s">
-        <v>1346</v>
+        <v>376</v>
       </c>
       <c r="B595" t="s">
-        <v>1349</v>
+        <v>563</v>
       </c>
       <c r="M595" t="s">
-        <v>1352</v>
+        <v>377</v>
       </c>
     </row>
     <row r="596" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
-        <v>1347</v>
+        <v>378</v>
       </c>
       <c r="B596" t="s">
-        <v>1350</v>
+        <v>563</v>
       </c>
       <c r="M596" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="597" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A597" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B597" t="s">
-        <v>1351</v>
-      </c>
-      <c r="M597" t="s">
-        <v>1354</v>
-      </c>
-    </row>
-    <row r="599" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A599" t="s">
-        <v>100</v>
-      </c>
-      <c r="B599" t="s">
-        <v>1008</v>
-      </c>
-      <c r="M599" t="s">
-        <v>674</v>
+        <v>377</v>
       </c>
     </row>
     <row r="600" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
-        <v>101</v>
+        <v>379</v>
       </c>
       <c r="B600" t="s">
-        <v>1009</v>
+        <v>564</v>
       </c>
       <c r="M600" t="s">
-        <v>675</v>
+        <v>617</v>
       </c>
     </row>
     <row r="601" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
-        <v>102</v>
+        <v>380</v>
       </c>
       <c r="B601" t="s">
-        <v>512</v>
+        <v>565</v>
       </c>
       <c r="M601" t="s">
-        <v>211</v>
+        <v>381</v>
       </c>
     </row>
     <row r="602" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
-        <v>103</v>
+        <v>382</v>
       </c>
       <c r="B602" t="s">
-        <v>513</v>
+        <v>565</v>
       </c>
       <c r="M602" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="603" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
-        <v>965</v>
-      </c>
-      <c r="B603" t="s">
-        <v>967</v>
-      </c>
-      <c r="M603" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="604" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A604" t="s">
-        <v>1392</v>
-      </c>
-      <c r="B604" t="s">
-        <v>1393</v>
-      </c>
-      <c r="M604" t="s">
-        <v>1394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="606" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
-        <v>865</v>
+        <v>1346</v>
       </c>
       <c r="B606" t="s">
-        <v>868</v>
+        <v>1349</v>
       </c>
       <c r="M606" t="s">
-        <v>871</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="607" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
-        <v>866</v>
+        <v>1347</v>
       </c>
       <c r="B607" t="s">
-        <v>869</v>
+        <v>1350</v>
       </c>
       <c r="M607" t="s">
-        <v>884</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="608" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
-        <v>867</v>
+        <v>1348</v>
       </c>
       <c r="B608" t="s">
-        <v>870</v>
+        <v>1351</v>
       </c>
       <c r="M608" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="609" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
-        <v>626</v>
-      </c>
-      <c r="B609" t="s">
-        <v>872</v>
-      </c>
-      <c r="M609" t="s">
-        <v>875</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="610" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
-        <v>628</v>
+        <v>100</v>
       </c>
       <c r="B610" t="s">
-        <v>873</v>
+        <v>1008</v>
       </c>
       <c r="M610" t="s">
-        <v>876</v>
+        <v>674</v>
       </c>
     </row>
     <row r="611" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A611" t="s">
-        <v>627</v>
+        <v>101</v>
       </c>
       <c r="B611" t="s">
-        <v>874</v>
+        <v>1009</v>
       </c>
       <c r="M611" t="s">
-        <v>877</v>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="612" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>102</v>
+      </c>
+      <c r="B612" t="s">
+        <v>512</v>
+      </c>
+      <c r="M612" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="613" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A613" t="s">
-        <v>878</v>
+        <v>103</v>
       </c>
       <c r="B613" t="s">
-        <v>879</v>
+        <v>513</v>
       </c>
       <c r="M613" t="s">
-        <v>880</v>
+        <v>212</v>
       </c>
     </row>
     <row r="614" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A614" t="s">
-        <v>881</v>
+        <v>965</v>
       </c>
       <c r="B614" t="s">
-        <v>882</v>
+        <v>967</v>
       </c>
       <c r="M614" t="s">
-        <v>883</v>
+        <v>966</v>
+      </c>
+    </row>
+    <row r="615" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1393</v>
+      </c>
+      <c r="M615" t="s">
+        <v>1394</v>
       </c>
     </row>
     <row r="616" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
-        <v>1092</v>
+        <v>1827</v>
       </c>
       <c r="B616" t="s">
-        <v>1093</v>
+        <v>1826</v>
       </c>
       <c r="M616" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="617" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B617" t="s">
-        <v>1082</v>
-      </c>
-      <c r="M617" t="s">
-        <v>1084</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="618" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
-        <v>1081</v>
+        <v>865</v>
       </c>
       <c r="B618" t="s">
-        <v>1083</v>
+        <v>868</v>
       </c>
       <c r="M618" t="s">
-        <v>1085</v>
+        <v>871</v>
       </c>
     </row>
     <row r="619" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
-        <v>629</v>
+        <v>866</v>
       </c>
       <c r="B619" t="s">
-        <v>625</v>
+        <v>869</v>
       </c>
       <c r="M619" t="s">
-        <v>630</v>
+        <v>884</v>
       </c>
     </row>
     <row r="620" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
-        <v>1520</v>
+        <v>867</v>
       </c>
       <c r="B620" t="s">
-        <v>1521</v>
+        <v>870</v>
       </c>
       <c r="M620" t="s">
-        <v>1522</v>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="621" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>626</v>
+      </c>
+      <c r="B621" t="s">
+        <v>872</v>
+      </c>
+      <c r="M621" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="622" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
-        <v>1683</v>
+        <v>628</v>
       </c>
       <c r="B622" t="s">
-        <v>1684</v>
+        <v>873</v>
       </c>
       <c r="M622" t="s">
-        <v>1685</v>
+        <v>876</v>
+      </c>
+    </row>
+    <row r="623" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>627</v>
+      </c>
+      <c r="B623" t="s">
+        <v>874</v>
+      </c>
+      <c r="M623" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="625" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>878</v>
+      </c>
+      <c r="B625" t="s">
+        <v>879</v>
+      </c>
+      <c r="M625" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="626" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
-        <v>213</v>
+        <v>881</v>
       </c>
       <c r="B626" t="s">
-        <v>514</v>
+        <v>882</v>
       </c>
       <c r="M626" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="627" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
-        <v>214</v>
-      </c>
-      <c r="B627" t="s">
-        <v>515</v>
-      </c>
-      <c r="M627" t="s">
-        <v>216</v>
+        <v>883</v>
+      </c>
+    </row>
+    <row r="628" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M628" t="s">
+        <v>1094</v>
       </c>
     </row>
     <row r="629" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
-        <v>217</v>
+        <v>1080</v>
       </c>
       <c r="B629" t="s">
-        <v>516</v>
+        <v>1082</v>
       </c>
       <c r="M629" t="s">
-        <v>1465</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="630" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A630" t="s">
-        <v>218</v>
+        <v>1081</v>
       </c>
       <c r="B630" t="s">
-        <v>517</v>
+        <v>1083</v>
       </c>
       <c r="M630" t="s">
-        <v>1466</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="631" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A631" t="s">
-        <v>219</v>
+        <v>629</v>
       </c>
       <c r="B631" t="s">
-        <v>518</v>
+        <v>625</v>
       </c>
       <c r="M631" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="633" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
-        <v>220</v>
-      </c>
-      <c r="B633" t="s">
-        <v>221</v>
-      </c>
-      <c r="M633" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="635" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A635" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B635" t="s">
-        <v>1251</v>
-      </c>
-      <c r="M635" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="637" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A637" t="s">
-        <v>394</v>
-      </c>
-      <c r="B637" t="s">
-        <v>586</v>
-      </c>
-      <c r="M637" t="s">
-        <v>1568</v>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="632" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1521</v>
+      </c>
+      <c r="M632" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="634" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B634" t="s">
+        <v>1684</v>
+      </c>
+      <c r="M634" t="s">
+        <v>1685</v>
       </c>
     </row>
     <row r="638" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A638" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B638" t="s">
-        <v>587</v>
+        <v>514</v>
       </c>
       <c r="M638" t="s">
-        <v>1569</v>
+        <v>215</v>
       </c>
     </row>
     <row r="639" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
-        <v>396</v>
+        <v>214</v>
       </c>
       <c r="B639" t="s">
-        <v>588</v>
+        <v>515</v>
       </c>
       <c r="M639" t="s">
-        <v>1570</v>
-      </c>
-    </row>
-    <row r="640" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A640" t="s">
-        <v>397</v>
-      </c>
-      <c r="B640" t="s">
-        <v>589</v>
-      </c>
-      <c r="M640" t="s">
-        <v>1571</v>
+        <v>216</v>
       </c>
     </row>
     <row r="641" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A641" t="s">
-        <v>1578</v>
+        <v>217</v>
       </c>
       <c r="B641" t="s">
-        <v>1579</v>
+        <v>516</v>
       </c>
       <c r="M641" t="s">
-        <v>1580</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="642" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A642" t="s">
-        <v>398</v>
-      </c>
-      <c r="B642" s="1" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C642" s="1"/>
-      <c r="D642" s="1"/>
-      <c r="E642" s="1"/>
-      <c r="F642" s="1"/>
-      <c r="G642" s="1"/>
-      <c r="H642" s="1"/>
-      <c r="I642" s="1"/>
-      <c r="J642" s="1"/>
-      <c r="K642" s="1"/>
-      <c r="L642" s="1"/>
-      <c r="M642" s="1" t="s">
-        <v>1468</v>
+        <v>218</v>
+      </c>
+      <c r="B642" t="s">
+        <v>517</v>
+      </c>
+      <c r="M642" t="s">
+        <v>1466</v>
       </c>
     </row>
     <row r="643" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A643" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B643" s="1" t="s">
-        <v>1573</v>
-      </c>
-      <c r="C643" s="1"/>
-      <c r="D643" s="1"/>
-      <c r="E643" s="1"/>
-      <c r="F643" s="1"/>
-      <c r="G643" s="1"/>
-      <c r="H643" s="1"/>
-      <c r="I643" s="1"/>
-      <c r="J643" s="1"/>
-      <c r="K643" s="1"/>
-      <c r="L643" s="1"/>
-      <c r="M643" s="1" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="644" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A644" t="s">
-        <v>1567</v>
-      </c>
-      <c r="B644" s="1" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C644" s="1"/>
-      <c r="D644" s="1"/>
-      <c r="E644" s="1"/>
-      <c r="F644" s="1"/>
-      <c r="G644" s="1"/>
-      <c r="H644" s="1"/>
-      <c r="I644" s="1"/>
-      <c r="J644" s="1"/>
-      <c r="K644" s="1"/>
-      <c r="L644" s="1"/>
-      <c r="M644" s="1" t="s">
-        <v>1572</v>
-      </c>
-    </row>
-    <row r="646" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A646" t="s">
-        <v>405</v>
-      </c>
-      <c r="B646" t="s">
-        <v>399</v>
-      </c>
-      <c r="M646" t="s">
-        <v>399</v>
+        <v>219</v>
+      </c>
+      <c r="B643" t="s">
+        <v>518</v>
+      </c>
+      <c r="M643" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="645" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>220</v>
+      </c>
+      <c r="B645" t="s">
+        <v>221</v>
+      </c>
+      <c r="M645" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="647" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
-        <v>735</v>
+        <v>1250</v>
       </c>
       <c r="B647" t="s">
-        <v>737</v>
+        <v>1251</v>
       </c>
       <c r="M647" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="648" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A648" t="s">
-        <v>736</v>
-      </c>
-      <c r="B648" t="s">
-        <v>738</v>
-      </c>
-      <c r="M648" t="s">
-        <v>740</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A649" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="B649" t="s">
-        <v>434</v>
+        <v>586</v>
       </c>
       <c r="M649" t="s">
-        <v>400</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A650" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="B650" t="s">
-        <v>435</v>
+        <v>587</v>
       </c>
       <c r="M650" t="s">
-        <v>401</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="651" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="B651" t="s">
-        <v>436</v>
+        <v>588</v>
       </c>
       <c r="M651" t="s">
-        <v>402</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="652" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A652" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="B652" t="s">
-        <v>437</v>
+        <v>589</v>
       </c>
       <c r="M652" t="s">
-        <v>403</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="653" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A653" t="s">
-        <v>409</v>
+        <v>1578</v>
       </c>
       <c r="B653" t="s">
-        <v>438</v>
+        <v>1579</v>
       </c>
       <c r="M653" t="s">
-        <v>404</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="654" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B654" t="s">
-        <v>1057</v>
-      </c>
-      <c r="M654" t="s">
-        <v>1059</v>
+        <v>398</v>
+      </c>
+      <c r="B654" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C654" s="1"/>
+      <c r="D654" s="1"/>
+      <c r="E654" s="1"/>
+      <c r="F654" s="1"/>
+      <c r="G654" s="1"/>
+      <c r="H654" s="1"/>
+      <c r="I654" s="1"/>
+      <c r="J654" s="1"/>
+      <c r="K654" s="1"/>
+      <c r="L654" s="1"/>
+      <c r="M654" s="1" t="s">
+        <v>1468</v>
       </c>
     </row>
     <row r="655" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B655" t="s">
-        <v>1550</v>
-      </c>
-      <c r="M655" t="s">
-        <v>1551</v>
+        <v>1566</v>
+      </c>
+      <c r="B655" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C655" s="1"/>
+      <c r="D655" s="1"/>
+      <c r="E655" s="1"/>
+      <c r="F655" s="1"/>
+      <c r="G655" s="1"/>
+      <c r="H655" s="1"/>
+      <c r="I655" s="1"/>
+      <c r="J655" s="1"/>
+      <c r="K655" s="1"/>
+      <c r="L655" s="1"/>
+      <c r="M655" s="1" t="s">
+        <v>1572</v>
       </c>
     </row>
     <row r="656" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B656" t="s">
-        <v>1731</v>
-      </c>
-      <c r="M656" t="s">
-        <v>1739</v>
+        <v>1567</v>
+      </c>
+      <c r="B656" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C656" s="1"/>
+      <c r="D656" s="1"/>
+      <c r="E656" s="1"/>
+      <c r="F656" s="1"/>
+      <c r="G656" s="1"/>
+      <c r="H656" s="1"/>
+      <c r="I656" s="1"/>
+      <c r="J656" s="1"/>
+      <c r="K656" s="1"/>
+      <c r="L656" s="1"/>
+      <c r="M656" s="1" t="s">
+        <v>1572</v>
       </c>
     </row>
     <row r="658" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A658" t="s">
-        <v>819</v>
+        <v>405</v>
       </c>
       <c r="B658" t="s">
-        <v>826</v>
+        <v>399</v>
       </c>
       <c r="M658" t="s">
-        <v>833</v>
+        <v>399</v>
       </c>
     </row>
     <row r="659" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
-        <v>820</v>
+        <v>735</v>
       </c>
       <c r="B659" t="s">
-        <v>827</v>
+        <v>737</v>
       </c>
       <c r="M659" t="s">
-        <v>834</v>
+        <v>739</v>
       </c>
     </row>
     <row r="660" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
-        <v>821</v>
+        <v>736</v>
       </c>
       <c r="B660" t="s">
-        <v>828</v>
+        <v>738</v>
       </c>
       <c r="M660" t="s">
-        <v>835</v>
+        <v>740</v>
       </c>
     </row>
     <row r="661" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
-        <v>822</v>
+        <v>410</v>
       </c>
       <c r="B661" t="s">
-        <v>829</v>
+        <v>434</v>
       </c>
       <c r="M661" t="s">
-        <v>836</v>
+        <v>400</v>
       </c>
     </row>
     <row r="662" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A662" t="s">
-        <v>823</v>
+        <v>406</v>
       </c>
       <c r="B662" t="s">
-        <v>830</v>
+        <v>435</v>
       </c>
       <c r="M662" t="s">
-        <v>837</v>
+        <v>401</v>
       </c>
     </row>
     <row r="663" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A663" t="s">
-        <v>824</v>
+        <v>407</v>
       </c>
       <c r="B663" t="s">
-        <v>831</v>
+        <v>436</v>
       </c>
       <c r="M663" t="s">
-        <v>838</v>
+        <v>402</v>
       </c>
     </row>
     <row r="664" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
-        <v>825</v>
+        <v>408</v>
       </c>
       <c r="B664" t="s">
-        <v>832</v>
+        <v>437</v>
       </c>
       <c r="M664" t="s">
-        <v>839</v>
+        <v>403</v>
       </c>
     </row>
     <row r="665" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A665" t="s">
-        <v>1061</v>
+        <v>409</v>
       </c>
       <c r="B665" t="s">
-        <v>1058</v>
+        <v>438</v>
       </c>
       <c r="M665" t="s">
-        <v>1060</v>
+        <v>404</v>
       </c>
     </row>
     <row r="666" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A666" t="s">
-        <v>1553</v>
+        <v>1056</v>
       </c>
       <c r="B666" t="s">
-        <v>1554</v>
+        <v>1057</v>
       </c>
       <c r="M666" t="s">
-        <v>1552</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="667" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
-        <v>1728</v>
+        <v>1549</v>
       </c>
       <c r="B667" t="s">
-        <v>1729</v>
+        <v>1550</v>
       </c>
       <c r="M667" t="s">
-        <v>1730</v>
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="668" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B668" t="s">
+        <v>1731</v>
+      </c>
+      <c r="M668" t="s">
+        <v>1739</v>
       </c>
     </row>
     <row r="669" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A669" t="s">
-        <v>840</v>
+        <v>1800</v>
       </c>
       <c r="B669" t="s">
-        <v>1526</v>
+        <v>1796</v>
       </c>
       <c r="M669" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="670" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A670" t="s">
-        <v>841</v>
-      </c>
-      <c r="B670" t="s">
-        <v>1530</v>
-      </c>
-      <c r="M670" t="s">
-        <v>1528</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="671" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A671" t="s">
-        <v>1489</v>
+        <v>819</v>
       </c>
       <c r="B671" t="s">
-        <v>1531</v>
+        <v>826</v>
       </c>
       <c r="M671" t="s">
-        <v>1532</v>
+        <v>833</v>
       </c>
     </row>
     <row r="672" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
-        <v>1491</v>
+        <v>820</v>
       </c>
       <c r="B672" t="s">
-        <v>1492</v>
+        <v>827</v>
       </c>
       <c r="M672" t="s">
-        <v>1495</v>
+        <v>834</v>
       </c>
     </row>
     <row r="673" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
-        <v>1490</v>
+        <v>821</v>
       </c>
       <c r="B673" t="s">
-        <v>1493</v>
+        <v>828</v>
       </c>
       <c r="M673" t="s">
-        <v>1494</v>
+        <v>835</v>
+      </c>
+    </row>
+    <row r="674" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A674" t="s">
+        <v>822</v>
+      </c>
+      <c r="B674" t="s">
+        <v>829</v>
+      </c>
+      <c r="M674" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="675" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
+        <v>823</v>
+      </c>
+      <c r="B675" t="s">
+        <v>830</v>
+      </c>
+      <c r="M675" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="676" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
+        <v>824</v>
+      </c>
+      <c r="B676" t="s">
+        <v>831</v>
+      </c>
+      <c r="M676" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="677" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A677" t="s">
-        <v>411</v>
+        <v>825</v>
       </c>
       <c r="B677" t="s">
-        <v>439</v>
+        <v>832</v>
       </c>
       <c r="M677" t="s">
-        <v>733</v>
+        <v>839</v>
       </c>
     </row>
     <row r="678" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A678" t="s">
-        <v>412</v>
+        <v>1061</v>
       </c>
       <c r="B678" t="s">
-        <v>415</v>
+        <v>1058</v>
       </c>
       <c r="M678" t="s">
-        <v>432</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="679" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A679" t="s">
-        <v>413</v>
+        <v>1553</v>
       </c>
       <c r="B679" t="s">
-        <v>414</v>
+        <v>1554</v>
       </c>
       <c r="M679" t="s">
-        <v>433</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="680" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
-        <v>845</v>
+        <v>1728</v>
       </c>
       <c r="B680" t="s">
-        <v>846</v>
+        <v>1729</v>
       </c>
       <c r="M680" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="681" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A681" t="s">
-        <v>848</v>
-      </c>
-      <c r="B681" t="s">
-        <v>849</v>
-      </c>
-      <c r="M681" t="s">
-        <v>850</v>
+        <v>1730</v>
       </c>
     </row>
     <row r="682" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>851</v>
-      </c>
-      <c r="B682" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C682" s="3"/>
-      <c r="D682" s="3"/>
-      <c r="E682" s="3"/>
-      <c r="F682" s="3"/>
-      <c r="G682" s="3"/>
-      <c r="H682" s="3"/>
-      <c r="I682" s="3"/>
-      <c r="J682" s="3"/>
-      <c r="K682" s="3"/>
-      <c r="L682" s="3"/>
-      <c r="M682" s="2" t="s">
-        <v>853</v>
+        <v>840</v>
+      </c>
+      <c r="B682" t="s">
+        <v>1526</v>
+      </c>
+      <c r="M682" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="683" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
-        <v>958</v>
-      </c>
-      <c r="B683" s="2" t="s">
-        <v>959</v>
-      </c>
-      <c r="C683" s="3"/>
-      <c r="D683" s="3"/>
-      <c r="E683" s="3"/>
-      <c r="F683" s="3"/>
-      <c r="G683" s="3"/>
-      <c r="H683" s="3"/>
-      <c r="I683" s="3"/>
-      <c r="J683" s="3"/>
-      <c r="K683" s="3"/>
-      <c r="L683" s="3"/>
-      <c r="M683" s="2" t="s">
-        <v>960</v>
+        <v>841</v>
+      </c>
+      <c r="B683" t="s">
+        <v>1530</v>
+      </c>
+      <c r="M683" t="s">
+        <v>1528</v>
       </c>
     </row>
     <row r="684" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A684" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B684" s="2" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C684" s="3"/>
-      <c r="D684" s="3"/>
-      <c r="E684" s="3"/>
-      <c r="F684" s="3"/>
-      <c r="G684" s="3"/>
-      <c r="H684" s="3"/>
-      <c r="I684" s="3"/>
-      <c r="J684" s="3"/>
-      <c r="K684" s="3"/>
-      <c r="L684" s="3"/>
-      <c r="M684" s="2" t="s">
-        <v>1291</v>
+        <v>1489</v>
+      </c>
+      <c r="B684" t="s">
+        <v>1531</v>
+      </c>
+      <c r="M684" t="s">
+        <v>1532</v>
       </c>
     </row>
     <row r="685" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A685" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B685" s="2" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C685" s="3"/>
-      <c r="D685" s="3"/>
-      <c r="E685" s="3"/>
-      <c r="F685" s="3"/>
-      <c r="G685" s="3"/>
-      <c r="H685" s="3"/>
-      <c r="I685" s="3"/>
-      <c r="J685" s="3"/>
-      <c r="K685" s="3"/>
-      <c r="L685" s="3"/>
-      <c r="M685" s="2" t="s">
-        <v>1564</v>
+        <v>1491</v>
+      </c>
+      <c r="B685" t="s">
+        <v>1492</v>
+      </c>
+      <c r="M685" t="s">
+        <v>1495</v>
       </c>
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A686" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B686" s="2" t="s">
-        <v>1768</v>
-      </c>
-      <c r="C686" s="3"/>
-      <c r="D686" s="3"/>
-      <c r="E686" s="3"/>
-      <c r="F686" s="3"/>
-      <c r="G686" s="3"/>
-      <c r="H686" s="3"/>
-      <c r="I686" s="3"/>
-      <c r="J686" s="3"/>
-      <c r="K686" s="3"/>
-      <c r="L686" s="3"/>
-      <c r="M686" s="2" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="687" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A687" t="s">
-        <v>1584</v>
-      </c>
-      <c r="B687" t="s">
-        <v>734</v>
-      </c>
-      <c r="M687" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="689" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
-        <v>1583</v>
-      </c>
-      <c r="B689" s="2" t="s">
-        <v>1581</v>
-      </c>
-      <c r="M689" s="2" t="s">
-        <v>1582</v>
+        <v>1490</v>
+      </c>
+      <c r="B686" t="s">
+        <v>1493</v>
+      </c>
+      <c r="M686" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="690" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>411</v>
+      </c>
+      <c r="B690" t="s">
+        <v>439</v>
+      </c>
+      <c r="M690" t="s">
+        <v>733</v>
       </c>
     </row>
     <row r="691" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
-        <v>420</v>
-      </c>
-      <c r="B691" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="M691" s="4" t="s">
-        <v>416</v>
+        <v>412</v>
+      </c>
+      <c r="B691" t="s">
+        <v>415</v>
+      </c>
+      <c r="M691" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="692" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A692" t="s">
-        <v>421</v>
-      </c>
-      <c r="B692" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="M692" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
+      </c>
+      <c r="B692" t="s">
+        <v>414</v>
+      </c>
+      <c r="M692" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="693" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
-        <v>422</v>
-      </c>
-      <c r="B693" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="M693" s="4" t="s">
-        <v>418</v>
+        <v>845</v>
+      </c>
+      <c r="B693" t="s">
+        <v>846</v>
+      </c>
+      <c r="M693" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="694" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
-        <v>423</v>
-      </c>
-      <c r="B694" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="M694" s="4" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="695" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>848</v>
+      </c>
+      <c r="B694" t="s">
+        <v>849</v>
+      </c>
+      <c r="M694" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="695" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
-        <v>1496</v>
-      </c>
-      <c r="B695" s="4" t="s">
-        <v>1497</v>
-      </c>
-      <c r="M695" s="4" t="s">
-        <v>1498</v>
+        <v>851</v>
+      </c>
+      <c r="B695" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="C695" s="3"/>
+      <c r="D695" s="3"/>
+      <c r="E695" s="3"/>
+      <c r="F695" s="3"/>
+      <c r="G695" s="3"/>
+      <c r="H695" s="3"/>
+      <c r="I695" s="3"/>
+      <c r="J695" s="3"/>
+      <c r="K695" s="3"/>
+      <c r="L695" s="3"/>
+      <c r="M695" s="2" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="696" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>958</v>
+      </c>
+      <c r="B696" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="C696" s="3"/>
+      <c r="D696" s="3"/>
+      <c r="E696" s="3"/>
+      <c r="F696" s="3"/>
+      <c r="G696" s="3"/>
+      <c r="H696" s="3"/>
+      <c r="I696" s="3"/>
+      <c r="J696" s="3"/>
+      <c r="K696" s="3"/>
+      <c r="L696" s="3"/>
+      <c r="M696" s="2" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="697" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B697" s="2" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C697" s="3"/>
+      <c r="D697" s="3"/>
+      <c r="E697" s="3"/>
+      <c r="F697" s="3"/>
+      <c r="G697" s="3"/>
+      <c r="H697" s="3"/>
+      <c r="I697" s="3"/>
+      <c r="J697" s="3"/>
+      <c r="K697" s="3"/>
+      <c r="L697" s="3"/>
+      <c r="M697" s="2" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row r="698" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
-        <v>594</v>
-      </c>
-      <c r="B698" t="s">
-        <v>425</v>
-      </c>
-      <c r="M698" t="s">
-        <v>429</v>
+        <v>1562</v>
+      </c>
+      <c r="B698" s="2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C698" s="3"/>
+      <c r="D698" s="3"/>
+      <c r="E698" s="3"/>
+      <c r="F698" s="3"/>
+      <c r="G698" s="3"/>
+      <c r="H698" s="3"/>
+      <c r="I698" s="3"/>
+      <c r="J698" s="3"/>
+      <c r="K698" s="3"/>
+      <c r="L698" s="3"/>
+      <c r="M698" s="2" t="s">
+        <v>1564</v>
       </c>
     </row>
     <row r="699" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A699" t="s">
-        <v>595</v>
-      </c>
-      <c r="B699" t="s">
-        <v>426</v>
-      </c>
-      <c r="M699" t="s">
-        <v>428</v>
+        <v>1767</v>
+      </c>
+      <c r="B699" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C699" s="3"/>
+      <c r="D699" s="3"/>
+      <c r="E699" s="3"/>
+      <c r="F699" s="3"/>
+      <c r="G699" s="3"/>
+      <c r="H699" s="3"/>
+      <c r="I699" s="3"/>
+      <c r="J699" s="3"/>
+      <c r="K699" s="3"/>
+      <c r="L699" s="3"/>
+      <c r="M699" s="2" t="s">
+        <v>1769</v>
       </c>
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>596</v>
-      </c>
-      <c r="B700" t="s">
-        <v>427</v>
-      </c>
-      <c r="M700" t="s">
-        <v>430</v>
+        <v>1798</v>
+      </c>
+      <c r="B700" s="2" t="s">
+        <v>1797</v>
+      </c>
+      <c r="M700" s="2" t="s">
+        <v>1799</v>
       </c>
     </row>
     <row r="701" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1523</v>
+        <v>1584</v>
       </c>
       <c r="B701" t="s">
-        <v>1525</v>
+        <v>734</v>
       </c>
       <c r="M701" t="s">
-        <v>1524</v>
+        <v>635</v>
       </c>
     </row>
     <row r="703" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>621</v>
-      </c>
-      <c r="B703" t="s">
-        <v>633</v>
-      </c>
-      <c r="M703" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="704" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A704" t="s">
-        <v>622</v>
-      </c>
-      <c r="B704" t="s">
-        <v>624</v>
-      </c>
-      <c r="M704" t="s">
-        <v>631</v>
+        <v>1583</v>
+      </c>
+      <c r="B703" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="M703" s="2" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="705" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
+        <v>420</v>
+      </c>
+      <c r="B705" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="M705" s="4" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="706" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>637</v>
-      </c>
-      <c r="B706" t="s">
-        <v>638</v>
-      </c>
-      <c r="M706" t="s">
-        <v>639</v>
+        <v>421</v>
+      </c>
+      <c r="B706" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="M706" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="707" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
+        <v>422</v>
+      </c>
+      <c r="B707" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="M707" s="4" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="708" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>742</v>
-      </c>
-      <c r="B708" t="s">
-        <v>743</v>
-      </c>
-      <c r="M708" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="709" spans="1:13" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="B708" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="M708" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="709" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>862</v>
-      </c>
-      <c r="B709" t="s">
-        <v>863</v>
-      </c>
-      <c r="M709" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="710" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
-        <v>746</v>
-      </c>
-      <c r="B710" t="s">
-        <v>744</v>
-      </c>
-      <c r="M710" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="711" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
-        <v>749</v>
-      </c>
-      <c r="B711" t="s">
-        <v>744</v>
-      </c>
-      <c r="M711" t="s">
-        <v>750</v>
+        <v>1496</v>
+      </c>
+      <c r="B709" s="4" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M709" s="4" t="s">
+        <v>1498</v>
       </c>
     </row>
     <row r="712" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>751</v>
+        <v>594</v>
       </c>
       <c r="B712" t="s">
-        <v>747</v>
+        <v>425</v>
       </c>
       <c r="M712" t="s">
-        <v>747</v>
+        <v>429</v>
       </c>
     </row>
     <row r="713" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1585</v>
+        <v>595</v>
       </c>
       <c r="B713" t="s">
-        <v>747</v>
+        <v>426</v>
       </c>
       <c r="M713" t="s">
-        <v>1586</v>
+        <v>428</v>
       </c>
     </row>
     <row r="714" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1738</v>
+        <v>596</v>
       </c>
       <c r="B714" t="s">
-        <v>863</v>
+        <v>427</v>
       </c>
       <c r="M714" t="s">
-        <v>863</v>
+        <v>430</v>
       </c>
     </row>
     <row r="715" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1636</v>
+        <v>1523</v>
       </c>
       <c r="B715" t="s">
-        <v>744</v>
+        <v>1525</v>
       </c>
       <c r="M715" t="s">
-        <v>1637</v>
-      </c>
-    </row>
-    <row r="716" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A716" t="s">
-        <v>1604</v>
-      </c>
-      <c r="B716" t="s">
-        <v>1605</v>
-      </c>
-      <c r="M716" t="s">
-        <v>1606</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="717" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1681</v>
+        <v>621</v>
       </c>
       <c r="B717" t="s">
-        <v>744</v>
+        <v>633</v>
       </c>
       <c r="M717" t="s">
-        <v>1682</v>
+        <v>634</v>
       </c>
     </row>
     <row r="718" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B718" s="5" t="s">
-        <v>1687</v>
+        <v>622</v>
+      </c>
+      <c r="B718" t="s">
+        <v>624</v>
       </c>
       <c r="M718" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="720" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="720" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>755</v>
-      </c>
-      <c r="B720" s="4" t="s">
-        <v>1431</v>
-      </c>
-      <c r="M720" s="4" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="721" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A721" t="s">
-        <v>756</v>
-      </c>
-      <c r="B721" s="4" t="s">
-        <v>1433</v>
-      </c>
-      <c r="M721" s="4" t="s">
-        <v>1434</v>
+        <v>637</v>
+      </c>
+      <c r="B720" t="s">
+        <v>638</v>
+      </c>
+      <c r="M720" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="722" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
+        <v>742</v>
+      </c>
+      <c r="B722" t="s">
+        <v>743</v>
+      </c>
+      <c r="M722" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="723" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A723" t="s">
+        <v>862</v>
+      </c>
+      <c r="B723" t="s">
+        <v>863</v>
+      </c>
+      <c r="M723" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="724" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
+        <v>746</v>
+      </c>
+      <c r="B724" t="s">
+        <v>744</v>
+      </c>
+      <c r="M724" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="725" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
+        <v>749</v>
+      </c>
+      <c r="B725" t="s">
+        <v>744</v>
+      </c>
+      <c r="M725" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="726" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
+        <v>751</v>
+      </c>
+      <c r="B726" t="s">
+        <v>747</v>
+      </c>
+      <c r="M726" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="727" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A727" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B727" t="s">
+        <v>747</v>
+      </c>
+      <c r="M727" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="728" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A728" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B728" t="s">
+        <v>863</v>
+      </c>
+      <c r="M728" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="729" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A729" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B729" t="s">
+        <v>744</v>
+      </c>
+      <c r="M729" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="730" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A730" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B730" t="s">
+        <v>1605</v>
+      </c>
+      <c r="M730" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="731" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B731" t="s">
+        <v>744</v>
+      </c>
+      <c r="M731" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="732" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B732" s="5" t="s">
+        <v>1687</v>
+      </c>
+      <c r="M732" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="734" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A734" t="s">
+        <v>755</v>
+      </c>
+      <c r="B734" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="M734" s="4" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="735" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
+        <v>756</v>
+      </c>
+      <c r="B735" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="M735" s="4" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="736" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A736" t="s">
         <v>757</v>
       </c>
-      <c r="B722" t="s">
+      <c r="B736" t="s">
         <v>759</v>
       </c>
-      <c r="M722" t="s">
+      <c r="M736" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="724" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A724" t="s">
+    <row r="738" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
         <v>1077</v>
       </c>
-      <c r="B724" s="4" t="s">
+      <c r="B738" s="4" t="s">
         <v>1435</v>
       </c>
-      <c r="M724" s="4" t="s">
+      <c r="M738" s="4" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="725" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A725" t="s">
+    <row r="739" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
         <v>1071</v>
       </c>
-      <c r="B725" s="4" t="s">
+      <c r="B739" s="4" t="s">
         <v>1437</v>
       </c>
-      <c r="M725" s="4" t="s">
+      <c r="M739" s="4" t="s">
         <v>1438</v>
       </c>
     </row>
-    <row r="726" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A726" t="s">
+    <row r="740" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
         <v>1072</v>
       </c>
-      <c r="B726" s="4" t="s">
+      <c r="B740" s="4" t="s">
         <v>1439</v>
       </c>
-      <c r="M726" s="4" t="s">
+      <c r="M740" s="4" t="s">
         <v>1440</v>
       </c>
     </row>
-    <row r="727" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A727" t="s">
+    <row r="741" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
         <v>1073</v>
       </c>
-      <c r="B727" s="4" t="s">
+      <c r="B741" s="4" t="s">
         <v>1441</v>
       </c>
-      <c r="M727" t="s">
+      <c r="M741" t="s">
         <v>1076</v>
       </c>
     </row>
-    <row r="728" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A728" t="s">
+    <row r="742" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
         <v>1074</v>
       </c>
-      <c r="B728" s="4" t="s">
+      <c r="B742" s="4" t="s">
         <v>1442</v>
       </c>
-      <c r="M728" s="4" t="s">
+      <c r="M742" s="4" t="s">
         <v>1443</v>
       </c>
     </row>
-    <row r="729" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A729" t="s">
+    <row r="743" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
         <v>1075</v>
       </c>
-      <c r="B729" s="4" t="s">
+      <c r="B743" s="4" t="s">
         <v>1444</v>
       </c>
-      <c r="M729" s="4" t="s">
+      <c r="M743" s="4" t="s">
         <v>1440</v>
       </c>
     </row>
@@ -12253,7 +12487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E24339F-182E-497F-BCB5-E8925B014635}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -12981,8 +13215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E03A3E-CD6E-42CA-AC43-3F5764A8A875}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13045,6 +13279,9 @@
       <c r="A2" t="s">
         <v>1309</v>
       </c>
+      <c r="B2" t="s">
+        <v>1795</v>
+      </c>
       <c r="M2" t="s">
         <v>1287</v>
       </c>
@@ -13053,6 +13290,9 @@
       <c r="A3" t="s">
         <v>1310</v>
       </c>
+      <c r="B3" t="s">
+        <v>1795</v>
+      </c>
       <c r="M3" t="s">
         <v>1288</v>
       </c>
@@ -13061,6 +13301,9 @@
       <c r="A4" t="s">
         <v>1311</v>
       </c>
+      <c r="B4" t="s">
+        <v>1795</v>
+      </c>
       <c r="M4" t="s">
         <v>1289</v>
       </c>
@@ -13069,6 +13312,9 @@
       <c r="A5" t="s">
         <v>1312</v>
       </c>
+      <c r="B5" t="s">
+        <v>1795</v>
+      </c>
       <c r="M5" t="s">
         <v>1290</v>
       </c>
@@ -13077,6 +13323,9 @@
       <c r="A6" t="s">
         <v>1313</v>
       </c>
+      <c r="B6" t="s">
+        <v>1795</v>
+      </c>
       <c r="M6" t="s">
         <v>1291</v>
       </c>
@@ -13085,6 +13334,9 @@
       <c r="A7" t="s">
         <v>1314</v>
       </c>
+      <c r="B7" t="s">
+        <v>1795</v>
+      </c>
       <c r="M7" t="s">
         <v>1292</v>
       </c>
@@ -13093,6 +13345,9 @@
       <c r="A8" t="s">
         <v>1315</v>
       </c>
+      <c r="B8" t="s">
+        <v>1795</v>
+      </c>
       <c r="M8" t="s">
         <v>1293</v>
       </c>
@@ -13101,6 +13356,9 @@
       <c r="A9" t="s">
         <v>1316</v>
       </c>
+      <c r="B9" t="s">
+        <v>1795</v>
+      </c>
       <c r="M9" t="s">
         <v>1294</v>
       </c>
@@ -13109,6 +13367,9 @@
       <c r="A10" t="s">
         <v>1317</v>
       </c>
+      <c r="B10" t="s">
+        <v>1795</v>
+      </c>
       <c r="M10" t="s">
         <v>1295</v>
       </c>
@@ -13117,6 +13378,9 @@
       <c r="A11" t="s">
         <v>1318</v>
       </c>
+      <c r="B11" t="s">
+        <v>1795</v>
+      </c>
       <c r="M11" t="s">
         <v>1296</v>
       </c>
@@ -13125,6 +13389,9 @@
       <c r="A12" t="s">
         <v>1319</v>
       </c>
+      <c r="B12" t="s">
+        <v>1795</v>
+      </c>
       <c r="M12" t="s">
         <v>1297</v>
       </c>
@@ -13133,6 +13400,9 @@
       <c r="A13" t="s">
         <v>1320</v>
       </c>
+      <c r="B13" t="s">
+        <v>1795</v>
+      </c>
       <c r="M13" t="s">
         <v>1298</v>
       </c>
@@ -13141,6 +13411,9 @@
       <c r="A14" t="s">
         <v>1321</v>
       </c>
+      <c r="B14" t="s">
+        <v>1795</v>
+      </c>
       <c r="M14" t="s">
         <v>1403</v>
       </c>
@@ -13149,6 +13422,9 @@
       <c r="A15" t="s">
         <v>1322</v>
       </c>
+      <c r="B15" t="s">
+        <v>1795</v>
+      </c>
       <c r="M15" t="s">
         <v>1299</v>
       </c>
@@ -13157,6 +13433,9 @@
       <c r="A16" t="s">
         <v>1323</v>
       </c>
+      <c r="B16" t="s">
+        <v>1795</v>
+      </c>
       <c r="M16" t="s">
         <v>1299</v>
       </c>
@@ -13165,6 +13444,9 @@
       <c r="A17" t="s">
         <v>1324</v>
       </c>
+      <c r="B17" t="s">
+        <v>1795</v>
+      </c>
       <c r="M17" t="s">
         <v>1400</v>
       </c>
@@ -13173,6 +13455,9 @@
       <c r="A18" t="s">
         <v>1325</v>
       </c>
+      <c r="B18" t="s">
+        <v>1795</v>
+      </c>
       <c r="M18" t="s">
         <v>1300</v>
       </c>
@@ -13181,6 +13466,9 @@
       <c r="A19" t="s">
         <v>1326</v>
       </c>
+      <c r="B19" t="s">
+        <v>1795</v>
+      </c>
       <c r="M19" t="s">
         <v>1301</v>
       </c>
@@ -13189,6 +13477,9 @@
       <c r="A20" t="s">
         <v>1327</v>
       </c>
+      <c r="B20" t="s">
+        <v>1795</v>
+      </c>
       <c r="M20" t="s">
         <v>1308</v>
       </c>
@@ -13197,6 +13488,9 @@
       <c r="A21" t="s">
         <v>1328</v>
       </c>
+      <c r="B21" t="s">
+        <v>1795</v>
+      </c>
       <c r="M21" t="s">
         <v>1302</v>
       </c>
@@ -13205,6 +13499,9 @@
       <c r="A22" t="s">
         <v>1329</v>
       </c>
+      <c r="B22" t="s">
+        <v>1795</v>
+      </c>
       <c r="M22" t="s">
         <v>1303</v>
       </c>
@@ -13213,6 +13510,9 @@
       <c r="A23" t="s">
         <v>1330</v>
       </c>
+      <c r="B23" t="s">
+        <v>1795</v>
+      </c>
       <c r="M23" t="s">
         <v>344</v>
       </c>
@@ -13221,6 +13521,9 @@
       <c r="A24" t="s">
         <v>1331</v>
       </c>
+      <c r="B24" t="s">
+        <v>1795</v>
+      </c>
       <c r="M24" t="s">
         <v>1302</v>
       </c>
@@ -13229,6 +13532,9 @@
       <c r="A25" t="s">
         <v>1332</v>
       </c>
+      <c r="B25" t="s">
+        <v>1795</v>
+      </c>
       <c r="M25" t="s">
         <v>1304</v>
       </c>
@@ -13237,6 +13543,9 @@
       <c r="A26" t="s">
         <v>1333</v>
       </c>
+      <c r="B26" t="s">
+        <v>1795</v>
+      </c>
       <c r="M26" t="s">
         <v>1305</v>
       </c>
@@ -13245,6 +13554,9 @@
       <c r="A27" t="s">
         <v>1334</v>
       </c>
+      <c r="B27" t="s">
+        <v>1795</v>
+      </c>
       <c r="M27" t="s">
         <v>1306</v>
       </c>
@@ -13253,6 +13565,9 @@
       <c r="A28" t="s">
         <v>1335</v>
       </c>
+      <c r="B28" t="s">
+        <v>1795</v>
+      </c>
       <c r="M28" t="s">
         <v>1307</v>
       </c>
@@ -13261,6 +13576,9 @@
       <c r="A29" t="s">
         <v>1336</v>
       </c>
+      <c r="B29" t="s">
+        <v>1795</v>
+      </c>
       <c r="M29" t="s">
         <v>1406</v>
       </c>
@@ -13269,6 +13587,9 @@
       <c r="A30" t="s">
         <v>1401</v>
       </c>
+      <c r="B30" t="s">
+        <v>1795</v>
+      </c>
       <c r="M30" t="s">
         <v>1402</v>
       </c>
@@ -13277,6 +13598,9 @@
       <c r="A31" t="s">
         <v>1500</v>
       </c>
+      <c r="B31" t="s">
+        <v>1795</v>
+      </c>
       <c r="M31" t="s">
         <v>1561</v>
       </c>
@@ -13284,6 +13608,9 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1499</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1795</v>
       </c>
       <c r="M32" t="s">
         <v>1501</v>

</xml_diff>

<commit_message>
update for tonsen's first march edition
* madmate is now an attribute, allowing it to double up with other roles
* madmate fanatic mode
* the GM is not a crewmate
* calculate madmate/fox tasks in the same function
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CB6863-CF49-45E0-A88B-FE27D32855D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DA0FD8-04C1-4E5E-9184-976928FB9702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="5130" windowWidth="21330" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="6045" windowWidth="21330" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -6367,8 +6367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q765"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A644" workbookViewId="0">
-      <selection activeCell="B650" sqref="B650"/>
+    <sheetView tabSelected="1" topLeftCell="A437" workbookViewId="0">
+      <selection activeCell="A452" sqref="A452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
partially update to v2022.3.29s
* add sprinter
* disable morphling until we can figure out how to make it work again
* pet prefab went missing, so we have to figure out a new way to spawn other people's pets for morphing
* HatBehaviour renamed to HatData, largely works the same otherwise (altshader seems to have gone missing tho)
* Dleks was removed from the game, so remove the ability to select it
* the role intro sequence was changed to a coroutine, making it harder to modify (temp solution still shows the original "your role is Crewmate" for a frame before swapping in the correct role)
* update nameplate patch, bc the first one in the list is no longer the blank nameplate
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF64BB7C-2584-4468-AB6D-5E3456D8A003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E48B32C-135E-4E54-A89A-A09FA5012367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="6090" windowWidth="29640" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="5925" windowWidth="27720" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -9183,8 +9183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A860" workbookViewId="0">
-      <selection activeCell="O828" sqref="O828"/>
+    <sheetView tabSelected="1" topLeftCell="A552" workbookViewId="0">
+      <selection activeCell="M568" sqref="M568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
few fixes from 3.5.5
* fix a bug that prevented jackal/fox/eraser from being able to create sidekicks/erase roles
* implemented sc translation for sprinter
* pass information about what role we're changing into when erasing old role info
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Streaming\Among Us\TheOtherRoles-GM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB9254A-C576-4442-8BC0-EE53B53BAD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F11DAE-925A-4898-A87A-59DF22E91E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38475" yWindow="6990" windowWidth="27720" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="7500" windowWidth="27720" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3121" uniqueCount="2747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3159" uniqueCount="2783">
   <si>
     <t>presetSelection</t>
   </si>
@@ -8815,6 +8815,114 @@
   </si>
   <si>
     <t>诱惑</t>
+  </si>
+  <si>
+    <t>sprinter</t>
+  </si>
+  <si>
+    <t>Sprinter</t>
+  </si>
+  <si>
+    <t>スプリンター</t>
+  </si>
+  <si>
+    <t>飞毛腿</t>
+  </si>
+  <si>
+    <t>sprinterIntroDesc</t>
+  </si>
+  <si>
+    <t>Run from the Impostors</t>
+  </si>
+  <si>
+    <t>走ってインポスターから逃げよう</t>
+  </si>
+  <si>
+    <t>只要不停下来，道路就会不断延伸</t>
+  </si>
+  <si>
+    <t>sprinterShortDesc</t>
+  </si>
+  <si>
+    <t>从内鬼身边溜走</t>
+  </si>
+  <si>
+    <t>sprinterFullDesc</t>
+  </si>
+  <si>
+    <t>A Crewmate who can run at super high speeds.</t>
+  </si>
+  <si>
+    <t>・能力を使うと移動速度が上がる</t>
+  </si>
+  <si>
+    <t>sprinterCooldown</t>
+  </si>
+  <si>
+    <t>Sprint Cooldown</t>
+  </si>
+  <si>
+    <t>スプリントクールダウン</t>
+  </si>
+  <si>
+    <t>飞毛腿冲刺冷却</t>
+  </si>
+  <si>
+    <t>sprinterDuration</t>
+  </si>
+  <si>
+    <t>Sprint Duration</t>
+  </si>
+  <si>
+    <t>スプリント持続時間</t>
+  </si>
+  <si>
+    <t>飞毛腿冲刺持续时间</t>
+  </si>
+  <si>
+    <t>sprinterSpeedBonus</t>
+  </si>
+  <si>
+    <t>Sprint Speed Bonus</t>
+  </si>
+  <si>
+    <t>スプリント中移動速度</t>
+  </si>
+  <si>
+    <t>毛腿冲刺持续时间内移动速度增幅</t>
+  </si>
+  <si>
+    <t>SprinterText</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>スプリント</t>
+  </si>
+  <si>
+    <t>冲刺</t>
+  </si>
+  <si>
+    <t>SprinterStopText</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>休む</t>
+  </si>
+  <si>
+    <t>停下</t>
+  </si>
+  <si>
+    <t>enabledHorseMode</t>
+  </si>
+  <si>
+    <t>Horse Around</t>
+  </si>
+  <si>
+    <t>ウマングアス</t>
   </si>
 </sst>
 </file>
@@ -9181,10 +9289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q864"/>
+  <dimension ref="A1:Q876"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="A292" sqref="A292"/>
+    <sheetView tabSelected="1" topLeftCell="A719" workbookViewId="0">
+      <selection activeCell="A726" sqref="A726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15754,2025 +15862,2142 @@
         <v>2734</v>
       </c>
     </row>
+    <row r="690" spans="1:15">
+      <c r="O690"/>
+    </row>
     <row r="691" spans="1:15">
       <c r="A691" t="s">
-        <v>1239</v>
+        <v>2747</v>
       </c>
       <c r="B691" t="s">
-        <v>1240</v>
+        <v>2748</v>
       </c>
       <c r="M691" t="s">
-        <v>1241</v>
-      </c>
-      <c r="O691" s="9" t="s">
-        <v>2419</v>
-      </c>
+        <v>2749</v>
+      </c>
+      <c r="O691" t="s">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="692" spans="1:15">
+      <c r="A692" t="s">
+        <v>2751</v>
+      </c>
+      <c r="B692" t="s">
+        <v>2752</v>
+      </c>
+      <c r="M692" t="s">
+        <v>2753</v>
+      </c>
+      <c r="O692" t="s">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="693" spans="1:15">
+      <c r="A693" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B693" t="s">
+        <v>2752</v>
+      </c>
+      <c r="M693" t="s">
+        <v>2753</v>
+      </c>
+      <c r="O693" t="s">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="694" spans="1:15">
+      <c r="A694" t="s">
+        <v>2757</v>
+      </c>
+      <c r="B694" t="s">
+        <v>2758</v>
+      </c>
+      <c r="M694" t="s">
+        <v>2759</v>
+      </c>
+      <c r="O694"/>
     </row>
     <row r="695" spans="1:15">
-      <c r="A695" t="s">
-        <v>374</v>
-      </c>
-      <c r="B695" t="s">
-        <v>562</v>
-      </c>
-      <c r="M695" t="s">
-        <v>375</v>
-      </c>
-      <c r="O695" s="9" t="s">
-        <v>2420</v>
-      </c>
+      <c r="O695"/>
     </row>
     <row r="696" spans="1:15">
       <c r="A696" t="s">
-        <v>376</v>
+        <v>2760</v>
       </c>
       <c r="B696" t="s">
-        <v>563</v>
-      </c>
-      <c r="M696" t="s">
-        <v>377</v>
-      </c>
-      <c r="O696" s="9" t="s">
-        <v>2421</v>
+        <v>2761</v>
+      </c>
+      <c r="M696" s="4" t="s">
+        <v>2762</v>
+      </c>
+      <c r="O696" t="s">
+        <v>2763</v>
       </c>
     </row>
     <row r="697" spans="1:15">
       <c r="A697" t="s">
-        <v>378</v>
+        <v>2764</v>
       </c>
       <c r="B697" t="s">
-        <v>563</v>
-      </c>
-      <c r="M697" t="s">
-        <v>377</v>
-      </c>
-      <c r="O697" s="9" t="s">
-        <v>2421</v>
-      </c>
-    </row>
-    <row r="701" spans="1:15">
-      <c r="A701" t="s">
-        <v>379</v>
-      </c>
-      <c r="B701" t="s">
-        <v>564</v>
-      </c>
-      <c r="M701" t="s">
-        <v>617</v>
-      </c>
-      <c r="O701" s="9" t="s">
-        <v>2422</v>
-      </c>
+        <v>2765</v>
+      </c>
+      <c r="M697" s="4" t="s">
+        <v>2766</v>
+      </c>
+      <c r="O697" t="s">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="698" spans="1:15">
+      <c r="A698" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B698" t="s">
+        <v>2769</v>
+      </c>
+      <c r="M698" s="4" t="s">
+        <v>2770</v>
+      </c>
+      <c r="O698" t="s">
+        <v>2771</v>
+      </c>
+    </row>
+    <row r="699" spans="1:15">
+      <c r="O699"/>
     </row>
     <row r="702" spans="1:15">
       <c r="A702" t="s">
-        <v>380</v>
+        <v>1239</v>
       </c>
       <c r="B702" t="s">
-        <v>565</v>
+        <v>1240</v>
       </c>
       <c r="M702" t="s">
-        <v>381</v>
+        <v>1241</v>
       </c>
       <c r="O702" s="9" t="s">
-        <v>2423</v>
-      </c>
-    </row>
-    <row r="703" spans="1:15">
-      <c r="A703" t="s">
-        <v>382</v>
-      </c>
-      <c r="B703" t="s">
-        <v>565</v>
-      </c>
-      <c r="M703" t="s">
-        <v>381</v>
-      </c>
-      <c r="O703" s="9" t="s">
-        <v>2423</v>
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="706" spans="1:15">
+      <c r="A706" t="s">
+        <v>374</v>
+      </c>
+      <c r="B706" t="s">
+        <v>562</v>
+      </c>
+      <c r="M706" t="s">
+        <v>375</v>
+      </c>
+      <c r="O706" s="9" t="s">
+        <v>2420</v>
       </c>
     </row>
     <row r="707" spans="1:15">
       <c r="A707" t="s">
-        <v>1346</v>
+        <v>376</v>
       </c>
       <c r="B707" t="s">
-        <v>1349</v>
+        <v>563</v>
       </c>
       <c r="M707" t="s">
-        <v>1352</v>
+        <v>377</v>
       </c>
       <c r="O707" s="9" t="s">
-        <v>2424</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="708" spans="1:15">
       <c r="A708" t="s">
-        <v>1347</v>
+        <v>378</v>
       </c>
       <c r="B708" t="s">
-        <v>1350</v>
+        <v>563</v>
       </c>
       <c r="M708" t="s">
-        <v>1353</v>
+        <v>377</v>
       </c>
       <c r="O708" s="9" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="709" spans="1:15">
-      <c r="A709" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B709" t="s">
-        <v>1351</v>
-      </c>
-      <c r="M709" t="s">
-        <v>1354</v>
-      </c>
-      <c r="O709" s="9" t="s">
-        <v>2426</v>
-      </c>
-    </row>
-    <row r="711" spans="1:15">
-      <c r="A711" t="s">
-        <v>100</v>
-      </c>
-      <c r="B711" t="s">
-        <v>1008</v>
-      </c>
-      <c r="M711" t="s">
-        <v>674</v>
-      </c>
-      <c r="O711" s="9" t="s">
-        <v>2427</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="712" spans="1:15">
       <c r="A712" t="s">
-        <v>101</v>
+        <v>379</v>
       </c>
       <c r="B712" t="s">
-        <v>1009</v>
+        <v>564</v>
       </c>
       <c r="M712" t="s">
-        <v>675</v>
+        <v>617</v>
       </c>
       <c r="O712" s="9" t="s">
-        <v>2428</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="713" spans="1:15">
       <c r="A713" t="s">
-        <v>102</v>
+        <v>380</v>
       </c>
       <c r="B713" t="s">
-        <v>512</v>
+        <v>565</v>
       </c>
       <c r="M713" t="s">
-        <v>211</v>
+        <v>381</v>
       </c>
       <c r="O713" s="9" t="s">
-        <v>2429</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="714" spans="1:15">
       <c r="A714" t="s">
-        <v>103</v>
+        <v>382</v>
       </c>
       <c r="B714" t="s">
-        <v>513</v>
+        <v>565</v>
       </c>
       <c r="M714" t="s">
-        <v>212</v>
+        <v>381</v>
       </c>
       <c r="O714" s="9" t="s">
-        <v>2430</v>
-      </c>
-    </row>
-    <row r="715" spans="1:15">
-      <c r="A715" t="s">
-        <v>965</v>
-      </c>
-      <c r="B715" t="s">
-        <v>967</v>
-      </c>
-      <c r="M715" t="s">
-        <v>966</v>
-      </c>
-      <c r="O715" s="9" t="s">
-        <v>2431</v>
-      </c>
-    </row>
-    <row r="716" spans="1:15">
-      <c r="A716" t="s">
-        <v>1392</v>
-      </c>
-      <c r="B716" t="s">
-        <v>1393</v>
-      </c>
-      <c r="M716" t="s">
-        <v>1394</v>
-      </c>
-      <c r="O716" s="9" t="s">
-        <v>2432</v>
-      </c>
-    </row>
-    <row r="717" spans="1:15">
-      <c r="A717" t="s">
-        <v>1827</v>
-      </c>
-      <c r="B717" t="s">
-        <v>1826</v>
-      </c>
-      <c r="M717" t="s">
-        <v>1825</v>
-      </c>
-      <c r="O717" s="9" t="s">
-        <v>2433</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="718" spans="1:15">
       <c r="A718" t="s">
-        <v>2053</v>
+        <v>1346</v>
       </c>
       <c r="B718" t="s">
-        <v>2051</v>
+        <v>1349</v>
       </c>
       <c r="M718" t="s">
-        <v>2052</v>
-      </c>
-      <c r="O718" s="10" t="s">
-        <v>2736</v>
+        <v>1352</v>
+      </c>
+      <c r="O718" s="9" t="s">
+        <v>2424</v>
+      </c>
+    </row>
+    <row r="719" spans="1:15">
+      <c r="A719" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B719" t="s">
+        <v>1350</v>
+      </c>
+      <c r="M719" t="s">
+        <v>1353</v>
+      </c>
+      <c r="O719" s="9" t="s">
+        <v>2425</v>
       </c>
     </row>
     <row r="720" spans="1:15">
       <c r="A720" t="s">
-        <v>865</v>
+        <v>1348</v>
       </c>
       <c r="B720" t="s">
-        <v>868</v>
+        <v>1351</v>
       </c>
       <c r="M720" t="s">
-        <v>871</v>
+        <v>1354</v>
       </c>
       <c r="O720" s="9" t="s">
-        <v>2737</v>
-      </c>
-    </row>
-    <row r="721" spans="1:15">
-      <c r="A721" t="s">
-        <v>866</v>
-      </c>
-      <c r="B721" t="s">
-        <v>869</v>
-      </c>
-      <c r="M721" t="s">
-        <v>884</v>
-      </c>
-      <c r="O721" s="9" t="s">
-        <v>2434</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="722" spans="1:15">
       <c r="A722" t="s">
-        <v>867</v>
+        <v>100</v>
       </c>
       <c r="B722" t="s">
-        <v>870</v>
+        <v>1008</v>
       </c>
       <c r="M722" t="s">
-        <v>885</v>
+        <v>674</v>
       </c>
       <c r="O722" s="9" t="s">
-        <v>2435</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="723" spans="1:15">
       <c r="A723" t="s">
-        <v>626</v>
+        <v>101</v>
       </c>
       <c r="B723" t="s">
-        <v>872</v>
+        <v>1009</v>
       </c>
       <c r="M723" t="s">
-        <v>875</v>
+        <v>675</v>
       </c>
       <c r="O723" s="9" t="s">
-        <v>2436</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="724" spans="1:15">
       <c r="A724" t="s">
-        <v>628</v>
+        <v>102</v>
       </c>
       <c r="B724" t="s">
-        <v>873</v>
+        <v>512</v>
       </c>
       <c r="M724" t="s">
-        <v>876</v>
+        <v>211</v>
       </c>
       <c r="O724" s="9" t="s">
-        <v>2437</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="725" spans="1:15">
       <c r="A725" t="s">
-        <v>627</v>
+        <v>103</v>
       </c>
       <c r="B725" t="s">
-        <v>874</v>
+        <v>513</v>
       </c>
       <c r="M725" t="s">
-        <v>877</v>
+        <v>212</v>
       </c>
       <c r="O725" s="9" t="s">
-        <v>2438</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="726" spans="1:15">
-      <c r="O726" s="9"/>
+      <c r="A726" t="s">
+        <v>965</v>
+      </c>
+      <c r="B726" t="s">
+        <v>967</v>
+      </c>
+      <c r="M726" t="s">
+        <v>966</v>
+      </c>
+      <c r="O726" s="9" t="s">
+        <v>2431</v>
+      </c>
     </row>
     <row r="727" spans="1:15">
       <c r="A727" t="s">
-        <v>878</v>
+        <v>1392</v>
       </c>
       <c r="B727" t="s">
-        <v>879</v>
+        <v>1393</v>
       </c>
       <c r="M727" t="s">
-        <v>880</v>
+        <v>1394</v>
       </c>
       <c r="O727" s="9" t="s">
-        <v>2439</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="728" spans="1:15">
       <c r="A728" t="s">
-        <v>881</v>
+        <v>1827</v>
       </c>
       <c r="B728" t="s">
-        <v>882</v>
+        <v>1826</v>
       </c>
       <c r="M728" t="s">
-        <v>883</v>
+        <v>1825</v>
       </c>
       <c r="O728" s="9" t="s">
-        <v>2440</v>
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="729" spans="1:15">
+      <c r="A729" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B729" t="s">
+        <v>2051</v>
+      </c>
+      <c r="M729" t="s">
+        <v>2052</v>
+      </c>
+      <c r="O729" s="10" t="s">
+        <v>2736</v>
       </c>
     </row>
     <row r="730" spans="1:15">
       <c r="A730" t="s">
-        <v>1092</v>
+        <v>2780</v>
       </c>
       <c r="B730" t="s">
-        <v>1093</v>
+        <v>2781</v>
       </c>
       <c r="M730" t="s">
-        <v>1094</v>
-      </c>
-      <c r="O730" s="9" t="s">
-        <v>2441</v>
-      </c>
-    </row>
-    <row r="731" spans="1:15">
-      <c r="A731" t="s">
-        <v>1080</v>
-      </c>
-      <c r="B731" t="s">
-        <v>1082</v>
-      </c>
-      <c r="M731" t="s">
-        <v>1084</v>
-      </c>
-      <c r="O731" s="9" t="s">
-        <v>2442</v>
-      </c>
+        <v>2782</v>
+      </c>
+      <c r="O730" s="17"/>
     </row>
     <row r="732" spans="1:15">
       <c r="A732" t="s">
-        <v>1081</v>
+        <v>865</v>
       </c>
       <c r="B732" t="s">
-        <v>1083</v>
+        <v>868</v>
       </c>
       <c r="M732" t="s">
-        <v>1085</v>
+        <v>871</v>
       </c>
       <c r="O732" s="9" t="s">
-        <v>2443</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="733" spans="1:15">
       <c r="A733" t="s">
-        <v>629</v>
+        <v>866</v>
       </c>
       <c r="B733" t="s">
-        <v>625</v>
+        <v>869</v>
       </c>
       <c r="M733" t="s">
-        <v>630</v>
+        <v>884</v>
       </c>
       <c r="O733" s="9" t="s">
-        <v>2444</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="734" spans="1:15">
       <c r="A734" t="s">
-        <v>1520</v>
+        <v>867</v>
       </c>
       <c r="B734" t="s">
-        <v>1521</v>
+        <v>870</v>
       </c>
       <c r="M734" t="s">
-        <v>1522</v>
+        <v>885</v>
       </c>
       <c r="O734" s="9" t="s">
-        <v>2445</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="735" spans="1:15">
       <c r="A735" t="s">
-        <v>1838</v>
+        <v>626</v>
       </c>
       <c r="B735" t="s">
-        <v>1843</v>
+        <v>872</v>
       </c>
       <c r="M735" t="s">
-        <v>1848</v>
+        <v>875</v>
       </c>
       <c r="O735" s="9" t="s">
-        <v>2446</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="736" spans="1:15">
       <c r="A736" t="s">
-        <v>1839</v>
+        <v>628</v>
       </c>
       <c r="B736" t="s">
-        <v>1844</v>
+        <v>873</v>
       </c>
       <c r="M736" t="s">
-        <v>1849</v>
+        <v>876</v>
       </c>
       <c r="O736" s="9" t="s">
-        <v>2447</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="737" spans="1:15">
       <c r="A737" t="s">
-        <v>1840</v>
+        <v>627</v>
       </c>
       <c r="B737" t="s">
-        <v>1845</v>
+        <v>874</v>
       </c>
       <c r="M737" t="s">
-        <v>1850</v>
+        <v>877</v>
       </c>
       <c r="O737" s="9" t="s">
-        <v>2448</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="738" spans="1:15">
-      <c r="A738" t="s">
-        <v>1841</v>
-      </c>
-      <c r="B738" t="s">
-        <v>1846</v>
-      </c>
-      <c r="M738" t="s">
-        <v>1851</v>
-      </c>
-      <c r="O738" s="9" t="s">
-        <v>2449</v>
-      </c>
+      <c r="O738" s="9"/>
     </row>
     <row r="739" spans="1:15">
       <c r="A739" t="s">
-        <v>1842</v>
+        <v>878</v>
       </c>
       <c r="B739" t="s">
-        <v>1847</v>
+        <v>879</v>
       </c>
       <c r="M739" t="s">
-        <v>2664</v>
+        <v>880</v>
       </c>
       <c r="O739" s="9" t="s">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="741" spans="1:15">
-      <c r="A741" t="s">
-        <v>1683</v>
-      </c>
-      <c r="B741" t="s">
-        <v>1684</v>
-      </c>
-      <c r="M741" t="s">
-        <v>1685</v>
-      </c>
-      <c r="O741" s="9" t="s">
-        <v>2451</v>
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="740" spans="1:15">
+      <c r="A740" t="s">
+        <v>881</v>
+      </c>
+      <c r="B740" t="s">
+        <v>882</v>
+      </c>
+      <c r="M740" t="s">
+        <v>883</v>
+      </c>
+      <c r="O740" s="9" t="s">
+        <v>2440</v>
       </c>
     </row>
     <row r="742" spans="1:15">
       <c r="A742" t="s">
-        <v>2058</v>
+        <v>1092</v>
       </c>
       <c r="B742" t="s">
-        <v>2057</v>
+        <v>1093</v>
       </c>
       <c r="M742" t="s">
-        <v>2056</v>
-      </c>
-      <c r="O742" s="10" t="s">
-        <v>2738</v>
+        <v>1094</v>
+      </c>
+      <c r="O742" s="9" t="s">
+        <v>2441</v>
       </c>
     </row>
     <row r="743" spans="1:15">
       <c r="A743" t="s">
-        <v>2055</v>
+        <v>1080</v>
       </c>
       <c r="B743" t="s">
-        <v>2054</v>
+        <v>1082</v>
       </c>
       <c r="M743" t="s">
-        <v>657</v>
-      </c>
-      <c r="O743" s="10" t="s">
-        <v>2739</v>
+        <v>1084</v>
+      </c>
+      <c r="O743" s="9" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="744" spans="1:15">
+      <c r="A744" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B744" t="s">
+        <v>1083</v>
+      </c>
+      <c r="M744" t="s">
+        <v>1085</v>
+      </c>
+      <c r="O744" s="9" t="s">
+        <v>2443</v>
       </c>
     </row>
     <row r="745" spans="1:15">
       <c r="A745" t="s">
-        <v>1877</v>
+        <v>629</v>
       </c>
       <c r="B745" t="s">
-        <v>1871</v>
+        <v>625</v>
       </c>
       <c r="M745" t="s">
-        <v>1872</v>
-      </c>
-      <c r="O745" s="12" t="s">
-        <v>2701</v>
+        <v>630</v>
+      </c>
+      <c r="O745" s="9" t="s">
+        <v>2444</v>
       </c>
     </row>
     <row r="746" spans="1:15">
       <c r="A746" t="s">
-        <v>1878</v>
+        <v>1520</v>
       </c>
       <c r="B746" t="s">
-        <v>1873</v>
+        <v>1521</v>
       </c>
       <c r="M746" t="s">
-        <v>1874</v>
-      </c>
-      <c r="O746" s="12" t="s">
-        <v>2702</v>
+        <v>1522</v>
+      </c>
+      <c r="O746" s="9" t="s">
+        <v>2445</v>
       </c>
     </row>
     <row r="747" spans="1:15">
       <c r="A747" t="s">
-        <v>1879</v>
+        <v>1838</v>
       </c>
       <c r="B747" t="s">
-        <v>1875</v>
+        <v>1843</v>
       </c>
       <c r="M747" t="s">
-        <v>1876</v>
-      </c>
-      <c r="O747" s="12" t="s">
-        <v>2703</v>
+        <v>1848</v>
+      </c>
+      <c r="O747" s="9" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="748" spans="1:15">
+      <c r="A748" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B748" t="s">
+        <v>1844</v>
+      </c>
+      <c r="M748" t="s">
+        <v>1849</v>
+      </c>
+      <c r="O748" s="9" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="749" spans="1:15">
+      <c r="A749" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B749" t="s">
+        <v>1845</v>
+      </c>
+      <c r="M749" t="s">
+        <v>1850</v>
+      </c>
+      <c r="O749" s="9" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="750" spans="1:15">
+      <c r="A750" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B750" t="s">
+        <v>1846</v>
+      </c>
+      <c r="M750" t="s">
+        <v>1851</v>
+      </c>
+      <c r="O750" s="9" t="s">
+        <v>2449</v>
       </c>
     </row>
     <row r="751" spans="1:15">
       <c r="A751" t="s">
-        <v>213</v>
+        <v>1842</v>
       </c>
       <c r="B751" t="s">
-        <v>514</v>
+        <v>1847</v>
       </c>
       <c r="M751" t="s">
-        <v>215</v>
+        <v>2664</v>
       </c>
       <c r="O751" s="9" t="s">
-        <v>2452</v>
-      </c>
-    </row>
-    <row r="752" spans="1:15">
-      <c r="A752" t="s">
-        <v>214</v>
-      </c>
-      <c r="B752" t="s">
-        <v>515</v>
-      </c>
-      <c r="M752" t="s">
-        <v>216</v>
-      </c>
-      <c r="O752" s="9" t="s">
-        <v>2453</v>
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="753" spans="1:15">
+      <c r="A753" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B753" t="s">
+        <v>1684</v>
+      </c>
+      <c r="M753" t="s">
+        <v>1685</v>
+      </c>
+      <c r="O753" s="9" t="s">
+        <v>2451</v>
       </c>
     </row>
     <row r="754" spans="1:15">
       <c r="A754" t="s">
-        <v>217</v>
+        <v>2058</v>
       </c>
       <c r="B754" t="s">
-        <v>516</v>
+        <v>2057</v>
       </c>
       <c r="M754" t="s">
-        <v>1465</v>
-      </c>
-      <c r="O754" s="9" t="s">
-        <v>2454</v>
+        <v>2056</v>
+      </c>
+      <c r="O754" s="10" t="s">
+        <v>2738</v>
       </c>
     </row>
     <row r="755" spans="1:15">
       <c r="A755" t="s">
-        <v>218</v>
+        <v>2055</v>
       </c>
       <c r="B755" t="s">
-        <v>517</v>
+        <v>2054</v>
       </c>
       <c r="M755" t="s">
-        <v>1466</v>
-      </c>
-      <c r="O755" s="9" t="s">
-        <v>2455</v>
-      </c>
-    </row>
-    <row r="756" spans="1:15">
-      <c r="A756" t="s">
-        <v>219</v>
-      </c>
-      <c r="B756" t="s">
-        <v>518</v>
-      </c>
-      <c r="M756" t="s">
-        <v>1467</v>
-      </c>
-      <c r="O756" s="9" t="s">
-        <v>2456</v>
+        <v>657</v>
+      </c>
+      <c r="O755" s="10" t="s">
+        <v>2739</v>
+      </c>
+    </row>
+    <row r="757" spans="1:15">
+      <c r="A757" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B757" t="s">
+        <v>1871</v>
+      </c>
+      <c r="M757" t="s">
+        <v>1872</v>
+      </c>
+      <c r="O757" s="12" t="s">
+        <v>2701</v>
       </c>
     </row>
     <row r="758" spans="1:15">
       <c r="A758" t="s">
-        <v>220</v>
+        <v>1878</v>
       </c>
       <c r="B758" t="s">
-        <v>221</v>
+        <v>1873</v>
       </c>
       <c r="M758" t="s">
-        <v>673</v>
-      </c>
-      <c r="O758" s="9" t="s">
-        <v>2457</v>
-      </c>
-    </row>
-    <row r="760" spans="1:15">
-      <c r="A760" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B760" t="s">
-        <v>1251</v>
-      </c>
-      <c r="M760" t="s">
-        <v>1252</v>
-      </c>
-      <c r="O760" s="9" t="s">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="762" spans="1:15">
-      <c r="A762" t="s">
-        <v>394</v>
-      </c>
-      <c r="B762" t="s">
-        <v>586</v>
-      </c>
-      <c r="M762" t="s">
-        <v>1568</v>
-      </c>
-      <c r="O762" s="9" t="s">
-        <v>2459</v>
+        <v>1874</v>
+      </c>
+      <c r="O758" s="12" t="s">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="759" spans="1:15">
+      <c r="A759" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B759" t="s">
+        <v>1875</v>
+      </c>
+      <c r="M759" t="s">
+        <v>1876</v>
+      </c>
+      <c r="O759" s="12" t="s">
+        <v>2703</v>
       </c>
     </row>
     <row r="763" spans="1:15">
       <c r="A763" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="B763" t="s">
-        <v>587</v>
+        <v>514</v>
       </c>
       <c r="M763" t="s">
-        <v>1569</v>
+        <v>215</v>
       </c>
       <c r="O763" s="9" t="s">
-        <v>2460</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="764" spans="1:15">
       <c r="A764" t="s">
-        <v>396</v>
+        <v>214</v>
       </c>
       <c r="B764" t="s">
-        <v>588</v>
+        <v>515</v>
       </c>
       <c r="M764" t="s">
-        <v>1570</v>
+        <v>216</v>
       </c>
       <c r="O764" s="9" t="s">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="765" spans="1:15">
-      <c r="A765" t="s">
-        <v>397</v>
-      </c>
-      <c r="B765" t="s">
-        <v>589</v>
-      </c>
-      <c r="M765" t="s">
-        <v>1571</v>
-      </c>
-      <c r="O765" s="9" t="s">
-        <v>2462</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="766" spans="1:15">
       <c r="A766" t="s">
-        <v>1578</v>
+        <v>217</v>
       </c>
       <c r="B766" t="s">
-        <v>1579</v>
+        <v>516</v>
       </c>
       <c r="M766" t="s">
-        <v>1580</v>
+        <v>1465</v>
       </c>
       <c r="O766" s="9" t="s">
-        <v>2463</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="767" spans="1:15">
       <c r="A767" t="s">
-        <v>398</v>
-      </c>
-      <c r="B767" s="1" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C767" s="1"/>
-      <c r="D767" s="1"/>
-      <c r="E767" s="1"/>
-      <c r="F767" s="1"/>
-      <c r="G767" s="1"/>
-      <c r="H767" s="1"/>
-      <c r="I767" s="1"/>
-      <c r="J767" s="1"/>
-      <c r="K767" s="1"/>
-      <c r="L767" s="1"/>
-      <c r="M767" s="1" t="s">
-        <v>1468</v>
+        <v>218</v>
+      </c>
+      <c r="B767" t="s">
+        <v>517</v>
+      </c>
+      <c r="M767" t="s">
+        <v>1466</v>
       </c>
       <c r="O767" s="9" t="s">
-        <v>2464</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="768" spans="1:15">
       <c r="A768" t="s">
-        <v>1869</v>
-      </c>
-      <c r="B768" s="1" t="s">
-        <v>1870</v>
-      </c>
-      <c r="C768" s="1"/>
-      <c r="D768" s="1"/>
-      <c r="E768" s="1"/>
-      <c r="F768" s="1"/>
-      <c r="G768" s="1"/>
-      <c r="H768" s="1"/>
-      <c r="I768" s="1"/>
-      <c r="J768" s="1"/>
-      <c r="K768" s="1"/>
-      <c r="L768" s="1"/>
-      <c r="M768" s="1" t="s">
-        <v>2662</v>
+        <v>219</v>
+      </c>
+      <c r="B768" t="s">
+        <v>518</v>
+      </c>
+      <c r="M768" t="s">
+        <v>1467</v>
       </c>
       <c r="O768" s="9" t="s">
-        <v>2465</v>
-      </c>
-    </row>
-    <row r="769" spans="1:15">
-      <c r="A769" t="s">
-        <v>2660</v>
-      </c>
-      <c r="B769" s="1" t="s">
-        <v>2661</v>
-      </c>
-      <c r="C769" s="1"/>
-      <c r="D769" s="1"/>
-      <c r="E769" s="1"/>
-      <c r="F769" s="1"/>
-      <c r="G769" s="1"/>
-      <c r="H769" s="1"/>
-      <c r="I769" s="1"/>
-      <c r="J769" s="1"/>
-      <c r="K769" s="1"/>
-      <c r="L769" s="1"/>
-      <c r="M769" s="1" t="s">
-        <v>2663</v>
-      </c>
-      <c r="O769" s="9" t="s">
-        <v>2740</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="770" spans="1:15">
-      <c r="B770" s="1"/>
-      <c r="C770" s="1"/>
-      <c r="D770" s="1"/>
-      <c r="E770" s="1"/>
-      <c r="F770" s="1"/>
-      <c r="G770" s="1"/>
-      <c r="H770" s="1"/>
-      <c r="I770" s="1"/>
-      <c r="J770" s="1"/>
-      <c r="K770" s="1"/>
-      <c r="L770" s="1"/>
-      <c r="M770" s="1"/>
-      <c r="O770" s="8"/>
-    </row>
-    <row r="771" spans="1:15">
-      <c r="A771" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B771" s="1" t="s">
-        <v>1573</v>
-      </c>
-      <c r="C771" s="1"/>
-      <c r="D771" s="1"/>
-      <c r="E771" s="1"/>
-      <c r="F771" s="1"/>
-      <c r="G771" s="1"/>
-      <c r="H771" s="1"/>
-      <c r="I771" s="1"/>
-      <c r="J771" s="1"/>
-      <c r="K771" s="1"/>
-      <c r="L771" s="1"/>
-      <c r="M771" s="1" t="s">
-        <v>1572</v>
-      </c>
-      <c r="O771" s="9" t="s">
-        <v>2466</v>
+      <c r="A770" t="s">
+        <v>220</v>
+      </c>
+      <c r="B770" t="s">
+        <v>221</v>
+      </c>
+      <c r="M770" t="s">
+        <v>673</v>
+      </c>
+      <c r="O770" s="9" t="s">
+        <v>2457</v>
       </c>
     </row>
     <row r="772" spans="1:15">
       <c r="A772" t="s">
-        <v>1567</v>
-      </c>
-      <c r="B772" s="1" t="s">
-        <v>1574</v>
-      </c>
-      <c r="C772" s="1"/>
-      <c r="D772" s="1"/>
-      <c r="E772" s="1"/>
-      <c r="F772" s="1"/>
-      <c r="G772" s="1"/>
-      <c r="H772" s="1"/>
-      <c r="I772" s="1"/>
-      <c r="J772" s="1"/>
-      <c r="K772" s="1"/>
-      <c r="L772" s="1"/>
-      <c r="M772" s="1" t="s">
-        <v>1572</v>
+        <v>1250</v>
+      </c>
+      <c r="B772" t="s">
+        <v>1251</v>
+      </c>
+      <c r="M772" t="s">
+        <v>1252</v>
       </c>
       <c r="O772" s="9" t="s">
-        <v>2467</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="774" spans="1:15">
       <c r="A774" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="B774" t="s">
-        <v>399</v>
+        <v>586</v>
       </c>
       <c r="M774" t="s">
-        <v>399</v>
+        <v>1568</v>
       </c>
       <c r="O774" s="9" t="s">
-        <v>2468</v>
+        <v>2459</v>
       </c>
     </row>
     <row r="775" spans="1:15">
       <c r="A775" t="s">
-        <v>735</v>
+        <v>395</v>
       </c>
       <c r="B775" t="s">
-        <v>737</v>
+        <v>587</v>
       </c>
       <c r="M775" t="s">
-        <v>739</v>
+        <v>1569</v>
       </c>
       <c r="O775" s="9" t="s">
-        <v>2469</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="776" spans="1:15">
       <c r="A776" t="s">
-        <v>736</v>
+        <v>396</v>
       </c>
       <c r="B776" t="s">
-        <v>738</v>
+        <v>588</v>
       </c>
       <c r="M776" t="s">
-        <v>740</v>
+        <v>1570</v>
       </c>
       <c r="O776" s="9" t="s">
-        <v>2470</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="777" spans="1:15">
       <c r="A777" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="B777" t="s">
-        <v>434</v>
+        <v>589</v>
       </c>
       <c r="M777" t="s">
-        <v>400</v>
+        <v>1571</v>
       </c>
       <c r="O777" s="9" t="s">
-        <v>2471</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="778" spans="1:15">
       <c r="A778" t="s">
-        <v>406</v>
+        <v>1578</v>
       </c>
       <c r="B778" t="s">
-        <v>435</v>
+        <v>1579</v>
       </c>
       <c r="M778" t="s">
-        <v>401</v>
+        <v>1580</v>
       </c>
       <c r="O778" s="9" t="s">
-        <v>2191</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="779" spans="1:15">
       <c r="A779" t="s">
-        <v>407</v>
-      </c>
-      <c r="B779" t="s">
-        <v>436</v>
-      </c>
-      <c r="M779" t="s">
-        <v>402</v>
+        <v>398</v>
+      </c>
+      <c r="B779" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C779" s="1"/>
+      <c r="D779" s="1"/>
+      <c r="E779" s="1"/>
+      <c r="F779" s="1"/>
+      <c r="G779" s="1"/>
+      <c r="H779" s="1"/>
+      <c r="I779" s="1"/>
+      <c r="J779" s="1"/>
+      <c r="K779" s="1"/>
+      <c r="L779" s="1"/>
+      <c r="M779" s="1" t="s">
+        <v>1468</v>
       </c>
       <c r="O779" s="9" t="s">
-        <v>2472</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="780" spans="1:15">
       <c r="A780" t="s">
-        <v>408</v>
-      </c>
-      <c r="B780" t="s">
-        <v>437</v>
-      </c>
-      <c r="M780" t="s">
-        <v>403</v>
+        <v>1869</v>
+      </c>
+      <c r="B780" s="1" t="s">
+        <v>1870</v>
+      </c>
+      <c r="C780" s="1"/>
+      <c r="D780" s="1"/>
+      <c r="E780" s="1"/>
+      <c r="F780" s="1"/>
+      <c r="G780" s="1"/>
+      <c r="H780" s="1"/>
+      <c r="I780" s="1"/>
+      <c r="J780" s="1"/>
+      <c r="K780" s="1"/>
+      <c r="L780" s="1"/>
+      <c r="M780" s="1" t="s">
+        <v>2662</v>
       </c>
       <c r="O780" s="9" t="s">
-        <v>2473</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="781" spans="1:15">
       <c r="A781" t="s">
-        <v>409</v>
-      </c>
-      <c r="B781" t="s">
-        <v>438</v>
-      </c>
-      <c r="M781" t="s">
-        <v>404</v>
+        <v>2660</v>
+      </c>
+      <c r="B781" s="1" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C781" s="1"/>
+      <c r="D781" s="1"/>
+      <c r="E781" s="1"/>
+      <c r="F781" s="1"/>
+      <c r="G781" s="1"/>
+      <c r="H781" s="1"/>
+      <c r="I781" s="1"/>
+      <c r="J781" s="1"/>
+      <c r="K781" s="1"/>
+      <c r="L781" s="1"/>
+      <c r="M781" s="1" t="s">
+        <v>2663</v>
       </c>
       <c r="O781" s="9" t="s">
-        <v>2474</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="782" spans="1:15">
-      <c r="A782" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B782" t="s">
-        <v>1057</v>
-      </c>
-      <c r="M782" t="s">
-        <v>1059</v>
-      </c>
-      <c r="O782" s="9" t="s">
-        <v>2475</v>
-      </c>
+      <c r="B782" s="1"/>
+      <c r="C782" s="1"/>
+      <c r="D782" s="1"/>
+      <c r="E782" s="1"/>
+      <c r="F782" s="1"/>
+      <c r="G782" s="1"/>
+      <c r="H782" s="1"/>
+      <c r="I782" s="1"/>
+      <c r="J782" s="1"/>
+      <c r="K782" s="1"/>
+      <c r="L782" s="1"/>
+      <c r="M782" s="1"/>
+      <c r="O782" s="8"/>
     </row>
     <row r="783" spans="1:15">
       <c r="A783" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B783" t="s">
-        <v>1550</v>
-      </c>
-      <c r="M783" t="s">
-        <v>1551</v>
+        <v>1566</v>
+      </c>
+      <c r="B783" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C783" s="1"/>
+      <c r="D783" s="1"/>
+      <c r="E783" s="1"/>
+      <c r="F783" s="1"/>
+      <c r="G783" s="1"/>
+      <c r="H783" s="1"/>
+      <c r="I783" s="1"/>
+      <c r="J783" s="1"/>
+      <c r="K783" s="1"/>
+      <c r="L783" s="1"/>
+      <c r="M783" s="1" t="s">
+        <v>1572</v>
       </c>
       <c r="O783" s="9" t="s">
-        <v>2476</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="784" spans="1:15">
       <c r="A784" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B784" t="s">
-        <v>1731</v>
-      </c>
-      <c r="M784" t="s">
-        <v>1739</v>
+        <v>1567</v>
+      </c>
+      <c r="B784" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C784" s="1"/>
+      <c r="D784" s="1"/>
+      <c r="E784" s="1"/>
+      <c r="F784" s="1"/>
+      <c r="G784" s="1"/>
+      <c r="H784" s="1"/>
+      <c r="I784" s="1"/>
+      <c r="J784" s="1"/>
+      <c r="K784" s="1"/>
+      <c r="L784" s="1"/>
+      <c r="M784" s="1" t="s">
+        <v>1572</v>
       </c>
       <c r="O784" s="9" t="s">
-        <v>2477</v>
-      </c>
-    </row>
-    <row r="785" spans="1:15">
-      <c r="A785" t="s">
-        <v>1909</v>
-      </c>
-      <c r="B785" t="s">
-        <v>1908</v>
-      </c>
-      <c r="M785" t="s">
-        <v>1907</v>
-      </c>
-      <c r="O785" s="10" t="s">
-        <v>2741</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="786" spans="1:15">
       <c r="A786" t="s">
-        <v>1800</v>
+        <v>405</v>
       </c>
       <c r="B786" t="s">
-        <v>1796</v>
+        <v>399</v>
       </c>
       <c r="M786" t="s">
-        <v>1801</v>
+        <v>399</v>
       </c>
       <c r="O786" s="9" t="s">
-        <v>2478</v>
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="787" spans="1:15">
+      <c r="A787" t="s">
+        <v>735</v>
+      </c>
+      <c r="B787" t="s">
+        <v>737</v>
+      </c>
+      <c r="M787" t="s">
+        <v>739</v>
+      </c>
+      <c r="O787" s="9" t="s">
+        <v>2469</v>
       </c>
     </row>
     <row r="788" spans="1:15">
       <c r="A788" t="s">
-        <v>819</v>
+        <v>736</v>
       </c>
       <c r="B788" t="s">
-        <v>826</v>
+        <v>738</v>
       </c>
       <c r="M788" t="s">
-        <v>833</v>
+        <v>740</v>
       </c>
       <c r="O788" s="9" t="s">
-        <v>2479</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="789" spans="1:15">
       <c r="A789" t="s">
-        <v>820</v>
+        <v>410</v>
       </c>
       <c r="B789" t="s">
-        <v>827</v>
+        <v>434</v>
       </c>
       <c r="M789" t="s">
-        <v>834</v>
+        <v>400</v>
       </c>
       <c r="O789" s="9" t="s">
-        <v>2480</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="790" spans="1:15">
       <c r="A790" t="s">
-        <v>821</v>
+        <v>406</v>
       </c>
       <c r="B790" t="s">
-        <v>828</v>
+        <v>435</v>
       </c>
       <c r="M790" t="s">
-        <v>835</v>
+        <v>401</v>
       </c>
       <c r="O790" s="9" t="s">
-        <v>2481</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="791" spans="1:15">
       <c r="A791" t="s">
-        <v>822</v>
+        <v>407</v>
       </c>
       <c r="B791" t="s">
-        <v>829</v>
+        <v>436</v>
       </c>
       <c r="M791" t="s">
-        <v>836</v>
+        <v>402</v>
       </c>
       <c r="O791" s="9" t="s">
-        <v>2482</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="792" spans="1:15">
       <c r="A792" t="s">
-        <v>823</v>
+        <v>408</v>
       </c>
       <c r="B792" t="s">
-        <v>830</v>
+        <v>437</v>
       </c>
       <c r="M792" t="s">
-        <v>837</v>
+        <v>403</v>
       </c>
       <c r="O792" s="9" t="s">
-        <v>2483</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="793" spans="1:15">
       <c r="A793" t="s">
-        <v>824</v>
+        <v>409</v>
       </c>
       <c r="B793" t="s">
-        <v>831</v>
+        <v>438</v>
       </c>
       <c r="M793" t="s">
-        <v>838</v>
+        <v>404</v>
       </c>
       <c r="O793" s="9" t="s">
-        <v>2484</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="794" spans="1:15">
       <c r="A794" t="s">
-        <v>825</v>
+        <v>1056</v>
       </c>
       <c r="B794" t="s">
-        <v>832</v>
+        <v>1057</v>
       </c>
       <c r="M794" t="s">
-        <v>839</v>
+        <v>1059</v>
       </c>
       <c r="O794" s="9" t="s">
-        <v>2485</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="795" spans="1:15">
       <c r="A795" t="s">
-        <v>1061</v>
+        <v>1549</v>
       </c>
       <c r="B795" t="s">
-        <v>1058</v>
+        <v>1550</v>
       </c>
       <c r="M795" t="s">
-        <v>1060</v>
+        <v>1551</v>
       </c>
       <c r="O795" s="9" t="s">
-        <v>2486</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="796" spans="1:15">
       <c r="A796" t="s">
-        <v>1553</v>
+        <v>1727</v>
       </c>
       <c r="B796" t="s">
-        <v>1554</v>
+        <v>1731</v>
       </c>
       <c r="M796" t="s">
-        <v>1552</v>
+        <v>1739</v>
       </c>
       <c r="O796" s="9" t="s">
-        <v>2487</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="797" spans="1:15">
       <c r="A797" t="s">
-        <v>1728</v>
+        <v>1909</v>
       </c>
       <c r="B797" t="s">
-        <v>1729</v>
+        <v>1908</v>
       </c>
       <c r="M797" t="s">
-        <v>1730</v>
-      </c>
-      <c r="O797" s="9" t="s">
-        <v>2488</v>
+        <v>1907</v>
+      </c>
+      <c r="O797" s="10" t="s">
+        <v>2741</v>
       </c>
     </row>
     <row r="798" spans="1:15">
       <c r="A798" t="s">
-        <v>1906</v>
+        <v>1800</v>
       </c>
       <c r="B798" t="s">
-        <v>1905</v>
+        <v>1796</v>
       </c>
       <c r="M798" t="s">
-        <v>1904</v>
-      </c>
-      <c r="O798" s="10" t="s">
-        <v>2742</v>
+        <v>1801</v>
+      </c>
+      <c r="O798" s="9" t="s">
+        <v>2478</v>
       </c>
     </row>
     <row r="800" spans="1:15">
       <c r="A800" t="s">
-        <v>840</v>
+        <v>819</v>
       </c>
       <c r="B800" t="s">
-        <v>1526</v>
+        <v>826</v>
       </c>
       <c r="M800" t="s">
-        <v>1529</v>
+        <v>833</v>
       </c>
       <c r="O800" s="9" t="s">
-        <v>2489</v>
+        <v>2479</v>
       </c>
     </row>
     <row r="801" spans="1:15">
       <c r="A801" t="s">
-        <v>841</v>
+        <v>820</v>
       </c>
       <c r="B801" t="s">
-        <v>1530</v>
+        <v>827</v>
       </c>
       <c r="M801" t="s">
-        <v>1528</v>
+        <v>834</v>
       </c>
       <c r="O801" s="9" t="s">
-        <v>2490</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="802" spans="1:15">
       <c r="A802" t="s">
-        <v>1489</v>
+        <v>821</v>
       </c>
       <c r="B802" t="s">
-        <v>1531</v>
+        <v>828</v>
       </c>
       <c r="M802" t="s">
-        <v>1532</v>
+        <v>835</v>
       </c>
       <c r="O802" s="9" t="s">
-        <v>2491</v>
+        <v>2481</v>
       </c>
     </row>
     <row r="803" spans="1:15">
       <c r="A803" t="s">
-        <v>1491</v>
+        <v>822</v>
       </c>
       <c r="B803" t="s">
-        <v>1492</v>
+        <v>829</v>
       </c>
       <c r="M803" t="s">
-        <v>1495</v>
+        <v>836</v>
       </c>
       <c r="O803" s="9" t="s">
-        <v>2492</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="804" spans="1:15">
       <c r="A804" t="s">
-        <v>1490</v>
+        <v>823</v>
       </c>
       <c r="B804" t="s">
-        <v>1493</v>
+        <v>830</v>
       </c>
       <c r="M804" t="s">
-        <v>1494</v>
+        <v>837</v>
       </c>
       <c r="O804" s="9" t="s">
-        <v>2493</v>
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="805" spans="1:15">
+      <c r="A805" t="s">
+        <v>824</v>
+      </c>
+      <c r="B805" t="s">
+        <v>831</v>
+      </c>
+      <c r="M805" t="s">
+        <v>838</v>
+      </c>
+      <c r="O805" s="9" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+    <row r="806" spans="1:15">
+      <c r="A806" t="s">
+        <v>825</v>
+      </c>
+      <c r="B806" t="s">
+        <v>832</v>
+      </c>
+      <c r="M806" t="s">
+        <v>839</v>
+      </c>
+      <c r="O806" s="9" t="s">
+        <v>2485</v>
+      </c>
+    </row>
+    <row r="807" spans="1:15">
+      <c r="A807" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B807" t="s">
+        <v>1058</v>
+      </c>
+      <c r="M807" t="s">
+        <v>1060</v>
+      </c>
+      <c r="O807" s="9" t="s">
+        <v>2486</v>
       </c>
     </row>
     <row r="808" spans="1:15">
       <c r="A808" t="s">
-        <v>411</v>
+        <v>1553</v>
       </c>
       <c r="B808" t="s">
-        <v>439</v>
+        <v>1554</v>
       </c>
       <c r="M808" t="s">
-        <v>733</v>
+        <v>1552</v>
       </c>
       <c r="O808" s="9" t="s">
-        <v>2494</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="809" spans="1:15">
       <c r="A809" t="s">
-        <v>412</v>
+        <v>1728</v>
       </c>
       <c r="B809" t="s">
-        <v>415</v>
+        <v>1729</v>
       </c>
       <c r="M809" t="s">
-        <v>432</v>
+        <v>1730</v>
       </c>
       <c r="O809" s="9" t="s">
-        <v>2495</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="810" spans="1:15">
       <c r="A810" t="s">
-        <v>413</v>
+        <v>1906</v>
       </c>
       <c r="B810" t="s">
-        <v>414</v>
+        <v>1905</v>
       </c>
       <c r="M810" t="s">
-        <v>433</v>
-      </c>
-      <c r="O810" s="9" t="s">
-        <v>2496</v>
-      </c>
-    </row>
-    <row r="811" spans="1:15">
-      <c r="A811" t="s">
-        <v>845</v>
-      </c>
-      <c r="B811" t="s">
-        <v>846</v>
-      </c>
-      <c r="M811" t="s">
-        <v>847</v>
-      </c>
-      <c r="O811" s="9" t="s">
-        <v>2497</v>
+        <v>1904</v>
+      </c>
+      <c r="O810" s="10" t="s">
+        <v>2742</v>
       </c>
     </row>
     <row r="812" spans="1:15">
       <c r="A812" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
       <c r="B812" t="s">
-        <v>849</v>
+        <v>1526</v>
       </c>
       <c r="M812" t="s">
-        <v>850</v>
+        <v>1529</v>
       </c>
       <c r="O812" s="9" t="s">
-        <v>2498</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="813" spans="1:15">
       <c r="A813" t="s">
-        <v>851</v>
-      </c>
-      <c r="B813" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C813" s="3"/>
-      <c r="D813" s="3"/>
-      <c r="E813" s="3"/>
-      <c r="F813" s="3"/>
-      <c r="G813" s="3"/>
-      <c r="H813" s="3"/>
-      <c r="I813" s="3"/>
-      <c r="J813" s="3"/>
-      <c r="K813" s="3"/>
-      <c r="L813" s="3"/>
-      <c r="M813" s="2" t="s">
-        <v>853</v>
+        <v>841</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1530</v>
+      </c>
+      <c r="M813" t="s">
+        <v>1528</v>
       </c>
       <c r="O813" s="9" t="s">
-        <v>2499</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="814" spans="1:15">
       <c r="A814" t="s">
-        <v>958</v>
-      </c>
-      <c r="B814" s="2" t="s">
-        <v>959</v>
-      </c>
-      <c r="C814" s="3"/>
-      <c r="D814" s="3"/>
-      <c r="E814" s="3"/>
-      <c r="F814" s="3"/>
-      <c r="G814" s="3"/>
-      <c r="H814" s="3"/>
-      <c r="I814" s="3"/>
-      <c r="J814" s="3"/>
-      <c r="K814" s="3"/>
-      <c r="L814" s="3"/>
-      <c r="M814" s="2" t="s">
-        <v>960</v>
+        <v>1489</v>
+      </c>
+      <c r="B814" t="s">
+        <v>1531</v>
+      </c>
+      <c r="M814" t="s">
+        <v>1532</v>
       </c>
       <c r="O814" s="9" t="s">
-        <v>2500</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="815" spans="1:15">
       <c r="A815" t="s">
-        <v>1555</v>
-      </c>
-      <c r="B815" s="2" t="s">
-        <v>1556</v>
-      </c>
-      <c r="C815" s="3"/>
-      <c r="D815" s="3"/>
-      <c r="E815" s="3"/>
-      <c r="F815" s="3"/>
-      <c r="G815" s="3"/>
-      <c r="H815" s="3"/>
-      <c r="I815" s="3"/>
-      <c r="J815" s="3"/>
-      <c r="K815" s="3"/>
-      <c r="L815" s="3"/>
-      <c r="M815" s="2" t="s">
-        <v>1291</v>
+        <v>1491</v>
+      </c>
+      <c r="B815" t="s">
+        <v>1492</v>
+      </c>
+      <c r="M815" t="s">
+        <v>1495</v>
       </c>
       <c r="O815" s="9" t="s">
-        <v>2609</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="816" spans="1:15">
       <c r="A816" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B816" s="2" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C816" s="3"/>
-      <c r="D816" s="3"/>
-      <c r="E816" s="3"/>
-      <c r="F816" s="3"/>
-      <c r="G816" s="3"/>
-      <c r="H816" s="3"/>
-      <c r="I816" s="3"/>
-      <c r="J816" s="3"/>
-      <c r="K816" s="3"/>
-      <c r="L816" s="3"/>
-      <c r="M816" s="2" t="s">
-        <v>1564</v>
+        <v>1490</v>
+      </c>
+      <c r="B816" t="s">
+        <v>1493</v>
+      </c>
+      <c r="M816" t="s">
+        <v>1494</v>
       </c>
       <c r="O816" s="9" t="s">
-        <v>2501</v>
-      </c>
-    </row>
-    <row r="817" spans="1:15">
-      <c r="A817" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B817" s="2" t="s">
-        <v>1768</v>
-      </c>
-      <c r="C817" s="3"/>
-      <c r="D817" s="3"/>
-      <c r="E817" s="3"/>
-      <c r="F817" s="3"/>
-      <c r="G817" s="3"/>
-      <c r="H817" s="3"/>
-      <c r="I817" s="3"/>
-      <c r="J817" s="3"/>
-      <c r="K817" s="3"/>
-      <c r="L817" s="3"/>
-      <c r="M817" s="2" t="s">
-        <v>1769</v>
-      </c>
-      <c r="O817" s="9" t="s">
-        <v>2502</v>
-      </c>
-    </row>
-    <row r="818" spans="1:15">
-      <c r="A818" t="s">
-        <v>1798</v>
-      </c>
-      <c r="B818" s="2" t="s">
-        <v>1797</v>
-      </c>
-      <c r="M818" s="2" t="s">
-        <v>1799</v>
-      </c>
-      <c r="O818" s="9" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="819" spans="1:15">
-      <c r="A819" t="s">
-        <v>1921</v>
-      </c>
-      <c r="B819" t="s">
-        <v>1920</v>
-      </c>
-      <c r="M819" t="s">
-        <v>1291</v>
-      </c>
-      <c r="O819" s="10" t="s">
-        <v>2743</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="820" spans="1:15">
       <c r="A820" t="s">
-        <v>1584</v>
+        <v>411</v>
       </c>
       <c r="B820" t="s">
-        <v>734</v>
+        <v>439</v>
       </c>
       <c r="M820" t="s">
-        <v>635</v>
+        <v>733</v>
       </c>
       <c r="O820" s="9" t="s">
-        <v>2503</v>
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="821" spans="1:15">
+      <c r="A821" t="s">
+        <v>412</v>
+      </c>
+      <c r="B821" t="s">
+        <v>415</v>
+      </c>
+      <c r="M821" t="s">
+        <v>432</v>
+      </c>
+      <c r="O821" s="9" t="s">
+        <v>2495</v>
       </c>
     </row>
     <row r="822" spans="1:15">
       <c r="A822" t="s">
-        <v>1583</v>
-      </c>
-      <c r="B822" s="2" t="s">
-        <v>1581</v>
-      </c>
-      <c r="M822" s="2" t="s">
-        <v>1582</v>
+        <v>413</v>
+      </c>
+      <c r="B822" t="s">
+        <v>414</v>
+      </c>
+      <c r="M822" t="s">
+        <v>433</v>
       </c>
       <c r="O822" s="9" t="s">
-        <v>2504</v>
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="823" spans="1:15">
+      <c r="A823" t="s">
+        <v>845</v>
+      </c>
+      <c r="B823" t="s">
+        <v>846</v>
+      </c>
+      <c r="M823" t="s">
+        <v>847</v>
+      </c>
+      <c r="O823" s="9" t="s">
+        <v>2497</v>
       </c>
     </row>
     <row r="824" spans="1:15">
       <c r="A824" t="s">
-        <v>420</v>
-      </c>
-      <c r="B824" s="4" t="s">
-        <v>590</v>
-      </c>
-      <c r="M824" s="4" t="s">
-        <v>416</v>
+        <v>848</v>
+      </c>
+      <c r="B824" t="s">
+        <v>849</v>
+      </c>
+      <c r="M824" t="s">
+        <v>850</v>
       </c>
       <c r="O824" s="9" t="s">
-        <v>2505</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="825" spans="1:15">
       <c r="A825" t="s">
-        <v>421</v>
-      </c>
-      <c r="B825" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="M825" s="4" t="s">
-        <v>417</v>
+        <v>851</v>
+      </c>
+      <c r="B825" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="C825" s="3"/>
+      <c r="D825" s="3"/>
+      <c r="E825" s="3"/>
+      <c r="F825" s="3"/>
+      <c r="G825" s="3"/>
+      <c r="H825" s="3"/>
+      <c r="I825" s="3"/>
+      <c r="J825" s="3"/>
+      <c r="K825" s="3"/>
+      <c r="L825" s="3"/>
+      <c r="M825" s="2" t="s">
+        <v>853</v>
       </c>
       <c r="O825" s="9" t="s">
-        <v>2506</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="826" spans="1:15">
       <c r="A826" t="s">
-        <v>422</v>
-      </c>
-      <c r="B826" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="M826" s="4" t="s">
-        <v>418</v>
+        <v>958</v>
+      </c>
+      <c r="B826" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="C826" s="3"/>
+      <c r="D826" s="3"/>
+      <c r="E826" s="3"/>
+      <c r="F826" s="3"/>
+      <c r="G826" s="3"/>
+      <c r="H826" s="3"/>
+      <c r="I826" s="3"/>
+      <c r="J826" s="3"/>
+      <c r="K826" s="3"/>
+      <c r="L826" s="3"/>
+      <c r="M826" s="2" t="s">
+        <v>960</v>
       </c>
       <c r="O826" s="9" t="s">
-        <v>2507</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="827" spans="1:15">
       <c r="A827" t="s">
-        <v>423</v>
-      </c>
-      <c r="B827" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="M827" s="4" t="s">
-        <v>419</v>
+        <v>1555</v>
+      </c>
+      <c r="B827" s="2" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C827" s="3"/>
+      <c r="D827" s="3"/>
+      <c r="E827" s="3"/>
+      <c r="F827" s="3"/>
+      <c r="G827" s="3"/>
+      <c r="H827" s="3"/>
+      <c r="I827" s="3"/>
+      <c r="J827" s="3"/>
+      <c r="K827" s="3"/>
+      <c r="L827" s="3"/>
+      <c r="M827" s="2" t="s">
+        <v>1291</v>
       </c>
       <c r="O827" s="9" t="s">
-        <v>2508</v>
-      </c>
-    </row>
-    <row r="828" spans="1:15" ht="45">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="828" spans="1:15">
       <c r="A828" t="s">
-        <v>1496</v>
-      </c>
-      <c r="B828" s="4" t="s">
-        <v>1497</v>
-      </c>
-      <c r="M828" s="4" t="s">
-        <v>1498</v>
+        <v>1562</v>
+      </c>
+      <c r="B828" s="2" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C828" s="3"/>
+      <c r="D828" s="3"/>
+      <c r="E828" s="3"/>
+      <c r="F828" s="3"/>
+      <c r="G828" s="3"/>
+      <c r="H828" s="3"/>
+      <c r="I828" s="3"/>
+      <c r="J828" s="3"/>
+      <c r="K828" s="3"/>
+      <c r="L828" s="3"/>
+      <c r="M828" s="2" t="s">
+        <v>1564</v>
       </c>
       <c r="O828" s="9" t="s">
-        <v>2509</v>
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="829" spans="1:15">
+      <c r="A829" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B829" s="2" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C829" s="3"/>
+      <c r="D829" s="3"/>
+      <c r="E829" s="3"/>
+      <c r="F829" s="3"/>
+      <c r="G829" s="3"/>
+      <c r="H829" s="3"/>
+      <c r="I829" s="3"/>
+      <c r="J829" s="3"/>
+      <c r="K829" s="3"/>
+      <c r="L829" s="3"/>
+      <c r="M829" s="2" t="s">
+        <v>1769</v>
+      </c>
+      <c r="O829" s="9" t="s">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="830" spans="1:15">
+      <c r="A830" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B830" s="2" t="s">
+        <v>1797</v>
+      </c>
+      <c r="M830" s="2" t="s">
+        <v>1799</v>
+      </c>
+      <c r="O830" s="9" t="s">
+        <v>1736</v>
       </c>
     </row>
     <row r="831" spans="1:15">
       <c r="A831" t="s">
-        <v>594</v>
+        <v>1921</v>
       </c>
       <c r="B831" t="s">
-        <v>425</v>
+        <v>1920</v>
       </c>
       <c r="M831" t="s">
-        <v>429</v>
-      </c>
-      <c r="O831" s="9" t="s">
-        <v>2510</v>
+        <v>1291</v>
+      </c>
+      <c r="O831" s="10" t="s">
+        <v>2743</v>
       </c>
     </row>
     <row r="832" spans="1:15">
       <c r="A832" t="s">
-        <v>595</v>
+        <v>1584</v>
       </c>
       <c r="B832" t="s">
-        <v>426</v>
+        <v>734</v>
       </c>
       <c r="M832" t="s">
-        <v>428</v>
+        <v>635</v>
       </c>
       <c r="O832" s="9" t="s">
-        <v>2511</v>
-      </c>
-    </row>
-    <row r="833" spans="1:15">
-      <c r="A833" t="s">
-        <v>596</v>
-      </c>
-      <c r="B833" t="s">
-        <v>427</v>
-      </c>
-      <c r="M833" t="s">
-        <v>430</v>
-      </c>
-      <c r="O833" s="9" t="s">
-        <v>2512</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="834" spans="1:15">
       <c r="A834" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B834" t="s">
-        <v>1525</v>
-      </c>
-      <c r="M834" t="s">
-        <v>1524</v>
+        <v>1583</v>
+      </c>
+      <c r="B834" s="2" t="s">
+        <v>1581</v>
+      </c>
+      <c r="M834" s="2" t="s">
+        <v>1582</v>
       </c>
       <c r="O834" s="9" t="s">
-        <v>2513</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="836" spans="1:15">
       <c r="A836" t="s">
-        <v>621</v>
-      </c>
-      <c r="B836" t="s">
-        <v>633</v>
-      </c>
-      <c r="M836" t="s">
-        <v>634</v>
+        <v>420</v>
+      </c>
+      <c r="B836" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="M836" s="4" t="s">
+        <v>416</v>
       </c>
       <c r="O836" s="9" t="s">
-        <v>2514</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="837" spans="1:15">
       <c r="A837" t="s">
-        <v>622</v>
-      </c>
-      <c r="B837" t="s">
-        <v>624</v>
-      </c>
-      <c r="M837" t="s">
-        <v>631</v>
+        <v>421</v>
+      </c>
+      <c r="B837" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="M837" s="4" t="s">
+        <v>417</v>
       </c>
       <c r="O837" s="9" t="s">
-        <v>2515</v>
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="838" spans="1:15">
+      <c r="A838" t="s">
+        <v>422</v>
+      </c>
+      <c r="B838" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="M838" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="O838" s="9" t="s">
+        <v>2507</v>
       </c>
     </row>
     <row r="839" spans="1:15">
       <c r="A839" t="s">
-        <v>637</v>
-      </c>
-      <c r="B839" t="s">
-        <v>638</v>
-      </c>
-      <c r="M839" t="s">
-        <v>639</v>
+        <v>423</v>
+      </c>
+      <c r="B839" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="M839" s="4" t="s">
+        <v>419</v>
       </c>
       <c r="O839" s="9" t="s">
-        <v>2516</v>
-      </c>
-    </row>
-    <row r="841" spans="1:15">
-      <c r="A841" t="s">
-        <v>742</v>
-      </c>
-      <c r="B841" t="s">
-        <v>743</v>
-      </c>
-      <c r="M841" t="s">
-        <v>745</v>
-      </c>
-      <c r="O841" s="9" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="842" spans="1:15">
-      <c r="A842" t="s">
-        <v>862</v>
-      </c>
-      <c r="B842" t="s">
-        <v>863</v>
-      </c>
-      <c r="M842" t="s">
-        <v>864</v>
-      </c>
-      <c r="O842" s="9" t="s">
-        <v>864</v>
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="840" spans="1:15" ht="45">
+      <c r="A840" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B840" s="4" t="s">
+        <v>1497</v>
+      </c>
+      <c r="M840" s="4" t="s">
+        <v>1498</v>
+      </c>
+      <c r="O840" s="9" t="s">
+        <v>2509</v>
       </c>
     </row>
     <row r="843" spans="1:15">
       <c r="A843" t="s">
-        <v>746</v>
+        <v>594</v>
       </c>
       <c r="B843" t="s">
-        <v>744</v>
+        <v>425</v>
       </c>
       <c r="M843" t="s">
-        <v>748</v>
+        <v>429</v>
       </c>
       <c r="O843" s="9" t="s">
-        <v>2517</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="844" spans="1:15">
       <c r="A844" t="s">
-        <v>749</v>
+        <v>595</v>
       </c>
       <c r="B844" t="s">
-        <v>744</v>
+        <v>426</v>
       </c>
       <c r="M844" t="s">
-        <v>750</v>
+        <v>428</v>
       </c>
       <c r="O844" s="9" t="s">
-        <v>2744</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="845" spans="1:15">
       <c r="A845" t="s">
-        <v>751</v>
+        <v>596</v>
       </c>
       <c r="B845" t="s">
-        <v>747</v>
+        <v>427</v>
       </c>
       <c r="M845" t="s">
-        <v>747</v>
+        <v>430</v>
       </c>
       <c r="O845" s="9" t="s">
-        <v>744</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="846" spans="1:15">
       <c r="A846" t="s">
-        <v>1585</v>
+        <v>1523</v>
       </c>
       <c r="B846" t="s">
-        <v>747</v>
+        <v>1525</v>
       </c>
       <c r="M846" t="s">
-        <v>1586</v>
+        <v>1524</v>
       </c>
       <c r="O846" s="9" t="s">
-        <v>2517</v>
-      </c>
-    </row>
-    <row r="847" spans="1:15">
-      <c r="A847" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B847" t="s">
-        <v>863</v>
-      </c>
-      <c r="M847" t="s">
-        <v>863</v>
-      </c>
-      <c r="O847" s="9" t="s">
-        <v>863</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="848" spans="1:15">
       <c r="A848" t="s">
-        <v>1636</v>
+        <v>621</v>
       </c>
       <c r="B848" t="s">
-        <v>744</v>
+        <v>633</v>
       </c>
       <c r="M848" t="s">
-        <v>1637</v>
+        <v>634</v>
       </c>
       <c r="O848" s="9" t="s">
-        <v>1637</v>
+        <v>2514</v>
       </c>
     </row>
     <row r="849" spans="1:15">
       <c r="A849" t="s">
-        <v>1604</v>
+        <v>622</v>
       </c>
       <c r="B849" t="s">
-        <v>1605</v>
+        <v>624</v>
       </c>
       <c r="M849" t="s">
-        <v>1606</v>
+        <v>631</v>
       </c>
       <c r="O849" s="9" t="s">
-        <v>2745</v>
-      </c>
-    </row>
-    <row r="850" spans="1:15">
-      <c r="A850" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B850" t="s">
-        <v>744</v>
-      </c>
-      <c r="M850" t="s">
-        <v>1682</v>
-      </c>
-      <c r="O850" s="9" t="s">
-        <v>1682</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="851" spans="1:15">
       <c r="A851" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B851" s="5" t="s">
-        <v>1687</v>
+        <v>637</v>
+      </c>
+      <c r="B851" t="s">
+        <v>638</v>
       </c>
       <c r="M851" t="s">
-        <v>1687</v>
+        <v>639</v>
       </c>
       <c r="O851" s="9" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="853" spans="1:15" ht="105">
+        <v>2516</v>
+      </c>
+    </row>
+    <row r="853" spans="1:15">
       <c r="A853" t="s">
-        <v>755</v>
-      </c>
-      <c r="B853" s="4" t="s">
-        <v>1431</v>
-      </c>
-      <c r="M853" s="4" t="s">
-        <v>1432</v>
-      </c>
-      <c r="O853" s="11" t="s">
-        <v>2518</v>
-      </c>
-    </row>
-    <row r="854" spans="1:15" ht="120">
+        <v>742</v>
+      </c>
+      <c r="B853" t="s">
+        <v>743</v>
+      </c>
+      <c r="M853" t="s">
+        <v>745</v>
+      </c>
+      <c r="O853" s="9" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="854" spans="1:15">
       <c r="A854" t="s">
-        <v>756</v>
-      </c>
-      <c r="B854" s="4" t="s">
-        <v>1433</v>
-      </c>
-      <c r="M854" s="4" t="s">
-        <v>1434</v>
-      </c>
-      <c r="O854" s="11" t="s">
-        <v>2519</v>
+        <v>862</v>
+      </c>
+      <c r="B854" t="s">
+        <v>863</v>
+      </c>
+      <c r="M854" t="s">
+        <v>864</v>
+      </c>
+      <c r="O854" s="9" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="855" spans="1:15">
       <c r="A855" t="s">
+        <v>746</v>
+      </c>
+      <c r="B855" t="s">
+        <v>744</v>
+      </c>
+      <c r="M855" t="s">
+        <v>748</v>
+      </c>
+      <c r="O855" s="9" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="856" spans="1:15">
+      <c r="A856" t="s">
+        <v>749</v>
+      </c>
+      <c r="B856" t="s">
+        <v>744</v>
+      </c>
+      <c r="M856" t="s">
+        <v>750</v>
+      </c>
+      <c r="O856" s="9" t="s">
+        <v>2744</v>
+      </c>
+    </row>
+    <row r="857" spans="1:15">
+      <c r="A857" t="s">
+        <v>751</v>
+      </c>
+      <c r="B857" t="s">
+        <v>747</v>
+      </c>
+      <c r="M857" t="s">
+        <v>747</v>
+      </c>
+      <c r="O857" s="9" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="858" spans="1:15">
+      <c r="A858" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B858" t="s">
+        <v>747</v>
+      </c>
+      <c r="M858" t="s">
+        <v>1586</v>
+      </c>
+      <c r="O858" s="9" t="s">
+        <v>2517</v>
+      </c>
+    </row>
+    <row r="859" spans="1:15">
+      <c r="A859" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B859" t="s">
+        <v>863</v>
+      </c>
+      <c r="M859" t="s">
+        <v>863</v>
+      </c>
+      <c r="O859" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="860" spans="1:15">
+      <c r="A860" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B860" t="s">
+        <v>744</v>
+      </c>
+      <c r="M860" t="s">
+        <v>1637</v>
+      </c>
+      <c r="O860" s="9" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="861" spans="1:15">
+      <c r="A861" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B861" t="s">
+        <v>1605</v>
+      </c>
+      <c r="M861" t="s">
+        <v>1606</v>
+      </c>
+      <c r="O861" s="9" t="s">
+        <v>2745</v>
+      </c>
+    </row>
+    <row r="862" spans="1:15">
+      <c r="A862" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B862" t="s">
+        <v>744</v>
+      </c>
+      <c r="M862" t="s">
+        <v>1682</v>
+      </c>
+      <c r="O862" s="9" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="863" spans="1:15">
+      <c r="A863" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B863" s="5" t="s">
+        <v>1687</v>
+      </c>
+      <c r="M863" t="s">
+        <v>1687</v>
+      </c>
+      <c r="O863" s="9" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="865" spans="1:15" ht="105">
+      <c r="A865" t="s">
+        <v>755</v>
+      </c>
+      <c r="B865" s="4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="M865" s="4" t="s">
+        <v>1432</v>
+      </c>
+      <c r="O865" s="11" t="s">
+        <v>2518</v>
+      </c>
+    </row>
+    <row r="866" spans="1:15" ht="120">
+      <c r="A866" t="s">
+        <v>756</v>
+      </c>
+      <c r="B866" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="M866" s="4" t="s">
+        <v>1434</v>
+      </c>
+      <c r="O866" s="11" t="s">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="867" spans="1:15">
+      <c r="A867" t="s">
         <v>757</v>
       </c>
-      <c r="B855" t="s">
+      <c r="B867" t="s">
         <v>759</v>
       </c>
-      <c r="M855" t="s">
+      <c r="M867" t="s">
         <v>758</v>
       </c>
-      <c r="O855" s="9" t="s">
+      <c r="O867" s="9" t="s">
         <v>2520</v>
       </c>
     </row>
-    <row r="857" spans="1:15" ht="30">
-      <c r="A857" t="s">
+    <row r="869" spans="1:15" ht="30">
+      <c r="A869" t="s">
         <v>1077</v>
       </c>
-      <c r="B857" s="4" t="s">
+      <c r="B869" s="4" t="s">
         <v>1435</v>
       </c>
-      <c r="M857" s="4" t="s">
+      <c r="M869" s="4" t="s">
         <v>1436</v>
       </c>
-      <c r="O857" s="11" t="s">
+      <c r="O869" s="11" t="s">
         <v>2521</v>
       </c>
     </row>
-    <row r="858" spans="1:15" ht="30">
-      <c r="A858" t="s">
+    <row r="870" spans="1:15" ht="30">
+      <c r="A870" t="s">
         <v>1071</v>
       </c>
-      <c r="B858" s="4" t="s">
+      <c r="B870" s="4" t="s">
         <v>1437</v>
       </c>
-      <c r="M858" s="4" t="s">
+      <c r="M870" s="4" t="s">
         <v>1438</v>
       </c>
-      <c r="O858" s="11" t="s">
+      <c r="O870" s="11" t="s">
         <v>2522</v>
       </c>
     </row>
-    <row r="859" spans="1:15" ht="45">
-      <c r="A859" t="s">
+    <row r="871" spans="1:15" ht="45">
+      <c r="A871" t="s">
         <v>1072</v>
       </c>
-      <c r="B859" s="4" t="s">
+      <c r="B871" s="4" t="s">
         <v>1439</v>
       </c>
-      <c r="M859" s="4" t="s">
+      <c r="M871" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="O859" s="11" t="s">
+      <c r="O871" s="11" t="s">
         <v>2523</v>
       </c>
     </row>
-    <row r="860" spans="1:15" ht="30">
-      <c r="A860" t="s">
+    <row r="872" spans="1:15" ht="30">
+      <c r="A872" t="s">
         <v>1073</v>
       </c>
-      <c r="B860" s="4" t="s">
+      <c r="B872" s="4" t="s">
         <v>1441</v>
       </c>
-      <c r="M860" t="s">
+      <c r="M872" t="s">
         <v>1076</v>
       </c>
-      <c r="O860" s="11" t="s">
+      <c r="O872" s="11" t="s">
         <v>2524</v>
       </c>
     </row>
-    <row r="861" spans="1:15" ht="45">
-      <c r="A861" t="s">
+    <row r="873" spans="1:15" ht="45">
+      <c r="A873" t="s">
         <v>1074</v>
       </c>
-      <c r="B861" s="4" t="s">
+      <c r="B873" s="4" t="s">
         <v>1442</v>
       </c>
-      <c r="M861" s="4" t="s">
+      <c r="M873" s="4" t="s">
         <v>1443</v>
       </c>
-      <c r="O861" s="11" t="s">
+      <c r="O873" s="11" t="s">
         <v>2525</v>
       </c>
     </row>
-    <row r="862" spans="1:15" ht="45">
-      <c r="A862" t="s">
+    <row r="874" spans="1:15" ht="45">
+      <c r="A874" t="s">
         <v>1075</v>
       </c>
-      <c r="B862" s="4" t="s">
+      <c r="B874" s="4" t="s">
         <v>1444</v>
       </c>
-      <c r="M862" s="4" t="s">
+      <c r="M874" s="4" t="s">
         <v>1440</v>
       </c>
-      <c r="O862" s="11" t="s">
+      <c r="O874" s="11" t="s">
         <v>2526</v>
       </c>
     </row>
-    <row r="863" spans="1:15" ht="45">
-      <c r="A863" t="s">
+    <row r="875" spans="1:15" ht="45">
+      <c r="A875" t="s">
         <v>1828</v>
       </c>
-      <c r="B863" s="4" t="s">
+      <c r="B875" s="4" t="s">
         <v>1831</v>
       </c>
-      <c r="M863" s="4" t="s">
+      <c r="M875" s="4" t="s">
         <v>1833</v>
       </c>
-      <c r="O863" s="11" t="s">
+      <c r="O875" s="11" t="s">
         <v>2527</v>
       </c>
     </row>
-    <row r="864" spans="1:15" ht="30">
-      <c r="A864" t="s">
+    <row r="876" spans="1:15" ht="30">
+      <c r="A876" t="s">
         <v>1830</v>
       </c>
-      <c r="B864" s="4" t="s">
+      <c r="B876" s="4" t="s">
         <v>1829</v>
       </c>
-      <c r="M864" s="4" t="s">
+      <c r="M876" s="4" t="s">
         <v>1832</v>
       </c>
-      <c r="O864" s="11" t="s">
+      <c r="O876" s="11" t="s">
         <v>2528</v>
       </c>
     </row>
@@ -19332,10 +19557,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E03A3E-CD6E-42CA-AC43-3F5764A8A875}">
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19924,6 +20149,34 @@
       </c>
       <c r="O39" s="18" t="s">
         <v>2746</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2773</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>2774</v>
+      </c>
+      <c r="O40" t="s">
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2777</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>2778</v>
+      </c>
+      <c r="O41" t="s">
+        <v>2779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>